<commit_message>
Now a better output decvar file
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -25,7 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>Irrad</t>
+  </si>
+  <si>
+    <t>cents/kWh</t>
+  </si>
   <si>
     <t>P_Subs</t>
   </si>
@@ -520,681 +532,1049 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1.8757755645241471e-6</v>
+        <v>1</v>
       </c>
       <c r="C1">
-        <v>1.8757707151821702e-6</v>
+        <v>2</v>
       </c>
       <c r="D1">
-        <v>2.912124004078675e-7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.04324175843655724</v>
+        <v>0.75</v>
       </c>
       <c r="C2">
-        <v>0.04336757545719688</v>
+        <v>0.777</v>
       </c>
       <c r="D2">
-        <v>0.04343499697093368</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.787</v>
+      </c>
+      <c r="E2">
+        <v>0.796</v>
+      </c>
+      <c r="F2">
+        <v>0.782</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.09637118013601688</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>-0.12476688498288527</v>
+        <v>0.8</v>
       </c>
       <c r="D3">
-        <v>-0.15222201772674998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>1.0</v>
+      </c>
+      <c r="F3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.05313129747502417</v>
+        <v>4.820404</v>
       </c>
       <c r="C4">
-        <v>0.08140118529640357</v>
+        <v>4.820404</v>
       </c>
       <c r="D4">
-        <v>0.1087873119682167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>4.820404</v>
+      </c>
+      <c r="E4">
+        <v>4.820404</v>
+      </c>
+      <c r="F4">
+        <v>30.18066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.005180603976812052</v>
+        <v>0.051314204920749056</v>
       </c>
       <c r="C5">
-        <v>0.005247282915344075</v>
+        <v>0.0515336941156942</v>
       </c>
       <c r="D5">
-        <v>0.005307294057575181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0.05166669096078263</v>
+      </c>
+      <c r="E5">
+        <v>0.05173997845342276</v>
+      </c>
+      <c r="F5">
+        <v>0.05090273745527078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.01059124006999165</v>
+        <v>0.04267080145312797</v>
       </c>
       <c r="C6">
-        <v>0.01071679309413224</v>
+        <v>0.042891099738211896</v>
       </c>
       <c r="D6">
-        <v>0.0108303141870792</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.04302459369637416</v>
+      </c>
+      <c r="E6">
+        <v>0.04309810318636273</v>
+      </c>
+      <c r="F6">
+        <v>0.04225781230236308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.017105477360126593</v>
+        <v>0.005024022632188014</v>
       </c>
       <c r="C7">
-        <v>0.016905707849663585</v>
+        <v>0.00502350080532581</v>
       </c>
       <c r="D7">
-        <v>0.016679593743412213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>0.005023212975893911</v>
+      </c>
+      <c r="E7">
+        <v>0.00502308366643496</v>
+      </c>
+      <c r="F7">
+        <v>0.005025024263081777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.005180707865374212</v>
+        <v>0.0036193808354330723</v>
       </c>
       <c r="C8">
-        <v>0.005247389494533827</v>
+        <v>0.003619093572156492</v>
       </c>
       <c r="D8">
-        <v>0.005307403087038479</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.0036188842885145544</v>
+      </c>
+      <c r="E8">
+        <v>0.0036187916006250693</v>
+      </c>
+      <c r="F8">
+        <v>0.0036199008898259236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.0051806678042761005</v>
+        <v>0.005000571378385479</v>
       </c>
       <c r="C9">
-        <v>0.005247348395491457</v>
+        <v>0.005180603942595949</v>
       </c>
       <c r="D9">
-        <v>0.005307361042575549</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0.005247282882398706</v>
+      </c>
+      <c r="E9">
+        <v>0.005307294026718522</v>
+      </c>
+      <c r="F9">
+        <v>0.005213943399840193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.005180322652746347</v>
+        <v>0.009997986470737593</v>
       </c>
       <c r="C10">
-        <v>0.005246994301848334</v>
+        <v>0.010357918891993494</v>
       </c>
       <c r="D10">
-        <v>0.00530699880394465</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>0.010491227353330477</v>
+      </c>
+      <c r="E10">
+        <v>0.01061120501823848</v>
+      </c>
+      <c r="F10">
+        <v>0.01042457299775907</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.024529729210252423</v>
+        <v>0.01766895580256375</v>
       </c>
       <c r="C11">
-        <v>0.02469825044413654</v>
+        <v>0.01698919222325956</v>
       </c>
       <c r="D11">
-        <v>0.024817199039566886</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>0.016789301477448892</v>
+      </c>
+      <c r="E11">
+        <v>0.016562756455375614</v>
+      </c>
+      <c r="F11">
+        <v>0.016189310662511343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.761727005119123</v>
+        <v>0.005000668116901921</v>
       </c>
       <c r="C12">
-        <v>0.7592452611688744</v>
+        <v>0.005180707778426727</v>
       </c>
       <c r="D12">
-        <v>0.7298232157535222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>0.00524738941229492</v>
+      </c>
+      <c r="E12">
+        <v>0.005307403012073319</v>
+      </c>
+      <c r="F12">
+        <v>0.005214048579497665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.7430108945540278</v>
+        <v>0.0050006308002073455</v>
       </c>
       <c r="C13">
-        <v>0.731048202312871</v>
+        <v>0.005180667725089316</v>
       </c>
       <c r="D13">
-        <v>0.7293812678517976</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>0.005247348320592993</v>
+      </c>
+      <c r="E13">
+        <v>0.005307360974301607</v>
+      </c>
+      <c r="F13">
+        <v>0.005214008008394043</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.0025900909128872647</v>
+        <v>0.005000309292381279</v>
       </c>
       <c r="C14">
-        <v>0.0026234299793156117</v>
+        <v>0.0051803226404165915</v>
       </c>
       <c r="D14">
-        <v>0.00265343523804923</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>0.005246994290186291</v>
+      </c>
+      <c r="E14">
+        <v>0.005306998793314076</v>
+      </c>
+      <c r="F14">
+        <v>0.005213658463051959</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.005648249834620189</v>
+        <v>0.014659372182184523</v>
       </c>
       <c r="C15">
-        <v>0.005710595625912609</v>
+        <v>0.01617955371008737</v>
       </c>
       <c r="D15">
-        <v>0.005766849184598267</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>0.016868088566846896</v>
+      </c>
+      <c r="E15">
+        <v>0.01765962826269832</v>
+      </c>
+      <c r="F15">
+        <v>0.01727176232328896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.01109675232166914</v>
+        <v>7.405262328279441e-5</v>
       </c>
       <c r="C16">
-        <v>0.011102807052079085</v>
+        <v>7.435898984486915e-5</v>
       </c>
       <c r="D16">
-        <v>0.011075425525536144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>7.4533641702042e-5</v>
+      </c>
+      <c r="E16">
+        <v>7.461188834528784e-5</v>
+      </c>
+      <c r="F16">
+        <v>7.346964245218109e-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.00259019590146115</v>
+        <v>4.989258095798899e-5</v>
       </c>
       <c r="C17">
-        <v>0.0026235376870031085</v>
+        <v>5.009480240295952e-5</v>
       </c>
       <c r="D17">
-        <v>0.0026535454219497553</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>5.019453492239171e-5</v>
+      </c>
+      <c r="E17">
+        <v>5.0265615559787286e-5</v>
+      </c>
+      <c r="F17">
+        <v>4.950012143843453e-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.0025902216879810248</v>
+        <v>0.0025000759768043493</v>
       </c>
       <c r="C18">
-        <v>0.002623564141544318</v>
+        <v>0.002590090878181582</v>
       </c>
       <c r="D18">
-        <v>0.0026535724849613166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>0.0026234299458988463</v>
+      </c>
+      <c r="E18">
+        <v>0.0026534352067510607</v>
+      </c>
+      <c r="F18">
+        <v>0.0026067603992019754</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.0025898715978761233</v>
+        <v>0.002732657152935766</v>
       </c>
       <c r="C19">
-        <v>0.002623204981378479</v>
+        <v>0.002849323378917998</v>
       </c>
       <c r="D19">
-        <v>0.002653205063265746</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>0.0028907272848052953</v>
+      </c>
+      <c r="E19">
+        <v>0.0029241288897002282</v>
+      </c>
+      <c r="F19">
+        <v>0.0028459354632558295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.002329679710045499</v>
+        <v>0.004414547343748728</v>
       </c>
       <c r="C20">
-        <v>0.002347770848266499</v>
+        <v>0.005547656394314283</v>
       </c>
       <c r="D20">
-        <v>0.0023588389551121975</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>0.006094579198109388</v>
+      </c>
+      <c r="E20">
+        <v>0.0067625132224153044</v>
+      </c>
+      <c r="F20">
+        <v>0.00659334955139506</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.5556747810645066</v>
+        <v>0.0025001737395008465</v>
       </c>
       <c r="C21">
-        <v>0.5580357085142854</v>
+        <v>0.002590195813344445</v>
       </c>
       <c r="D21">
-        <v>0.5239074384496273</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>0.0026235376036582996</v>
+      </c>
+      <c r="E21">
+        <v>0.002653545345976505</v>
+      </c>
+      <c r="F21">
+        <v>0.002606866692424894</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.5230352129955067</v>
+        <v>0.0025001977597068925</v>
       </c>
       <c r="C22">
-        <v>0.5099986394624434</v>
+        <v>0.002590221594870122</v>
       </c>
       <c r="D22">
-        <v>0.5126134820522538</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>0.0026235640534757873</v>
+      </c>
+      <c r="E22">
+        <v>0.0026535724046821575</v>
+      </c>
+      <c r="F22">
+        <v>0.002606892807185479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>3.1638285449950865e-5</v>
+        <v>0.0024998716516098636</v>
       </c>
       <c r="C23">
-        <v>3.245805019279032e-5</v>
+        <v>0.002589871572578869</v>
       </c>
       <c r="D23">
-        <v>3.320478511222428e-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>0.0026232049574511844</v>
+      </c>
+      <c r="E23">
+        <v>0.0026532050414547416</v>
+      </c>
+      <c r="F23">
+        <v>0.0026065382603997077</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.00013587860137611606</v>
+        <v>0.0019188368768929206</v>
       </c>
       <c r="C24">
-        <v>0.00013906990827180124</v>
+        <v>0.001980793073940546</v>
       </c>
       <c r="D24">
-        <v>0.000141985938327706</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>0.002013052001004336</v>
+      </c>
+      <c r="E24">
+        <v>0.0020447804783942074</v>
+      </c>
+      <c r="F24">
+        <v>0.0019644027968446862</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.0003920786174019595</v>
+        <v>2.371104479111432e-5</v>
       </c>
       <c r="C25">
-        <v>0.0003857986387458257</v>
+        <v>2.3706205504398593e-5</v>
       </c>
       <c r="D25">
-        <v>0.0003780645866617025</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>2.3703291845529456e-5</v>
+      </c>
+      <c r="E25">
+        <v>2.3701685981049558e-5</v>
+      </c>
+      <c r="F25">
+        <v>2.3720229748177704e-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>3.165457465296649e-5</v>
+        <v>1.2307855614160535e-5</v>
       </c>
       <c r="C26">
-        <v>3.247467823495547e-5</v>
+        <v>1.2306034363860468e-5</v>
       </c>
       <c r="D26">
-        <v>3.3221675549836177e-5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>1.2304947451612389e-5</v>
+      </c>
+      <c r="E26">
+        <v>1.2304345175344038e-5</v>
+      </c>
+      <c r="F26">
+        <v>1.2311317445593029e-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>3.165430904437857e-5</v>
+        <v>2.9474042144264115e-5</v>
       </c>
       <c r="C27">
-        <v>3.2474402237356014e-5</v>
+        <v>3.1635147445243404e-5</v>
       </c>
       <c r="D27">
-        <v>3.322138997465457e-5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>3.245502872889913e-5</v>
+      </c>
+      <c r="E27">
+        <v>3.320195520669227e-5</v>
+      </c>
+      <c r="F27">
+        <v>3.204392728430245e-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>3.165430904437857e-5</v>
+        <v>0.00010130030175364274</v>
       </c>
       <c r="C28">
-        <v>3.2474402237356014e-5</v>
+        <v>0.00010882598907297721</v>
       </c>
       <c r="D28">
-        <v>3.322138997465457e-5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>0.00011167220676901554</v>
+      </c>
+      <c r="E28">
+        <v>0.0001142441603560652</v>
+      </c>
+      <c r="F28">
+        <v>0.00011011522258086881</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1.0609</v>
+        <v>0.00031276907899746575</v>
       </c>
       <c r="C29">
-        <v>1.0609</v>
+        <v>0.00030120383813518283</v>
       </c>
       <c r="D29">
-        <v>1.0609</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>0.0003008438367533325</v>
+      </c>
+      <c r="E29">
+        <v>0.0003018198770550414</v>
+      </c>
+      <c r="F29">
+        <v>0.00028815240899914506</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>1.060336488671325</v>
+        <v>2.9486152075728904e-5</v>
       </c>
       <c r="C30">
-        <v>1.060333650530811</v>
+        <v>3.164844300236681e-5</v>
       </c>
       <c r="D30">
-        <v>1.0603317761912678</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>3.246887863941623e-5</v>
+      </c>
+      <c r="E30">
+        <v>3.321638890840964e-5</v>
+      </c>
+      <c r="F30">
+        <v>3.2057542130117967e-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>1.0491774413819643</v>
+        <v>2.9485913314018506e-5</v>
       </c>
       <c r="C31">
-        <v>1.0494469103045367</v>
+        <v>3.164817749666981e-5</v>
       </c>
       <c r="D31">
-        <v>1.0501494116777736</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>3.246860274038923e-5</v>
+      </c>
+      <c r="E31">
+        <v>3.3216103424110566e-5</v>
+      </c>
+      <c r="F31">
+        <v>3.2057271457742984e-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>1.060166228262348</v>
+        <v>2.9485913314018506e-5</v>
       </c>
       <c r="C32">
-        <v>1.0601611987686603</v>
+        <v>3.16481774966698e-5</v>
       </c>
       <c r="D32">
-        <v>1.0601573522091028</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>3.246860274038923e-5</v>
+      </c>
+      <c r="E32">
+        <v>3.321610342411056e-5</v>
+      </c>
+      <c r="F32">
+        <v>3.205727145774298e-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>1.0602028881821097</v>
+        <v>1.0609</v>
       </c>
       <c r="C33">
-        <v>1.0601985232706381</v>
+        <v>1.0609</v>
       </c>
       <c r="D33">
-        <v>1.0601952699250805</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>1.0609</v>
+      </c>
+      <c r="E33">
+        <v>1.0609</v>
+      </c>
+      <c r="F33">
+        <v>1.0609</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1.059842034274568</v>
+        <v>1.0604617394225673</v>
       </c>
       <c r="C34">
-        <v>1.0598425719095228</v>
+        <v>1.060441650393495</v>
       </c>
       <c r="D34">
-        <v>1.0598451237607587</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>1.0604323482943674</v>
+      </c>
+      <c r="E34">
+        <v>1.060422136686849</v>
+      </c>
+      <c r="F34">
+        <v>1.060431989315611</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1.0596206747961616</v>
+        <v>1.060858371812388</v>
       </c>
       <c r="C35">
-        <v>1.059618363363562</v>
+        <v>1.0608583709639388</v>
       </c>
       <c r="D35">
-        <v>1.05961835105037</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>1.060858370402619</v>
+      </c>
+      <c r="E35">
+        <v>1.0608583701539906</v>
+      </c>
+      <c r="F35">
+        <v>1.0608583733572843</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1.0596717695848445</v>
+        <v>1.0602973956553108</v>
       </c>
       <c r="C36">
-        <v>1.0596701157557418</v>
+        <v>1.0602713899852751</v>
       </c>
       <c r="D36">
-        <v>1.0596706952859751</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>1.0602598965329457</v>
+      </c>
+      <c r="E36">
+        <v>1.0602477127053669</v>
+      </c>
+      <c r="F36">
+        <v>1.06026063323107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1.0596295659822168</v>
+        <v>1.0603677021379236</v>
       </c>
       <c r="C37">
-        <v>1.0596273689835114</v>
+        <v>1.0603440021670187</v>
       </c>
       <c r="D37">
-        <v>1.0596274596609148</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>1.0603333849722005</v>
+      </c>
+      <c r="E37">
+        <v>1.0603220374447273</v>
+      </c>
+      <c r="F37">
+        <v>1.0603339808671042</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>1.048634749062134</v>
+        <v>1.060075599651318</v>
       </c>
       <c r="C38">
-        <v>1.0483863631018688</v>
+        <v>1.0600473279019493</v>
       </c>
       <c r="D38">
-        <v>1.0479937846258143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>1.0600318410838698</v>
+      </c>
+      <c r="E38">
+        <v>1.0600137700939622</v>
+      </c>
+      <c r="F38">
+        <v>1.0600331242956231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.0006423859643664419</v>
+        <v>1.059861932636617</v>
       </c>
       <c r="C39">
-        <v>-0.0005140972184173544</v>
+        <v>1.0598259684260423</v>
       </c>
       <c r="D39">
-        <v>-0.0003656079485116869</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>1.0598076325402732</v>
+      </c>
+      <c r="E39">
+        <v>1.0597869973857286</v>
+      </c>
+      <c r="F39">
+        <v>1.059810340286327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>-9.919663652755882e-20</v>
+        <v>1.059911251897293</v>
       </c>
       <c r="C40">
-        <v>-2.9565388839606985e-20</v>
+        <v>1.0598770632145331</v>
       </c>
       <c r="D40">
-        <v>1.4139575301641614e-20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>1.0598593849322713</v>
+      </c>
+      <c r="E40">
+        <v>1.0598393416211682</v>
+      </c>
+      <c r="F40">
+        <v>1.0598617638765369</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.0004671522876676836</v>
+        <v>1.0598705148516268</v>
       </c>
       <c r="C41">
-        <v>-0.000462808384463364</v>
+        <v>1.0598348596120346</v>
       </c>
       <c r="D41">
-        <v>-0.00045904094746690595</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>1.0598166381601632</v>
+      </c>
+      <c r="E41">
+        <v>1.0597961059962193</v>
+      </c>
+      <c r="F41">
+        <v>1.059819288689257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42">
-        <v>-9.022343987739603e-5</v>
+        <v>1.060843889514316</v>
       </c>
       <c r="C42">
-        <v>-9.126819779663008e-5</v>
+        <v>1.0608438907722857</v>
       </c>
       <c r="D42">
-        <v>-9.24252387794357e-5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>1.0608438924263985</v>
+      </c>
+      <c r="E42">
+        <v>1.0608438927419062</v>
+      </c>
+      <c r="F42">
+        <v>1.0608438876454969</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.002322714282136691</v>
+        <v>0.0045268852161094745</v>
       </c>
       <c r="C43">
-        <v>0.0023187177131289804</v>
+        <v>0.003694958320204721</v>
       </c>
       <c r="D43">
-        <v>0.002315385941511528</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>0.0032580775980534937</v>
+      </c>
+      <c r="E43">
+        <v>0.0026852866742830793</v>
+      </c>
+      <c r="F43">
+        <v>0.002675699699297939</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.0011891599605450111</v>
+        <v>1.7475176701477044e-20</v>
       </c>
       <c r="C44">
-        <v>0.0011892494024726464</v>
+        <v>1.5767987415293315e-19</v>
       </c>
       <c r="D44">
-        <v>0.0011895082353379084</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>-8.004823744950932e-20</v>
+      </c>
+      <c r="E44">
+        <v>6.278478846541676e-20</v>
+      </c>
+      <c r="F44">
+        <v>6.278478846541676e-20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.0020892940637454267</v>
+        <v>0.002268218001124278</v>
       </c>
       <c r="C45">
-        <v>0.002093054096559011</v>
+        <v>0.0023316072183796367</v>
       </c>
       <c r="D45">
-        <v>0.0020961800276369847</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>0.0023568908773417777</v>
+      </c>
+      <c r="E45">
+        <v>0.0023835081447315214</v>
+      </c>
+      <c r="F45">
+        <v>0.002368338090282289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.0010734870210011114</v>
+        <v>0.0010619540996073718</v>
       </c>
       <c r="C46">
-        <v>0.0010734034351496187</v>
+        <v>0.0011207246068114895</v>
       </c>
       <c r="D46">
-        <v>0.0010731551763651685</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>0.0011440335913507895</v>
+      </c>
+      <c r="E46">
+        <v>0.001168918213414903</v>
+      </c>
+      <c r="F46">
+        <v>0.0011608517756489735</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.011671071658824144</v>
+        <v>1.8531663249974447e-6</v>
       </c>
       <c r="C47">
-        <v>0.011670638647813507</v>
+        <v>1.853012895368771e-6</v>
       </c>
       <c r="D47">
-        <v>0.01166375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>1.852944744777265e-6</v>
+      </c>
+      <c r="E47">
+        <v>1.852893581402168e-6</v>
+      </c>
+      <c r="F47">
+        <v>1.853132452312067e-6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48">
-        <v>0.005833340624621853</v>
+        <v>1.8514179014854117e-6</v>
       </c>
       <c r="C48">
-        <v>0.005833229204181795</v>
+        <v>1.8517912810201577e-6</v>
       </c>
       <c r="D48">
+        <v>1.8518815390585768e-6</v>
+      </c>
+      <c r="E48">
+        <v>1.8519993115151072e-6</v>
+      </c>
+      <c r="F48">
+        <v>1.8524289984240668e-6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>1.672248414503899e-6</v>
+      </c>
+      <c r="C49">
+        <v>1.6723735136409043e-6</v>
+      </c>
+      <c r="D49">
+        <v>1.6724290929278828e-6</v>
+      </c>
+      <c r="E49">
+        <v>1.6724708236081307e-6</v>
+      </c>
+      <c r="F49">
+        <v>1.6722760292885052e-6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>1.6717395248228366e-6</v>
+      </c>
+      <c r="C50">
+        <v>1.6714348655626888e-6</v>
+      </c>
+      <c r="D50">
+        <v>1.671361254415699e-6</v>
+      </c>
+      <c r="E50">
+        <v>1.6712652239204567e-6</v>
+      </c>
+      <c r="F50">
+        <v>1.6709150572101737e-6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>0.011663750246519798</v>
+      </c>
+      <c r="C51">
+        <v>0.011663750215598144</v>
+      </c>
+      <c r="D51">
+        <v>0.011663750061428916</v>
+      </c>
+      <c r="E51">
+        <v>0.01166374981472745</v>
+      </c>
+      <c r="F51">
+        <v>0.01166375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>0.005833624121190807</v>
+      </c>
+      <c r="C52">
+        <v>0.005833623917786131</v>
+      </c>
+      <c r="D52">
+        <v>0.00583362387761201</v>
+      </c>
+      <c r="E52">
+        <v>0.005833624050406454</v>
+      </c>
+      <c r="F52">
         <v>0.005833624999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Not much changed even after using actual dollar amount for objective function
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -623,19 +623,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.051314204920749056</v>
+        <v>-8.11407673534362e-9</v>
       </c>
       <c r="C5">
-        <v>0.0515336941156942</v>
+        <v>-8.114076735446819e-9</v>
       </c>
       <c r="D5">
-        <v>0.05166669096078263</v>
+        <v>-8.114076735509334e-9</v>
       </c>
       <c r="E5">
-        <v>0.05173997845342276</v>
+        <v>-8.114076735543718e-9</v>
       </c>
       <c r="F5">
-        <v>0.05090273745527078</v>
+        <v>-8.114076735149643e-9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -643,19 +643,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.04267080145312797</v>
+        <v>0.04267278849067333</v>
       </c>
       <c r="C6">
-        <v>0.042891099738211896</v>
+        <v>0.04289296817092081</v>
       </c>
       <c r="D6">
-        <v>0.04302459369637416</v>
+        <v>0.043026375592555566</v>
       </c>
       <c r="E6">
-        <v>0.04309810318636273</v>
+        <v>0.04309975312991184</v>
       </c>
       <c r="F6">
-        <v>0.04225781230236308</v>
+        <v>0.04225941696976104</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -663,19 +663,19 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.005024022632188014</v>
+        <v>-0.18616990724214555</v>
       </c>
       <c r="C7">
-        <v>0.00502350080532581</v>
+        <v>-0.18634528991700805</v>
       </c>
       <c r="D7">
-        <v>0.005023212975893911</v>
+        <v>-0.18645157012503108</v>
       </c>
       <c r="E7">
-        <v>0.00502308366643496</v>
+        <v>-0.18651002881727677</v>
       </c>
       <c r="F7">
-        <v>0.005025024263081777</v>
+        <v>-0.18584064589797633</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -683,19 +683,19 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.0036193808354330723</v>
+        <v>0.14349711063739545</v>
       </c>
       <c r="C8">
-        <v>0.003619093572156492</v>
+        <v>0.1434523136320105</v>
       </c>
       <c r="D8">
-        <v>0.0036188842885145544</v>
+        <v>0.14342518641839877</v>
       </c>
       <c r="E8">
-        <v>0.0036187916006250693</v>
+        <v>0.14341026757328817</v>
       </c>
       <c r="F8">
-        <v>0.0036199008898259236</v>
+        <v>0.14358122081413854</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -703,19 +703,19 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.005000571378385479</v>
+        <v>0.005000571413263254</v>
       </c>
       <c r="C9">
-        <v>0.005180603942595949</v>
+        <v>0.0051806039760951</v>
       </c>
       <c r="D9">
-        <v>0.005247282882398706</v>
+        <v>0.0052472829146299966</v>
       </c>
       <c r="E9">
-        <v>0.005307294026718522</v>
+        <v>0.005307294056865159</v>
       </c>
       <c r="F9">
-        <v>0.005213943399840193</v>
+        <v>0.005213943428881287</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -723,19 +723,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.009997986470737593</v>
+        <v>0.009998062702596202</v>
       </c>
       <c r="C10">
-        <v>0.010357918891993494</v>
+        <v>0.010358011163705293</v>
       </c>
       <c r="D10">
-        <v>0.010491227353330477</v>
+        <v>0.010491325447960506</v>
       </c>
       <c r="E10">
-        <v>0.01061120501823848</v>
+        <v>0.010611308244979203</v>
       </c>
       <c r="F10">
-        <v>0.01042457299775907</v>
+        <v>0.010424667425185137</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -743,19 +743,19 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.01766895580256375</v>
+        <v>0.017669841922028157</v>
       </c>
       <c r="C11">
-        <v>0.01698919222325956</v>
+        <v>0.01699000255435733</v>
       </c>
       <c r="D11">
-        <v>0.016789301477448892</v>
+        <v>0.01679006037467482</v>
       </c>
       <c r="E11">
-        <v>0.016562756455375614</v>
+        <v>0.016563438988404514</v>
       </c>
       <c r="F11">
-        <v>0.016189310662511343</v>
+        <v>0.016189974347630958</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -763,19 +763,19 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.005000668116901921</v>
+        <v>0.005000668208116438</v>
       </c>
       <c r="C12">
-        <v>0.005180707778426727</v>
+        <v>0.0051807078634956375</v>
       </c>
       <c r="D12">
-        <v>0.00524738941229492</v>
+        <v>0.00524738949265046</v>
       </c>
       <c r="E12">
-        <v>0.005307403012073319</v>
+        <v>0.005307403085154682</v>
       </c>
       <c r="F12">
-        <v>0.005214048579497665</v>
+        <v>0.005214048649905797</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -783,19 +783,19 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.0050006308002073455</v>
+        <v>0.005000630883280346</v>
       </c>
       <c r="C13">
-        <v>0.005180667725089316</v>
+        <v>0.005180667802565203</v>
       </c>
       <c r="D13">
-        <v>0.005247348320592993</v>
+        <v>0.005247348393776196</v>
       </c>
       <c r="E13">
-        <v>0.005307360974301607</v>
+        <v>0.005307361040859895</v>
       </c>
       <c r="F13">
-        <v>0.005214008008394043</v>
+        <v>0.005214008072517727</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -803,19 +803,19 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.005000309292381279</v>
+        <v>0.005000309305316134</v>
       </c>
       <c r="C14">
-        <v>0.0051803226404165915</v>
+        <v>0.005180322652479951</v>
       </c>
       <c r="D14">
-        <v>0.005246994290186291</v>
+        <v>0.0052469943015812604</v>
       </c>
       <c r="E14">
-        <v>0.005306998793314076</v>
+        <v>0.005306998803677514</v>
       </c>
       <c r="F14">
-        <v>0.005213658463051959</v>
+        <v>0.005213658473036318</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -823,19 +823,19 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.014659372182184523</v>
+        <v>0.02398164072690172</v>
       </c>
       <c r="C15">
-        <v>0.01617955371008737</v>
+        <v>0.024521582990941784</v>
       </c>
       <c r="D15">
-        <v>0.016868088566846896</v>
+        <v>0.024691603687843535</v>
       </c>
       <c r="E15">
-        <v>0.01765962826269832</v>
+        <v>0.024812503388652454</v>
       </c>
       <c r="F15">
-        <v>0.01727176232328896</v>
+        <v>0.02441143085231938</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -843,19 +843,19 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>7.405262328279441e-5</v>
+        <v>-1.4221559355755569</v>
       </c>
       <c r="C16">
-        <v>7.435898984486915e-5</v>
+        <v>-1.4221137819375027</v>
       </c>
       <c r="D16">
-        <v>7.4533641702042e-5</v>
+        <v>-1.4220882280638245</v>
       </c>
       <c r="E16">
-        <v>7.461188834528784e-5</v>
+        <v>-1.4220741693655379</v>
       </c>
       <c r="F16">
-        <v>7.346964245218109e-5</v>
+        <v>-1.4222350234058094</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -863,19 +863,19 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4.989258095798899e-5</v>
+        <v>-1.512188508422315</v>
       </c>
       <c r="C17">
-        <v>5.009480240295952e-5</v>
+        <v>-1.5121838355430783</v>
       </c>
       <c r="D17">
-        <v>5.019453492239171e-5</v>
+        <v>-1.5121810183281013</v>
       </c>
       <c r="E17">
-        <v>5.0265615559787286e-5</v>
+        <v>-1.5121794625517695</v>
       </c>
       <c r="F17">
-        <v>4.950012143843453e-5</v>
+        <v>-1.512197167428314</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -883,19 +883,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.0025000759768043493</v>
+        <v>0.00250007601218117</v>
       </c>
       <c r="C18">
-        <v>0.002590090878181582</v>
+        <v>0.0025900909121600534</v>
       </c>
       <c r="D18">
-        <v>0.0026234299458988463</v>
+        <v>0.002623429978591316</v>
       </c>
       <c r="E18">
-        <v>0.0026534352067510607</v>
+        <v>0.0026534352373290483</v>
       </c>
       <c r="F18">
-        <v>0.0026067603992019754</v>
+        <v>0.002606760428658602</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -903,19 +903,19 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.002732657152935766</v>
+        <v>0.005486378506089839</v>
       </c>
       <c r="C19">
-        <v>0.002849323378917998</v>
+        <v>0.0056526226661973615</v>
       </c>
       <c r="D19">
-        <v>0.0028907272848052953</v>
+        <v>0.005714217264325665</v>
       </c>
       <c r="E19">
-        <v>0.0029241288897002282</v>
+        <v>0.005769853927509638</v>
       </c>
       <c r="F19">
-        <v>0.0028459354632558295</v>
+        <v>0.005685351023857658</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -923,19 +923,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.004414547343748728</v>
+        <v>0.010980998086839227</v>
       </c>
       <c r="C20">
-        <v>0.005547656394314283</v>
+        <v>0.011084410356678278</v>
       </c>
       <c r="D20">
-        <v>0.006094579198109388</v>
+        <v>0.011092712039849965</v>
       </c>
       <c r="E20">
-        <v>0.0067625132224153044</v>
+        <v>0.011067895241514823</v>
       </c>
       <c r="F20">
-        <v>0.00659334955139506</v>
+        <v>0.0108918705180177</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -943,19 +943,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.0025001737395008465</v>
+        <v>0.0025001738319419646</v>
       </c>
       <c r="C21">
-        <v>0.002590195813344445</v>
+        <v>0.0025901958995573145</v>
       </c>
       <c r="D21">
-        <v>0.0026235376036582996</v>
+        <v>0.002623537685094416</v>
       </c>
       <c r="E21">
-        <v>0.002653545345976505</v>
+        <v>0.0026535454200406258</v>
       </c>
       <c r="F21">
-        <v>0.002606866692424894</v>
+        <v>0.0026068667637798356</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -963,19 +963,19 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.0025001977597068925</v>
+        <v>0.00250019785738736</v>
       </c>
       <c r="C22">
-        <v>0.002590221594870122</v>
+        <v>0.0025902216859692846</v>
       </c>
       <c r="D22">
-        <v>0.0026235640534757873</v>
+        <v>0.0026235641395274466</v>
       </c>
       <c r="E22">
-        <v>0.0026535724046821575</v>
+        <v>0.0026535724829439837</v>
       </c>
       <c r="F22">
-        <v>0.002606892807185479</v>
+        <v>0.002606892882584602</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -983,19 +983,19 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.0024998716516098636</v>
+        <v>0.0024998716781486205</v>
       </c>
       <c r="C23">
-        <v>0.002589871572578869</v>
+        <v>0.0025898715973295544</v>
       </c>
       <c r="D23">
-        <v>0.0026232049574511844</v>
+        <v>0.0026232049808305163</v>
       </c>
       <c r="E23">
-        <v>0.0026532050414547416</v>
+        <v>0.0026532050627176575</v>
       </c>
       <c r="F23">
-        <v>0.0026065382603997077</v>
+        <v>0.0026065382808848577</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1003,19 +1003,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.0019188368768929206</v>
+        <v>0.0022585407879416454</v>
       </c>
       <c r="C24">
-        <v>0.001980793073940546</v>
+        <v>0.002300984733434881</v>
       </c>
       <c r="D24">
-        <v>0.002013052001004336</v>
+        <v>0.002319675975362818</v>
       </c>
       <c r="E24">
-        <v>0.0020447804783942074</v>
+        <v>0.0023312743871574657</v>
       </c>
       <c r="F24">
-        <v>0.0019644027968446862</v>
+        <v>0.0022450525323725206</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1023,19 +1023,19 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>2.371104479111432e-5</v>
+        <v>1.9390958049051548</v>
       </c>
       <c r="C25">
-        <v>2.3706205504398593e-5</v>
+        <v>1.9390443734749772</v>
       </c>
       <c r="D25">
-        <v>2.3703291845529456e-5</v>
+        <v>1.9390132117717318</v>
       </c>
       <c r="E25">
-        <v>2.3701685981049558e-5</v>
+        <v>1.93899607314067</v>
       </c>
       <c r="F25">
-        <v>2.3720229748177704e-5</v>
+        <v>1.9391923908364115</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1043,19 +1043,19 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1.2307855614160535e-5</v>
+        <v>2.174856730854773</v>
       </c>
       <c r="C26">
-        <v>1.2306034363860468e-5</v>
+        <v>2.1748312930174447</v>
       </c>
       <c r="D26">
-        <v>1.2304947451612389e-5</v>
+        <v>2.1748159263729168</v>
       </c>
       <c r="E26">
-        <v>1.2304345175344038e-5</v>
+        <v>2.174807457636802</v>
       </c>
       <c r="F26">
-        <v>1.2311317445593029e-5</v>
+        <v>2.1749041758382623</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1063,19 +1063,19 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2.9474042144264115e-5</v>
+        <v>2.9477240831714792e-5</v>
       </c>
       <c r="C27">
-        <v>3.1635147445243404e-5</v>
+        <v>3.163821969727627e-5</v>
       </c>
       <c r="D27">
-        <v>3.245502872889913e-5</v>
+        <v>3.24579847037672e-5</v>
       </c>
       <c r="E27">
-        <v>3.320195520669227e-5</v>
+        <v>3.320471999513211e-5</v>
       </c>
       <c r="F27">
-        <v>3.204392728430245e-5</v>
+        <v>3.204659068193962e-5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1083,19 +1083,19 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.00010130030175364274</v>
+        <v>0.00012265950077622456</v>
       </c>
       <c r="C28">
-        <v>0.00010882598907297721</v>
+        <v>0.0001313170285372922</v>
       </c>
       <c r="D28">
-        <v>0.00011167220676901554</v>
+        <v>0.00013459903746485555</v>
       </c>
       <c r="E28">
-        <v>0.0001142441603560652</v>
+        <v>0.0001375897453592473</v>
       </c>
       <c r="F28">
-        <v>0.00011011522258086881</v>
+        <v>0.00013297280163801077</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1103,19 +1103,19 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.00031276907899746575</v>
+        <v>0.00040817369267680693</v>
       </c>
       <c r="C29">
-        <v>0.00030120383813518283</v>
+        <v>0.000388106490190614</v>
       </c>
       <c r="D29">
-        <v>0.0003008438367533325</v>
+        <v>0.00038191144746627467</v>
       </c>
       <c r="E29">
-        <v>0.0003018198770550414</v>
+        <v>0.0003742649568761022</v>
       </c>
       <c r="F29">
-        <v>0.00028815240899914506</v>
+        <v>0.00035907983395989663</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1123,19 +1123,19 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>2.9486152075728904e-5</v>
+        <v>2.949258464304242e-5</v>
       </c>
       <c r="C30">
-        <v>3.164844300236681e-5</v>
+        <v>3.165444217345958e-5</v>
       </c>
       <c r="D30">
-        <v>3.246887863941623e-5</v>
+        <v>3.247454541748751e-5</v>
       </c>
       <c r="E30">
-        <v>3.321638890840964e-5</v>
+        <v>3.3221542701979445e-5</v>
       </c>
       <c r="F30">
-        <v>3.2057542130117967e-5</v>
+        <v>3.2062507403936046e-5</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1143,19 +1143,19 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>2.9485913314018506e-5</v>
+        <v>2.9492345777144864e-5</v>
       </c>
       <c r="C31">
-        <v>3.164817749666981e-5</v>
+        <v>3.165417656709492e-5</v>
       </c>
       <c r="D31">
-        <v>3.246860274038923e-5</v>
+        <v>3.247426942214567e-5</v>
       </c>
       <c r="E31">
-        <v>3.3216103424110566e-5</v>
+        <v>3.3221257129081806e-5</v>
       </c>
       <c r="F31">
-        <v>3.2057271457742984e-5</v>
+        <v>3.206223664770651e-5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1163,19 +1163,19 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>2.9485913314018506e-5</v>
+        <v>2.9492345777144857e-5</v>
       </c>
       <c r="C32">
-        <v>3.16481774966698e-5</v>
+        <v>3.1654176567094915e-5</v>
       </c>
       <c r="D32">
-        <v>3.246860274038923e-5</v>
+        <v>3.247426942214569e-5</v>
       </c>
       <c r="E32">
-        <v>3.321610342411056e-5</v>
+        <v>3.32212571290818e-5</v>
       </c>
       <c r="F32">
-        <v>3.205727145774298e-5</v>
+        <v>3.2062236647706516e-5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1203,19 +1203,19 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1.0604617394225673</v>
+        <v>1.0603466825226278</v>
       </c>
       <c r="C34">
-        <v>1.060441650393495</v>
+        <v>1.0603386919800197</v>
       </c>
       <c r="D34">
-        <v>1.0604323482943674</v>
+        <v>1.0603357895706005</v>
       </c>
       <c r="E34">
-        <v>1.060422136686849</v>
+        <v>1.060333855243991</v>
       </c>
       <c r="F34">
-        <v>1.060431989315611</v>
+        <v>1.0603438708737556</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1223,19 +1223,19 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1.060858371812388</v>
+        <v>1.0859808453709558</v>
       </c>
       <c r="C35">
-        <v>1.0608583709639388</v>
+        <v>1.0859815575394023</v>
       </c>
       <c r="D35">
-        <v>1.060858370402619</v>
+        <v>1.0859819889559348</v>
       </c>
       <c r="E35">
-        <v>1.0608583701539906</v>
+        <v>1.0859822262048857</v>
       </c>
       <c r="F35">
-        <v>1.0608583733572843</v>
+        <v>1.0859795075184864</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1243,19 +1243,19 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1.0602973956553108</v>
+        <v>1.0601823387545997</v>
       </c>
       <c r="C36">
-        <v>1.0602713899852751</v>
+        <v>1.0601684315710587</v>
       </c>
       <c r="D36">
-        <v>1.0602598965329457</v>
+        <v>1.0601633378084658</v>
       </c>
       <c r="E36">
-        <v>1.0602477127053669</v>
+        <v>1.0601594312618416</v>
       </c>
       <c r="F36">
-        <v>1.06026063323107</v>
+        <v>1.0601725147885723</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1263,19 +1263,19 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1.0603677021379236</v>
+        <v>1.060218657731482</v>
       </c>
       <c r="C37">
-        <v>1.0603440021670187</v>
+        <v>1.0602064442835548</v>
       </c>
       <c r="D37">
-        <v>1.0603333849722005</v>
+        <v>1.0602019775584375</v>
       </c>
       <c r="E37">
-        <v>1.0603220374447273</v>
+        <v>1.060198632862457</v>
       </c>
       <c r="F37">
-        <v>1.0603339808671042</v>
+        <v>1.0602108171911862</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1283,19 +1283,19 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>1.060075599651318</v>
+        <v>1.0598444353356313</v>
       </c>
       <c r="C38">
-        <v>1.0600473279019493</v>
+        <v>1.0598464689767166</v>
       </c>
       <c r="D38">
-        <v>1.0600318410838698</v>
+        <v>1.059846905636889</v>
       </c>
       <c r="E38">
-        <v>1.0600137700939622</v>
+        <v>1.0598493610120587</v>
       </c>
       <c r="F38">
-        <v>1.0600331242956231</v>
+        <v>1.0598689996251651</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1303,19 +1303,19 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1.059861932636617</v>
+        <v>1.0596307683183084</v>
       </c>
       <c r="C39">
-        <v>1.0598259684260423</v>
+        <v>1.0596251094983642</v>
       </c>
       <c r="D39">
-        <v>1.0598076325402732</v>
+        <v>1.0596226970909828</v>
       </c>
       <c r="E39">
-        <v>1.0597869973857286</v>
+        <v>1.0596225883017243</v>
       </c>
       <c r="F39">
-        <v>1.059810340286327</v>
+        <v>1.0596462156138453</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1323,19 +1323,19 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>1.059911251897293</v>
+        <v>1.0596800875791859</v>
       </c>
       <c r="C40">
-        <v>1.0598770632145331</v>
+        <v>1.0596762042870431</v>
       </c>
       <c r="D40">
-        <v>1.0598593849322713</v>
+        <v>1.059674449483158</v>
       </c>
       <c r="E40">
-        <v>1.0598393416211682</v>
+        <v>1.0596749325373254</v>
       </c>
       <c r="F40">
-        <v>1.0598617638765369</v>
+        <v>1.0596976392042103</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1343,19 +1343,19 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1.0598705148516268</v>
+        <v>1.059639350533384</v>
       </c>
       <c r="C41">
-        <v>1.0598348596120346</v>
+        <v>1.0596340006844183</v>
       </c>
       <c r="D41">
-        <v>1.0598166381601632</v>
+        <v>1.0596317027109308</v>
       </c>
       <c r="E41">
-        <v>1.0597961059962193</v>
+        <v>1.0596316969122677</v>
       </c>
       <c r="F41">
-        <v>1.059819288689257</v>
+        <v>1.059655164016826</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1363,19 +1363,19 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>1.060843889514316</v>
+        <v>1.0823989433572518</v>
       </c>
       <c r="C42">
-        <v>1.0608438907722857</v>
+        <v>1.082399552851273</v>
       </c>
       <c r="D42">
-        <v>1.0608438924263985</v>
+        <v>1.082399922133606</v>
       </c>
       <c r="E42">
-        <v>1.0608438927419062</v>
+        <v>1.0824001251219446</v>
       </c>
       <c r="F42">
-        <v>1.0608438876454969</v>
+        <v>1.0823977971651118</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1383,19 +1383,19 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.0045268852161094745</v>
+        <v>-0.0008919103824805479</v>
       </c>
       <c r="C43">
-        <v>0.003694958320204721</v>
+        <v>-0.0006316482174238614</v>
       </c>
       <c r="D43">
-        <v>0.0032580775980534937</v>
+        <v>-0.0005055935395941902</v>
       </c>
       <c r="E43">
-        <v>0.0026852866742830793</v>
+        <v>-0.00035964865734512333</v>
       </c>
       <c r="F43">
-        <v>0.002675699699297939</v>
+        <v>-0.00036823806952544563</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1403,19 +1403,19 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>1.7475176701477044e-20</v>
+        <v>9.967310392012425e-22</v>
       </c>
       <c r="C44">
-        <v>1.5767987415293315e-19</v>
+        <v>-9.829717723932946e-20</v>
       </c>
       <c r="D44">
-        <v>-8.004823744950932e-20</v>
+        <v>5.999115317587511e-20</v>
       </c>
       <c r="E44">
-        <v>6.278478846541676e-20</v>
+        <v>4.093159761592188e-20</v>
       </c>
       <c r="F44">
-        <v>6.278478846541676e-20</v>
+        <v>4.093159761592188e-20</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1423,19 +1423,19 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.002268218001124278</v>
+        <v>-0.00048537153810864213</v>
       </c>
       <c r="C45">
-        <v>0.0023316072183796367</v>
+        <v>-0.00047155327005715377</v>
       </c>
       <c r="D45">
-        <v>0.0023568908773417777</v>
+        <v>-0.0004664576139397097</v>
       </c>
       <c r="E45">
-        <v>0.0023835081447315214</v>
+        <v>-0.00046207282058258284</v>
       </c>
       <c r="F45">
-        <v>0.002368338090282289</v>
+        <v>-0.00047093640945295893</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1443,19 +1443,19 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.0010619540996073718</v>
+        <v>-8.485739208970507e-5</v>
       </c>
       <c r="C46">
-        <v>0.0011207246068114895</v>
+        <v>-8.86543429255147e-5</v>
       </c>
       <c r="D46">
-        <v>0.0011440335913507895</v>
+        <v>-8.971123458695566e-5</v>
       </c>
       <c r="E46">
-        <v>0.001168918213414903</v>
+        <v>-9.088784199941676e-5</v>
       </c>
       <c r="F46">
-        <v>0.0011608517756489735</v>
+        <v>-9.310421310054262e-5</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1463,19 +1463,19 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>1.8531663249974447e-6</v>
+        <v>2.0993320770248966e-6</v>
       </c>
       <c r="C47">
-        <v>1.853012895368771e-6</v>
+        <v>2.106139472085875e-6</v>
       </c>
       <c r="D47">
-        <v>1.852944744777265e-6</v>
+        <v>2.108555783440064e-6</v>
       </c>
       <c r="E47">
-        <v>1.852893581402168e-6</v>
+        <v>2.1106361979856894e-6</v>
       </c>
       <c r="F47">
-        <v>1.853132452312067e-6</v>
+        <v>2.1068380473971538e-6</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1483,19 +1483,19 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>1.8514179014854117e-6</v>
+        <v>2.374521956174667e-6</v>
       </c>
       <c r="C48">
-        <v>1.8517912810201577e-6</v>
+        <v>2.3739899784138335e-6</v>
       </c>
       <c r="D48">
-        <v>1.8518815390585768e-6</v>
+        <v>2.3737793004399404e-6</v>
       </c>
       <c r="E48">
-        <v>1.8519993115151072e-6</v>
+        <v>2.3732545600553326e-6</v>
       </c>
       <c r="F48">
-        <v>1.8524289984240668e-6</v>
+        <v>2.370592455300252e-6</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1503,19 +1503,19 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>1.672248414503899e-6</v>
+        <v>1.906608213206597e-6</v>
       </c>
       <c r="C49">
-        <v>1.6723735136409043e-6</v>
+        <v>1.9010682622889227e-6</v>
       </c>
       <c r="D49">
-        <v>1.6724290929278828e-6</v>
+        <v>1.8990998655082748e-6</v>
       </c>
       <c r="E49">
-        <v>1.6724708236081307e-6</v>
+        <v>1.8974041550411791e-6</v>
       </c>
       <c r="F49">
-        <v>1.6722760292885052e-6</v>
+        <v>1.900499678040642e-6</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1523,19 +1523,19 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>1.6717395248228366e-6</v>
+        <v>2.140784145672382e-6</v>
       </c>
       <c r="C50">
-        <v>1.6714348655626888e-6</v>
+        <v>2.1412174339978615e-6</v>
       </c>
       <c r="D50">
-        <v>1.671361254415699e-6</v>
+        <v>2.1413887907442063e-6</v>
       </c>
       <c r="E50">
-        <v>1.6712652239204567e-6</v>
+        <v>2.141815915988925e-6</v>
       </c>
       <c r="F50">
-        <v>1.6709150572101737e-6</v>
+        <v>2.1439834845688995e-6</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1543,16 +1543,16 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.011663750246519798</v>
+        <v>0.011663737409459272</v>
       </c>
       <c r="C51">
-        <v>0.011663750215598144</v>
+        <v>0.011663737117471134</v>
       </c>
       <c r="D51">
-        <v>0.011663750061428916</v>
+        <v>0.011663741192975394</v>
       </c>
       <c r="E51">
-        <v>0.01166374981472745</v>
+        <v>0.011663749029831859</v>
       </c>
       <c r="F51">
         <v>0.01166375</v>
@@ -1563,16 +1563,16 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.005833624121190807</v>
+        <v>0.0058336273388629204</v>
       </c>
       <c r="C52">
-        <v>0.005833623917786131</v>
+        <v>0.005833628716253995</v>
       </c>
       <c r="D52">
-        <v>0.00583362387761201</v>
+        <v>0.005833629713125472</v>
       </c>
       <c r="E52">
-        <v>0.005833624050406454</v>
+        <v>0.005833629761888063</v>
       </c>
       <c r="F52">
         <v>0.005833624999999999</v>

</xml_diff>

<commit_message>
Need to add output values to the table
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -623,19 +623,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-8.11407673534362e-9</v>
+        <v>-4.30813814202642e-9</v>
       </c>
       <c r="C5">
-        <v>-8.114076735446819e-9</v>
+        <v>-4.3081376419921005e-9</v>
       </c>
       <c r="D5">
-        <v>-8.114076735509334e-9</v>
+        <v>-4.308137523078548e-9</v>
       </c>
       <c r="E5">
-        <v>-8.114076735543718e-9</v>
+        <v>-4.3081371509771066e-9</v>
       </c>
       <c r="F5">
-        <v>-8.114076735149643e-9</v>
+        <v>-9.090908574732907e-9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -643,19 +643,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.04267278849067333</v>
+        <v>0.04267407439113609</v>
       </c>
       <c r="C6">
-        <v>0.04289296817092081</v>
+        <v>0.042894280744237914</v>
       </c>
       <c r="D6">
-        <v>0.043026375592555566</v>
+        <v>0.0430276985218409</v>
       </c>
       <c r="E6">
-        <v>0.04309975312991184</v>
+        <v>0.043101077761150575</v>
       </c>
       <c r="F6">
-        <v>0.04225941696976104</v>
+        <v>0.042260660261863925</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -663,19 +663,19 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.18616990724214555</v>
+        <v>-0.05333160688517414</v>
       </c>
       <c r="C7">
-        <v>-0.18634528991700805</v>
+        <v>-0.053288804082253866</v>
       </c>
       <c r="D7">
-        <v>-0.18645157012503108</v>
+        <v>-0.05557683628089839</v>
       </c>
       <c r="E7">
-        <v>-0.18651002881727677</v>
+        <v>-0.06525313270591816</v>
       </c>
       <c r="F7">
-        <v>-0.18584064589797633</v>
+        <v>-0.030267369093617522</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -683,19 +683,19 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.14349711063739545</v>
+        <v>0.010657528185899915</v>
       </c>
       <c r="C8">
-        <v>0.1434523136320105</v>
+        <v>0.010394519029878308</v>
       </c>
       <c r="D8">
-        <v>0.14342518641839877</v>
+        <v>0.012549133450919972</v>
       </c>
       <c r="E8">
-        <v>0.14341026757328817</v>
+        <v>0.022152050636630435</v>
       </c>
       <c r="F8">
-        <v>0.14358122081413854</v>
+        <v>-0.011993300259154982</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -703,19 +703,19 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.005000571413263254</v>
+        <v>0.005000571413257865</v>
       </c>
       <c r="C9">
-        <v>0.0051806039760951</v>
+        <v>0.0051806039760923725</v>
       </c>
       <c r="D9">
-        <v>0.0052472829146299966</v>
+        <v>0.0052472829146281595</v>
       </c>
       <c r="E9">
-        <v>0.005307294056865159</v>
+        <v>0.005307294056864217</v>
       </c>
       <c r="F9">
-        <v>0.005213943428881287</v>
+        <v>0.0052139434288796084</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -723,19 +723,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.009998062702596202</v>
+        <v>0.009998580069983257</v>
       </c>
       <c r="C10">
-        <v>0.010358011163705293</v>
+        <v>0.01035856792971497</v>
       </c>
       <c r="D10">
-        <v>0.010491325447960506</v>
+        <v>0.010491901005877567</v>
       </c>
       <c r="E10">
-        <v>0.010611308244979203</v>
+        <v>0.010611904026549646</v>
       </c>
       <c r="F10">
-        <v>0.010424667425185137</v>
+        <v>0.010425251031502618</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -743,19 +743,19 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.017669841922028157</v>
+        <v>0.017670610425920653</v>
       </c>
       <c r="C11">
-        <v>0.01699000255435733</v>
+        <v>0.016990758226373782</v>
       </c>
       <c r="D11">
-        <v>0.01679006037467482</v>
+        <v>0.01679080757647534</v>
       </c>
       <c r="E11">
-        <v>0.016563438988404514</v>
+        <v>0.016564167637040973</v>
       </c>
       <c r="F11">
-        <v>0.016189974347630958</v>
+        <v>0.016190633876931777</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -763,19 +763,19 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.005000668208116438</v>
+        <v>0.005000668208106999</v>
       </c>
       <c r="C12">
-        <v>0.0051807078634956375</v>
+        <v>0.005180707863493138</v>
       </c>
       <c r="D12">
-        <v>0.00524738949265046</v>
+        <v>0.005247389492650469</v>
       </c>
       <c r="E12">
-        <v>0.005307403085154682</v>
+        <v>0.005307403085157084</v>
       </c>
       <c r="F12">
-        <v>0.005214048649905797</v>
+        <v>0.0052140486499064305</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -783,19 +783,19 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.005000630883280346</v>
+        <v>0.005000630883271751</v>
       </c>
       <c r="C13">
-        <v>0.005180667802565203</v>
+        <v>0.005180667802562927</v>
       </c>
       <c r="D13">
-        <v>0.005247348393776196</v>
+        <v>0.005247348393776203</v>
       </c>
       <c r="E13">
-        <v>0.005307361040859895</v>
+        <v>0.005307361040862082</v>
       </c>
       <c r="F13">
-        <v>0.005214008072517727</v>
+        <v>0.005214008072518304</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -803,19 +803,19 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.005000309305316134</v>
+        <v>0.0050003093053147965</v>
       </c>
       <c r="C14">
-        <v>0.005180322652479951</v>
+        <v>0.005180322652479597</v>
       </c>
       <c r="D14">
-        <v>0.0052469943015812604</v>
+        <v>0.005246994301581261</v>
       </c>
       <c r="E14">
-        <v>0.005306998803677514</v>
+        <v>0.005306998803677855</v>
       </c>
       <c r="F14">
-        <v>0.005213658473036318</v>
+        <v>0.005213658473036407</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -823,19 +823,19 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.02398164072690172</v>
+        <v>0.02397957211052107</v>
       </c>
       <c r="C15">
-        <v>0.024521582990941784</v>
+        <v>0.024520262607329243</v>
       </c>
       <c r="D15">
-        <v>0.024691603687843535</v>
+        <v>0.024690511467573107</v>
       </c>
       <c r="E15">
-        <v>0.024812503388652454</v>
+        <v>0.024811632614961734</v>
       </c>
       <c r="F15">
-        <v>0.02441143085231938</v>
+        <v>0.02441041081199054</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -843,19 +843,19 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-1.4221559355755569</v>
+        <v>0.18514854580690884</v>
       </c>
       <c r="C16">
-        <v>-1.4221137819375027</v>
+        <v>0.18528930995297396</v>
       </c>
       <c r="D16">
-        <v>-1.4220882280638245</v>
+        <v>0.18419856393761458</v>
       </c>
       <c r="E16">
-        <v>-1.4220741693655379</v>
+        <v>0.1801950824656111</v>
       </c>
       <c r="F16">
-        <v>-1.4222350234058094</v>
+        <v>-0.20338184217921984</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -863,19 +863,19 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-1.512188508422315</v>
+        <v>0.19489585424575645</v>
       </c>
       <c r="C17">
-        <v>-1.5121838355430783</v>
+        <v>0.19503315331446322</v>
       </c>
       <c r="D17">
-        <v>-1.5121810183281013</v>
+        <v>0.19466177812698635</v>
       </c>
       <c r="E17">
-        <v>-1.5121794625517695</v>
+        <v>0.19345732332778878</v>
       </c>
       <c r="F17">
-        <v>-1.512197167428314</v>
+        <v>-0.20634294306688447</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -883,19 +883,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.00250007601218117</v>
+        <v>0.0025000760121757044</v>
       </c>
       <c r="C18">
-        <v>0.0025900909121600534</v>
+        <v>0.0025900909121572874</v>
       </c>
       <c r="D18">
-        <v>0.002623429978591316</v>
+        <v>0.002623429978589453</v>
       </c>
       <c r="E18">
-        <v>0.0026534352373290483</v>
+        <v>0.0026534352373280925</v>
       </c>
       <c r="F18">
-        <v>0.002606760428658602</v>
+        <v>0.0026067604286568995</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -903,19 +903,19 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.005486378506089839</v>
+        <v>0.005485414961530933</v>
       </c>
       <c r="C19">
-        <v>0.0056526226661973615</v>
+        <v>0.0056519068619503</v>
       </c>
       <c r="D19">
-        <v>0.005714217264325665</v>
+        <v>0.005713549235630298</v>
       </c>
       <c r="E19">
-        <v>0.005769853927509638</v>
+        <v>0.005769239685276451</v>
       </c>
       <c r="F19">
-        <v>0.005685351023857658</v>
+        <v>0.005684609531719483</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -923,19 +923,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.010980998086839227</v>
+        <v>0.01097989295530378</v>
       </c>
       <c r="C20">
-        <v>0.011084410356678278</v>
+        <v>0.011083805500507771</v>
       </c>
       <c r="D20">
-        <v>0.011092712039849965</v>
+        <v>0.011092287501341285</v>
       </c>
       <c r="E20">
-        <v>0.011067895241514823</v>
+        <v>0.011067638298749816</v>
       </c>
       <c r="F20">
-        <v>0.0108918705180177</v>
+        <v>0.010891591649661435</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -943,19 +943,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.0025001738319419646</v>
+        <v>0.0025001738319323993</v>
       </c>
       <c r="C21">
-        <v>0.0025901958995573145</v>
+        <v>0.002590195899554782</v>
       </c>
       <c r="D21">
-        <v>0.002623537685094416</v>
+        <v>0.002623537685094424</v>
       </c>
       <c r="E21">
-        <v>0.0026535454200406258</v>
+        <v>0.002653545420043059</v>
       </c>
       <c r="F21">
-        <v>0.0026068667637798356</v>
+        <v>0.0026068667637804775</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -963,19 +963,19 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.00250019785738736</v>
+        <v>0.0025001978573772525</v>
       </c>
       <c r="C22">
-        <v>0.0025902216859692846</v>
+        <v>0.002590221685966609</v>
       </c>
       <c r="D22">
-        <v>0.0026235641395274466</v>
+        <v>0.0026235641395274552</v>
       </c>
       <c r="E22">
-        <v>0.0026535724829439837</v>
+        <v>0.002653572482946556</v>
       </c>
       <c r="F22">
-        <v>0.002606892882584602</v>
+        <v>0.0026068928825852804</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -983,19 +983,19 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.0024998716781486205</v>
+        <v>0.002499871678145875</v>
       </c>
       <c r="C23">
-        <v>0.0025898715973295544</v>
+        <v>0.0025898715973288276</v>
       </c>
       <c r="D23">
-        <v>0.0026232049808305163</v>
+        <v>0.002623204980830519</v>
       </c>
       <c r="E23">
-        <v>0.0026532050627176575</v>
+        <v>0.0026532050627183566</v>
       </c>
       <c r="F23">
-        <v>0.0026065382808848577</v>
+        <v>0.002606538280885042</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1003,19 +1003,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.0022585407879416454</v>
+        <v>0.002258550464868548</v>
       </c>
       <c r="C24">
-        <v>0.002300984733434881</v>
+        <v>0.0023010295875199606</v>
       </c>
       <c r="D24">
-        <v>0.002319675975362818</v>
+        <v>0.0023197321929759756</v>
       </c>
       <c r="E24">
-        <v>0.0023312743871574657</v>
+        <v>0.0023313410357977448</v>
       </c>
       <c r="F24">
-        <v>0.0022450525323725206</v>
+        <v>0.002245104412455492</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1023,19 +1023,19 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1.9390958049051548</v>
+        <v>0.034993096112758186</v>
       </c>
       <c r="C25">
-        <v>1.9390443734749772</v>
+        <v>0.03503794560576232</v>
       </c>
       <c r="D25">
-        <v>1.9390132117717318</v>
+        <v>0.03489285229035758</v>
       </c>
       <c r="E25">
-        <v>1.93899607314067</v>
+        <v>0.03461982326703022</v>
       </c>
       <c r="F25">
-        <v>1.9391923908364115</v>
+        <v>0.03985314874887429</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1043,19 +1043,19 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>2.174856730854773</v>
+        <v>0.03591092899623125</v>
       </c>
       <c r="C26">
-        <v>2.1748312930174447</v>
+        <v>0.03595617374290462</v>
       </c>
       <c r="D26">
-        <v>2.1748159263729168</v>
+        <v>0.03586635488843895</v>
       </c>
       <c r="E26">
-        <v>2.174807457636802</v>
+        <v>0.035739820001720116</v>
       </c>
       <c r="F26">
-        <v>2.1749041758382623</v>
+        <v>0.04026879686539362</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1063,19 +1063,19 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2.9477240831714792e-5</v>
+        <v>2.9477240337494127e-5</v>
       </c>
       <c r="C27">
-        <v>3.163821969727627e-5</v>
+        <v>3.1638219447170265e-5</v>
       </c>
       <c r="D27">
-        <v>3.24579847037672e-5</v>
+        <v>3.245798453529442e-5</v>
       </c>
       <c r="E27">
-        <v>3.320471999513211e-5</v>
+        <v>3.3204719908694875e-5</v>
       </c>
       <c r="F27">
-        <v>3.204659068193962e-5</v>
+        <v>3.204659052801731e-5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1083,19 +1083,19 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.00012265950077622456</v>
+        <v>0.00012265919940622017</v>
       </c>
       <c r="C28">
-        <v>0.0001313170285372922</v>
+        <v>0.00013132019027135063</v>
       </c>
       <c r="D28">
-        <v>0.00013459903746485555</v>
+        <v>0.00013460314228443745</v>
       </c>
       <c r="E28">
-        <v>0.0001375897453592473</v>
+        <v>0.00013759490122489384</v>
       </c>
       <c r="F28">
-        <v>0.00013297280163801077</v>
+        <v>0.00013297623962034557</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1103,19 +1103,19 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.00040817369267680693</v>
+        <v>0.00040817636751258406</v>
       </c>
       <c r="C29">
-        <v>0.000388106490190614</v>
+        <v>0.00038811801583059195</v>
       </c>
       <c r="D29">
-        <v>0.00038191144746627467</v>
+        <v>0.0003819261832578754</v>
       </c>
       <c r="E29">
-        <v>0.0003742649568761022</v>
+        <v>0.0003742823131069778</v>
       </c>
       <c r="F29">
-        <v>0.00035907983395989663</v>
+        <v>0.00035909421012304837</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1123,19 +1123,19 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>2.949258464304242e-5</v>
+        <v>2.94925839774373e-5</v>
       </c>
       <c r="C30">
-        <v>3.165444217345958e-5</v>
+        <v>3.165444199722731e-5</v>
       </c>
       <c r="D30">
-        <v>3.247454541748751e-5</v>
+        <v>3.247454541806554e-5</v>
       </c>
       <c r="E30">
-        <v>3.3221542701979445e-5</v>
+        <v>3.32215428713223e-5</v>
       </c>
       <c r="F30">
-        <v>3.2062507403936046e-5</v>
+        <v>3.206250744860781e-5</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1143,19 +1143,19 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>2.9492345777144864e-5</v>
+        <v>2.9492345111550528e-5</v>
       </c>
       <c r="C31">
-        <v>3.165417656709492e-5</v>
+        <v>3.16541763908656e-5</v>
       </c>
       <c r="D31">
-        <v>3.247426942214567e-5</v>
+        <v>3.24742694227237e-5</v>
       </c>
       <c r="E31">
-        <v>3.3221257129081806e-5</v>
+        <v>3.3221257298421744e-5</v>
       </c>
       <c r="F31">
-        <v>3.206223664770651e-5</v>
+        <v>3.206223669237753e-5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1163,19 +1163,19 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>2.9492345777144857e-5</v>
+        <v>2.9492345111550528e-5</v>
       </c>
       <c r="C32">
-        <v>3.1654176567094915e-5</v>
+        <v>3.16541763908656e-5</v>
       </c>
       <c r="D32">
-        <v>3.247426942214569e-5</v>
+        <v>3.24742694227237e-5</v>
       </c>
       <c r="E32">
-        <v>3.32212571290818e-5</v>
+        <v>3.322125729842175e-5</v>
       </c>
       <c r="F32">
-        <v>3.2062236647706516e-5</v>
+        <v>3.206223669237752e-5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1203,19 +1203,19 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1.0603466825226278</v>
+        <v>1.060346700297827</v>
       </c>
       <c r="C34">
-        <v>1.0603386919800197</v>
+        <v>1.0603387003608413</v>
       </c>
       <c r="D34">
-        <v>1.0603357895706005</v>
+        <v>1.060335795073358</v>
       </c>
       <c r="E34">
-        <v>1.060333855243991</v>
+        <v>1.0603338580037491</v>
       </c>
       <c r="F34">
-        <v>1.0603438708737556</v>
+        <v>1.0603438759658415</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1223,19 +1223,19 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1.0859808453709558</v>
+        <v>1.0582828207010737</v>
       </c>
       <c r="C35">
-        <v>1.0859815575394023</v>
+        <v>1.0582801620312687</v>
       </c>
       <c r="D35">
-        <v>1.0859819889559348</v>
+        <v>1.058316516381771</v>
       </c>
       <c r="E35">
-        <v>1.0859822262048857</v>
+        <v>1.0584602553159828</v>
       </c>
       <c r="F35">
-        <v>1.0859795075184864</v>
+        <v>1.0644961639565997</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1243,19 +1243,19 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1.0601823387545997</v>
+        <v>1.0601823565297992</v>
       </c>
       <c r="C36">
-        <v>1.0601684315710587</v>
+        <v>1.0601684399518805</v>
       </c>
       <c r="D36">
-        <v>1.0601633378084658</v>
+        <v>1.0601633433112234</v>
       </c>
       <c r="E36">
-        <v>1.0601594312618416</v>
+        <v>1.0601594340216</v>
       </c>
       <c r="F36">
-        <v>1.0601725147885723</v>
+        <v>1.0601725198806582</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1263,19 +1263,19 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1.060218657731482</v>
+        <v>1.0602186842782253</v>
       </c>
       <c r="C37">
-        <v>1.0602064442835548</v>
+        <v>1.0602064581406496</v>
       </c>
       <c r="D37">
-        <v>1.0602019775584375</v>
+        <v>1.0602019878344746</v>
       </c>
       <c r="E37">
-        <v>1.060198632862457</v>
+        <v>1.0601986396096783</v>
       </c>
       <c r="F37">
-        <v>1.0602108171911862</v>
+        <v>1.0602108279146962</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1283,19 +1283,19 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>1.0598444353356313</v>
+        <v>1.0598444592499354</v>
       </c>
       <c r="C38">
-        <v>1.0598464689767166</v>
+        <v>1.0598464748760148</v>
       </c>
       <c r="D38">
-        <v>1.059846905636889</v>
+        <v>1.0598469056179907</v>
       </c>
       <c r="E38">
-        <v>1.0598493610120587</v>
+        <v>1.0598493556107205</v>
       </c>
       <c r="F38">
-        <v>1.0598689996251651</v>
+        <v>1.0598689981487588</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1303,19 +1303,19 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1.0596307683183084</v>
+        <v>1.0596307922326127</v>
       </c>
       <c r="C39">
-        <v>1.0596251094983642</v>
+        <v>1.0596251153976626</v>
       </c>
       <c r="D39">
-        <v>1.0596226970909828</v>
+        <v>1.0596226970720841</v>
       </c>
       <c r="E39">
-        <v>1.0596225883017243</v>
+        <v>1.059622582900386</v>
       </c>
       <c r="F39">
-        <v>1.0596462156138453</v>
+        <v>1.059646214137439</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1323,19 +1323,19 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>1.0596800875791859</v>
+        <v>1.05968011149349</v>
       </c>
       <c r="C40">
-        <v>1.0596762042870431</v>
+        <v>1.0596762101863413</v>
       </c>
       <c r="D40">
-        <v>1.059674449483158</v>
+        <v>1.0596744494642596</v>
       </c>
       <c r="E40">
-        <v>1.0596749325373254</v>
+        <v>1.0596749271359869</v>
       </c>
       <c r="F40">
-        <v>1.0596976392042103</v>
+        <v>1.0596976377278038</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1343,19 +1343,19 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1.059639350533384</v>
+        <v>1.0596393744476884</v>
       </c>
       <c r="C41">
-        <v>1.0596340006844183</v>
+        <v>1.0596340065837166</v>
       </c>
       <c r="D41">
-        <v>1.0596317027109308</v>
+        <v>1.059631702692032</v>
       </c>
       <c r="E41">
-        <v>1.0596316969122677</v>
+        <v>1.0596316915109292</v>
       </c>
       <c r="F41">
-        <v>1.059655164016826</v>
+        <v>1.0596551625404196</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1363,19 +1363,19 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>1.0823989433572518</v>
+        <v>1.057720892318825</v>
       </c>
       <c r="C42">
-        <v>1.082399552851273</v>
+        <v>1.0577227911701494</v>
       </c>
       <c r="D42">
-        <v>1.082399922133606</v>
+        <v>1.0576955928437255</v>
       </c>
       <c r="E42">
-        <v>1.0824001251219446</v>
+        <v>1.0575674196332712</v>
       </c>
       <c r="F42">
-        <v>1.0823977971651118</v>
+        <v>1.0642859594585514</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1383,19 +1383,19 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-0.0008919103824805479</v>
+        <v>-0.0008908827352805736</v>
       </c>
       <c r="C43">
-        <v>-0.0006316482174238614</v>
+        <v>-0.0006311047860027225</v>
       </c>
       <c r="D43">
-        <v>-0.0005055935395941902</v>
+        <v>-0.0005052228634117533</v>
       </c>
       <c r="E43">
-        <v>-0.00035964865734512333</v>
+        <v>-0.00035943700716228546</v>
       </c>
       <c r="F43">
-        <v>-0.00036823806952544563</v>
+        <v>-0.00036800863153772095</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1403,19 +1403,19 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>9.967310392012425e-22</v>
+        <v>1.438684068520384e-19</v>
       </c>
       <c r="C44">
-        <v>-9.829717723932946e-20</v>
+        <v>-1.0963699529388172e-19</v>
       </c>
       <c r="D44">
-        <v>5.999115317587511e-20</v>
+        <v>1.497565535865285e-19</v>
       </c>
       <c r="E44">
-        <v>4.093159761592188e-20</v>
+        <v>8.922480328977489e-20</v>
       </c>
       <c r="F44">
-        <v>4.093159761592188e-20</v>
+        <v>8.922480328977489e-20</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1423,19 +1423,19 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-0.00048537153810864213</v>
+        <v>-0.00048440799540957796</v>
       </c>
       <c r="C45">
-        <v>-0.00047155327005715377</v>
+        <v>-0.0004708374462980982</v>
       </c>
       <c r="D45">
-        <v>-0.0004664576139397097</v>
+        <v>-0.00046578955991228996</v>
       </c>
       <c r="E45">
-        <v>-0.00046207282058258284</v>
+        <v>-0.000461458546531027</v>
       </c>
       <c r="F45">
-        <v>-0.00047093640945295893</v>
+        <v>-0.00047019489609798017</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1443,19 +1443,19 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-8.485739208970507e-5</v>
+        <v>-8.477988412594885e-5</v>
       </c>
       <c r="C46">
-        <v>-8.86543429255147e-5</v>
+        <v>-8.859281628432011e-5</v>
       </c>
       <c r="D46">
-        <v>-8.971123458695566e-5</v>
+        <v>-8.965724198303109e-5</v>
       </c>
       <c r="E46">
-        <v>-9.088784199941676e-5</v>
+        <v>-9.084239596753449e-5</v>
       </c>
       <c r="F46">
-        <v>-9.310421310054262e-5</v>
+        <v>-9.305465563245771e-5</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1463,19 +1463,19 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>2.0993320770248966e-6</v>
+        <v>7.877236809590782e-6</v>
       </c>
       <c r="C47">
-        <v>2.106139472085875e-6</v>
+        <v>7.903491312090182e-6</v>
       </c>
       <c r="D47">
-        <v>2.108555783440064e-6</v>
+        <v>7.916606733211724e-6</v>
       </c>
       <c r="E47">
-        <v>2.1106361979856894e-6</v>
+        <v>7.929570743402394e-6</v>
       </c>
       <c r="F47">
-        <v>2.1068380473971538e-6</v>
+        <v>7.920311578617106e-6</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1483,19 +1483,19 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>2.374521956174667e-6</v>
+        <v>9.900110659230514e-6</v>
       </c>
       <c r="C48">
-        <v>2.3739899784138335e-6</v>
+        <v>9.892543046976181e-6</v>
       </c>
       <c r="D48">
-        <v>2.3737793004399404e-6</v>
+        <v>9.887774846979489e-6</v>
       </c>
       <c r="E48">
-        <v>2.3732545600553326e-6</v>
+        <v>9.877221582804596e-6</v>
       </c>
       <c r="F48">
-        <v>2.370592455300252e-6</v>
+        <v>9.8369666787723e-6</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1503,19 +1503,19 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>1.906608213206597e-6</v>
+        <v>7.167144649691226e-6</v>
       </c>
       <c r="C49">
-        <v>1.9010682622889227e-6</v>
+        <v>7.141663629376297e-6</v>
       </c>
       <c r="D49">
-        <v>1.8990998655082748e-6</v>
+        <v>7.131605279617561e-6</v>
       </c>
       <c r="E49">
-        <v>1.8974041550411791e-6</v>
+        <v>7.120572681687092e-6</v>
       </c>
       <c r="F49">
-        <v>1.900499678040642e-6</v>
+        <v>7.130377261789335e-6</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1523,19 +1523,19 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>2.140784145672382e-6</v>
+        <v>8.897892261574474e-6</v>
       </c>
       <c r="C50">
-        <v>2.1412174339978615e-6</v>
+        <v>8.904198979781336e-6</v>
       </c>
       <c r="D50">
-        <v>2.1413887907442063e-6</v>
+        <v>8.908311026319314e-6</v>
       </c>
       <c r="E50">
-        <v>2.141815915988925e-6</v>
+        <v>8.917285645474704e-6</v>
       </c>
       <c r="F50">
-        <v>2.1439834845688995e-6</v>
+        <v>8.950953762173813e-6</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1543,16 +1543,16 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.011663737409459272</v>
+        <v>0.011663689012179963</v>
       </c>
       <c r="C51">
-        <v>0.011663737117471134</v>
+        <v>0.011663679788263947</v>
       </c>
       <c r="D51">
-        <v>0.011663741192975394</v>
+        <v>0.011663693611734584</v>
       </c>
       <c r="E51">
-        <v>0.011663749029831859</v>
+        <v>0.011663731364275882</v>
       </c>
       <c r="F51">
         <v>0.01166375</v>
@@ -1563,16 +1563,16 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.0058336273388629204</v>
+        <v>0.005833663902745664</v>
       </c>
       <c r="C52">
-        <v>0.005833628716253995</v>
+        <v>0.005833688977608943</v>
       </c>
       <c r="D52">
-        <v>0.005833629713125472</v>
+        <v>0.005833705194212184</v>
       </c>
       <c r="E52">
-        <v>0.005833629761888063</v>
+        <v>0.005833701938246927</v>
       </c>
       <c r="F52">
         <v>0.005833624999999999</v>

</xml_diff>

<commit_message>
all thanks to master optimizer @shishirstute my mpopf simulation seems to work appropriately now.
The cause was incorrect set `Nm1` being used for nodal real and reactive power balance equations, where instead of using all nodes except substation, I was using all nodes NOT connected to the substation. This caused garbage output for nodes connected to the substation: `1, 2, 10`
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -623,19 +623,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-4.30813814202642e-9</v>
+        <v>0.06332391581074477</v>
       </c>
       <c r="C5">
-        <v>-4.3081376419921005e-9</v>
+        <v>0.06355916260465252</v>
       </c>
       <c r="D5">
-        <v>-4.308137523078548e-9</v>
+        <v>0.06382514201487238</v>
       </c>
       <c r="E5">
-        <v>-4.3081371509771066e-9</v>
+        <v>0.06418211644711853</v>
       </c>
       <c r="F5">
-        <v>-9.090908574732907e-9</v>
+        <v>0.053771550193894437</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -643,19 +643,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.04267407439113609</v>
+        <v>0.044494579503654264</v>
       </c>
       <c r="C6">
-        <v>0.042894280744237914</v>
+        <v>0.04471003908686566</v>
       </c>
       <c r="D6">
-        <v>0.0430276985218409</v>
+        <v>0.04494275373159534</v>
       </c>
       <c r="E6">
-        <v>0.043101077761150575</v>
+        <v>0.04529312148249381</v>
       </c>
       <c r="F6">
-        <v>0.042260660261863925</v>
+        <v>0.03525584559914957</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -663,19 +663,19 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.05333160688517414</v>
+        <v>0.009997973752444302</v>
       </c>
       <c r="C7">
-        <v>-0.053288804082253866</v>
+        <v>0.010357918479412587</v>
       </c>
       <c r="D7">
-        <v>-0.05557683628089839</v>
+        <v>0.010491231652976257</v>
       </c>
       <c r="E7">
-        <v>-0.06525313270591816</v>
+        <v>0.010611213653251754</v>
       </c>
       <c r="F7">
-        <v>-0.030267369093617522</v>
+        <v>0.01042457504513188</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -683,19 +683,19 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.010657528185899915</v>
+        <v>0.008831362554646203</v>
       </c>
       <c r="C8">
-        <v>0.010394519029878308</v>
+        <v>0.008491205038374274</v>
       </c>
       <c r="D8">
-        <v>0.012549133450919972</v>
+        <v>0.008391156630300782</v>
       </c>
       <c r="E8">
-        <v>0.022152050636630435</v>
+        <v>0.008277781311372977</v>
       </c>
       <c r="F8">
-        <v>-0.011993300259154982</v>
+        <v>0.008091129549612984</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -703,19 +703,19 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.005000571413257865</v>
+        <v>0.00500057137543115</v>
       </c>
       <c r="C9">
-        <v>0.0051806039760923725</v>
+        <v>0.005180603940082182</v>
       </c>
       <c r="D9">
-        <v>0.0052472829146281595</v>
+        <v>0.005247282880301897</v>
       </c>
       <c r="E9">
-        <v>0.005307294056864217</v>
+        <v>0.0053072940254593505</v>
       </c>
       <c r="F9">
-        <v>0.0052139434288796084</v>
+        <v>0.005213943379754853</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -723,19 +723,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.009998580069983257</v>
+        <v>0.011369152118397572</v>
       </c>
       <c r="C10">
-        <v>0.01035856792971497</v>
+        <v>0.011584617583574184</v>
       </c>
       <c r="D10">
-        <v>0.010491901005877567</v>
+        <v>0.011728123964554063</v>
       </c>
       <c r="E10">
-        <v>0.010611904026549646</v>
+        <v>0.011945571284034685</v>
       </c>
       <c r="F10">
-        <v>0.010425251031502618</v>
+        <v>0.005758649387649733</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -743,19 +743,19 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.017670610425920653</v>
+        <v>0.018121249006797863</v>
       </c>
       <c r="C11">
-        <v>0.016990758226373782</v>
+        <v>0.01758111310566857</v>
       </c>
       <c r="D11">
-        <v>0.01679080757647534</v>
+        <v>0.017470218260015515</v>
       </c>
       <c r="E11">
-        <v>0.016564167637040973</v>
+        <v>0.01742298958043143</v>
       </c>
       <c r="F11">
-        <v>0.016190633876931777</v>
+        <v>0.013854953261631183</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -763,19 +763,19 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.005000668208106999</v>
+        <v>0.0050006681096306</v>
       </c>
       <c r="C12">
-        <v>0.005180707863493138</v>
+        <v>0.005180707773371025</v>
       </c>
       <c r="D12">
-        <v>0.005247389492650469</v>
+        <v>0.005247389408775227</v>
       </c>
       <c r="E12">
-        <v>0.005307403085157084</v>
+        <v>0.005307403011427218</v>
       </c>
       <c r="F12">
-        <v>0.0052140486499064305</v>
+        <v>0.005214048529859005</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -783,19 +783,19 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.005000630883271751</v>
+        <v>0.00500063079358504</v>
       </c>
       <c r="C13">
-        <v>0.005180667802562927</v>
+        <v>0.005180667720484873</v>
       </c>
       <c r="D13">
-        <v>0.005247348393776203</v>
+        <v>0.005247348317387458</v>
       </c>
       <c r="E13">
-        <v>0.005307361040862082</v>
+        <v>0.005307360973713176</v>
       </c>
       <c r="F13">
-        <v>0.005214008072518304</v>
+        <v>0.005214007963186004</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -803,19 +803,19 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.0050003093053147965</v>
+        <v>0.005000309291350155</v>
       </c>
       <c r="C14">
-        <v>0.005180322652479597</v>
+        <v>0.005180322639699659</v>
       </c>
       <c r="D14">
-        <v>0.005246994301581261</v>
+        <v>0.005246994289687175</v>
       </c>
       <c r="E14">
-        <v>0.005306998803677855</v>
+        <v>0.005306998793222455</v>
       </c>
       <c r="F14">
-        <v>0.005213658473036407</v>
+        <v>0.005213658456012855</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -823,19 +823,19 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.02397957211052107</v>
+        <v>0.012978671719861955</v>
       </c>
       <c r="C15">
-        <v>0.024520262607329243</v>
+        <v>0.014664902722496813</v>
       </c>
       <c r="D15">
-        <v>0.024690511467573107</v>
+        <v>0.015422012773512558</v>
       </c>
       <c r="E15">
-        <v>0.024811632614961734</v>
+        <v>0.01628853837341492</v>
       </c>
       <c r="F15">
-        <v>0.02441041081199054</v>
+        <v>0.015753518592662212</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -843,19 +843,19 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.18514854580690884</v>
+        <v>0.005001219967288982</v>
       </c>
       <c r="C16">
-        <v>0.18528930995297396</v>
+        <v>0.005181300067762836</v>
       </c>
       <c r="D16">
-        <v>0.18419856393761458</v>
+        <v>0.0052479970394988</v>
       </c>
       <c r="E16">
-        <v>0.1801950824656111</v>
+        <v>0.005308024609028374</v>
       </c>
       <c r="F16">
-        <v>-0.20338184217921984</v>
+        <v>0.005214648510507081</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -863,19 +863,19 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.19489585424575645</v>
+        <v>0.0026953431676274807</v>
       </c>
       <c r="C17">
-        <v>0.19503315331446322</v>
+        <v>0.003271018949616974</v>
       </c>
       <c r="D17">
-        <v>0.19466177812698635</v>
+        <v>0.003549848770650065</v>
       </c>
       <c r="E17">
-        <v>0.19345732332778878</v>
+        <v>0.003890148426135566</v>
       </c>
       <c r="F17">
-        <v>-0.20634294306688447</v>
+        <v>0.0036842932696121177</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -883,19 +883,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.0025000760121757044</v>
+        <v>0.0025000759738077485</v>
       </c>
       <c r="C18">
-        <v>0.0025900909121572874</v>
+        <v>0.0025900908756318476</v>
       </c>
       <c r="D18">
-        <v>0.002623429978589453</v>
+        <v>0.0026234299437720363</v>
       </c>
       <c r="E18">
-        <v>0.0026534352373280925</v>
+        <v>0.0026534352054738727</v>
       </c>
       <c r="F18">
-        <v>0.0026067604286568995</v>
+        <v>0.002606760378829247</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -903,19 +903,19 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.005485414961530933</v>
+        <v>0.001988491321734766</v>
       </c>
       <c r="C19">
-        <v>0.0056519068619503</v>
+        <v>0.0021559703211032205</v>
       </c>
       <c r="D19">
-        <v>0.005713549235630298</v>
+        <v>0.002218305446441517</v>
       </c>
       <c r="E19">
-        <v>0.005769239685276451</v>
+        <v>0.002274100888020736</v>
       </c>
       <c r="F19">
-        <v>0.005684609531719483</v>
+        <v>0.0021280208361198543</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -923,19 +923,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.01097989295530378</v>
+        <v>0.0034773596365156776</v>
       </c>
       <c r="C20">
-        <v>0.011083805500507771</v>
+        <v>0.004725704210333591</v>
       </c>
       <c r="D20">
-        <v>0.011092287501341285</v>
+        <v>0.005320216020576618</v>
       </c>
       <c r="E20">
-        <v>0.011067638298749816</v>
+        <v>0.006040594262941408</v>
       </c>
       <c r="F20">
-        <v>0.010891591649661435</v>
+        <v>0.0057964693147216535</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -943,19 +943,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.0025001738319323993</v>
+        <v>0.002500173732131745</v>
       </c>
       <c r="C21">
-        <v>0.002590195899554782</v>
+        <v>0.002590195808220757</v>
       </c>
       <c r="D21">
-        <v>0.002623537685094424</v>
+        <v>0.002623537600091275</v>
       </c>
       <c r="E21">
-        <v>0.002653545420043059</v>
+        <v>0.002653545345321716</v>
       </c>
       <c r="F21">
-        <v>0.0026068667637804775</v>
+        <v>0.002606866642118722</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -963,19 +963,19 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.0025001978573772525</v>
+        <v>0.0025001977519201273</v>
       </c>
       <c r="C22">
-        <v>0.002590221685966609</v>
+        <v>0.002590221589456038</v>
       </c>
       <c r="D22">
-        <v>0.0026235641395274552</v>
+        <v>0.002623564049706595</v>
       </c>
       <c r="E22">
-        <v>0.002653572482946556</v>
+        <v>0.0026535724039902574</v>
       </c>
       <c r="F22">
-        <v>0.0026068928825852804</v>
+        <v>0.002606892754028105</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -983,19 +983,19 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.002499871678145875</v>
+        <v>0.0024998716494942816</v>
       </c>
       <c r="C23">
-        <v>0.0025898715973288276</v>
+        <v>0.002589871571107919</v>
       </c>
       <c r="D23">
-        <v>0.002623204980830519</v>
+        <v>0.002623204956427134</v>
       </c>
       <c r="E23">
-        <v>0.0026532050627183566</v>
+        <v>0.0026532050412667596</v>
       </c>
       <c r="F23">
-        <v>0.002606538280885042</v>
+        <v>0.0026065382459574075</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1003,19 +1003,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.002258550464868548</v>
+        <v>0.002024662168522598</v>
       </c>
       <c r="C24">
-        <v>0.0023010295875199606</v>
+        <v>0.0020868091920567267</v>
       </c>
       <c r="D24">
-        <v>0.0023197321929759756</v>
+        <v>0.0021279751529137613</v>
       </c>
       <c r="E24">
-        <v>0.0023313410357977448</v>
+        <v>0.002183661074367119</v>
       </c>
       <c r="F24">
-        <v>0.002245104412455492</v>
+        <v>0.0014055498550281777</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1023,19 +1023,19 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.034993096112758186</v>
+        <v>0.00011779779462322102</v>
       </c>
       <c r="C25">
-        <v>0.03503794560576232</v>
+        <v>0.00012643260026237716</v>
       </c>
       <c r="D25">
-        <v>0.03489285229035758</v>
+        <v>0.00012970818599585172</v>
       </c>
       <c r="E25">
-        <v>0.03461982326703022</v>
+        <v>0.00013269203548402987</v>
       </c>
       <c r="F25">
-        <v>0.03985314874887429</v>
+        <v>0.00012806515596165523</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1043,19 +1043,19 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.03591092899623125</v>
+        <v>8.01271931734294e-5</v>
       </c>
       <c r="C26">
-        <v>0.03595617374290462</v>
+        <v>7.783592052828577e-5</v>
       </c>
       <c r="D26">
-        <v>0.03586635488843895</v>
+        <v>7.804415762771203e-5</v>
       </c>
       <c r="E26">
-        <v>0.035739820001720116</v>
+        <v>7.865648042758507e-5</v>
       </c>
       <c r="F26">
-        <v>0.04026879686539362</v>
+        <v>7.450178060733178e-5</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1063,19 +1063,19 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2.9477240337494127e-5</v>
+        <v>2.9473771198790548e-5</v>
       </c>
       <c r="C27">
-        <v>3.1638219447170265e-5</v>
+        <v>3.163491690433745e-5</v>
       </c>
       <c r="D27">
-        <v>3.245798453529442e-5</v>
+        <v>3.245483642782512e-5</v>
       </c>
       <c r="E27">
-        <v>3.3204719908694875e-5</v>
+        <v>3.32018397263991e-5</v>
       </c>
       <c r="F27">
-        <v>3.204659052801731e-5</v>
+        <v>3.204208523096305e-5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1083,19 +1083,19 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.00012265919940622017</v>
+        <v>0.00012554357077840337</v>
       </c>
       <c r="C28">
-        <v>0.00013132019027135063</v>
+        <v>0.00013090660220814636</v>
       </c>
       <c r="D28">
-        <v>0.00013460314228443745</v>
+        <v>0.00013432468139175897</v>
       </c>
       <c r="E28">
-        <v>0.00013759490122489384</v>
+        <v>0.00013938119969232358</v>
       </c>
       <c r="F28">
-        <v>0.00013297623962034557</v>
+        <v>3.554053815717879e-5</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1103,19 +1103,19 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.00040817636751258406</v>
+        <v>0.0003209791638092843</v>
       </c>
       <c r="C29">
-        <v>0.00038811801583059195</v>
+        <v>0.0003124925463587206</v>
       </c>
       <c r="D29">
-        <v>0.0003819261832578754</v>
+        <v>0.00031447082366101506</v>
       </c>
       <c r="E29">
-        <v>0.0003742823131069778</v>
+        <v>0.0003206462652343732</v>
       </c>
       <c r="F29">
-        <v>0.00035909421012304837</v>
+        <v>0.0002126923455470125</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1123,19 +1123,19 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>2.94925839774373e-5</v>
+        <v>2.9485639292648346e-5</v>
       </c>
       <c r="C30">
-        <v>3.165444199722731e-5</v>
+        <v>3.164808646761617e-5</v>
       </c>
       <c r="D30">
-        <v>3.247454541806554e-5</v>
+        <v>3.2468630426003706e-5</v>
       </c>
       <c r="E30">
-        <v>3.32215428713223e-5</v>
+        <v>3.3216343344529106e-5</v>
       </c>
       <c r="F30">
-        <v>3.206250744860781e-5</v>
+        <v>3.205404154674865e-5</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1143,19 +1143,19 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>2.9492345111550528e-5</v>
+        <v>2.948540053924244e-5</v>
       </c>
       <c r="C31">
-        <v>3.16541763908656e-5</v>
+        <v>3.164782096790132e-5</v>
       </c>
       <c r="D31">
-        <v>3.24742694227237e-5</v>
+        <v>3.2468354531195046e-5</v>
       </c>
       <c r="E31">
-        <v>3.3221257298421744e-5</v>
+        <v>3.321605786101328e-5</v>
       </c>
       <c r="F31">
-        <v>3.206223669237753e-5</v>
+        <v>3.205377093348442e-5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1163,19 +1163,19 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>2.9492345111550528e-5</v>
+        <v>2.9485400539242442e-5</v>
       </c>
       <c r="C32">
-        <v>3.16541763908656e-5</v>
+        <v>3.1647820967901323e-5</v>
       </c>
       <c r="D32">
-        <v>3.24742694227237e-5</v>
+        <v>3.246835453119505e-5</v>
       </c>
       <c r="E32">
-        <v>3.322125729842175e-5</v>
+        <v>3.321605786101327e-5</v>
       </c>
       <c r="F32">
-        <v>3.206223669237752e-5</v>
+        <v>3.205377093348443e-5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1203,19 +1203,19 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1.060346700297827</v>
+        <v>1.060471486463274</v>
       </c>
       <c r="C34">
-        <v>1.0603387003608413</v>
+        <v>1.0604493771525947</v>
       </c>
       <c r="D34">
-        <v>1.060335795073358</v>
+        <v>1.0604386305180635</v>
       </c>
       <c r="E34">
-        <v>1.0603338580037491</v>
+        <v>1.0604258243415199</v>
       </c>
       <c r="F34">
-        <v>1.0603438759658415</v>
+        <v>1.0604929421723979</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1223,19 +1223,19 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1.0582828207010737</v>
+        <v>1.0607372295225344</v>
       </c>
       <c r="C35">
-        <v>1.0582801620312687</v>
+        <v>1.060731369416348</v>
       </c>
       <c r="D35">
-        <v>1.058316516381771</v>
+        <v>1.0607291990001404</v>
       </c>
       <c r="E35">
-        <v>1.0584602553159828</v>
+        <v>1.0607272456225454</v>
       </c>
       <c r="F35">
-        <v>1.0644961639565997</v>
+        <v>1.0607302842086839</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1243,19 +1243,19 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1.0601823565297992</v>
+        <v>1.0603071426960828</v>
       </c>
       <c r="C36">
-        <v>1.0601684399518805</v>
+        <v>1.0602791167444305</v>
       </c>
       <c r="D36">
-        <v>1.0601633433112234</v>
+        <v>1.060266178756688</v>
       </c>
       <c r="E36">
-        <v>1.0601594340216</v>
+        <v>1.0602514003600656</v>
       </c>
       <c r="F36">
-        <v>1.0601725198806582</v>
+        <v>1.0603215860883013</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1263,19 +1263,19 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1.0602186842782253</v>
+        <v>1.060378363542893</v>
       </c>
       <c r="C37">
-        <v>1.0602064581406496</v>
+        <v>1.0603528875405295</v>
       </c>
       <c r="D37">
-        <v>1.0602019878344746</v>
+        <v>1.0603405059717077</v>
       </c>
       <c r="E37">
-        <v>1.0601986396096783</v>
+        <v>1.0603256995976507</v>
       </c>
       <c r="F37">
-        <v>1.0602108279146962</v>
+        <v>1.0604319388490702</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1283,19 +1283,19 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>1.0598444592499354</v>
+        <v>1.0600940315335743</v>
       </c>
       <c r="C38">
-        <v>1.0598464748760148</v>
+        <v>1.0600592674234022</v>
       </c>
       <c r="D38">
-        <v>1.0598469056179907</v>
+        <v>1.0600399429619058</v>
       </c>
       <c r="E38">
-        <v>1.0598493556107205</v>
+        <v>1.0600152237791725</v>
       </c>
       <c r="F38">
-        <v>1.0598689981487588</v>
+        <v>1.0601488649084456</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1303,19 +1303,19 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1.0596307922326127</v>
+        <v>1.059880364519082</v>
       </c>
       <c r="C39">
-        <v>1.0596251153976626</v>
+        <v>1.0598379079476403</v>
       </c>
       <c r="D39">
-        <v>1.0596226970720841</v>
+        <v>1.0598157344184105</v>
       </c>
       <c r="E39">
-        <v>1.059622582900386</v>
+        <v>1.0597884510709572</v>
       </c>
       <c r="F39">
-        <v>1.059646214137439</v>
+        <v>1.0599260809005766</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1323,19 +1323,19 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>1.05968011149349</v>
+        <v>1.0599296837797423</v>
       </c>
       <c r="C40">
-        <v>1.0596762101863413</v>
+        <v>1.05988900273612</v>
       </c>
       <c r="D40">
-        <v>1.0596744494642596</v>
+        <v>1.0598674868104008</v>
       </c>
       <c r="E40">
-        <v>1.0596749271359869</v>
+        <v>1.0598407953063955</v>
       </c>
       <c r="F40">
-        <v>1.0596976377278038</v>
+        <v>1.0599775044906765</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1343,19 +1343,19 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1.0596393744476884</v>
+        <v>1.0598889467340868</v>
       </c>
       <c r="C41">
-        <v>1.0596340065837166</v>
+        <v>1.0598467991336291</v>
       </c>
       <c r="D41">
-        <v>1.059631702692032</v>
+        <v>1.0598247400382979</v>
       </c>
       <c r="E41">
-        <v>1.0596316915109292</v>
+        <v>1.0597975596814475</v>
       </c>
       <c r="F41">
-        <v>1.0596551625404196</v>
+        <v>1.0599350293034706</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1363,19 +1363,19 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>1.057720892318825</v>
+        <v>1.0607232105806008</v>
       </c>
       <c r="C42">
-        <v>1.0577227911701494</v>
+        <v>1.060719489586395</v>
       </c>
       <c r="D42">
-        <v>1.0576955928437255</v>
+        <v>1.0607166981199432</v>
       </c>
       <c r="E42">
-        <v>1.0575674196332712</v>
+        <v>1.0607131578303646</v>
       </c>
       <c r="F42">
-        <v>1.0642859594585514</v>
+        <v>1.0607192014172477</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1383,19 +1383,19 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-0.0008908827352805736</v>
+        <v>0.005036026207556386</v>
       </c>
       <c r="C43">
-        <v>-0.0006311047860027225</v>
+        <v>0.004132669373122418</v>
       </c>
       <c r="D43">
-        <v>-0.0005052228634117533</v>
+        <v>0.003666872680988475</v>
       </c>
       <c r="E43">
-        <v>-0.00035943700716228546</v>
+        <v>0.0030622165506399724</v>
       </c>
       <c r="F43">
-        <v>-0.00036800863153772095</v>
+        <v>0.003089824594449595</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1403,19 +1403,19 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>1.438684068520384e-19</v>
+        <v>0.0023055277210955417</v>
       </c>
       <c r="C44">
-        <v>-1.0963699529388172e-19</v>
+        <v>0.0019098431845174946</v>
       </c>
       <c r="D44">
-        <v>1.497565535865285e-19</v>
+        <v>0.0016976849770697743</v>
       </c>
       <c r="E44">
-        <v>8.922480328977489e-20</v>
+        <v>0.0014173930663445257</v>
       </c>
       <c r="F44">
-        <v>8.922480328977489e-20</v>
+        <v>0.0015298780289751922</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1423,19 +1423,19 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-0.00048440799540957796</v>
+        <v>0.003012533444693624</v>
       </c>
       <c r="C45">
-        <v>-0.0004708374462980982</v>
+        <v>0.0030250965421749765</v>
       </c>
       <c r="D45">
-        <v>-0.00046578955991228996</v>
+        <v>0.003029452510812138</v>
       </c>
       <c r="E45">
-        <v>-0.000461458546531027</v>
+        <v>0.00303369127449974</v>
       </c>
       <c r="F45">
-        <v>-0.00047019489609798017</v>
+        <v>0.003085792495030601</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1443,19 +1443,19 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-8.477988412594885e-5</v>
+        <v>0.0014900733847792735</v>
       </c>
       <c r="C46">
-        <v>-8.859281628432011e-5</v>
+        <v>0.0015050655296811194</v>
       </c>
       <c r="D46">
-        <v>-8.965724198303109e-5</v>
+        <v>0.0015097221534455907</v>
       </c>
       <c r="E46">
-        <v>-9.084239596753449e-5</v>
+        <v>0.0015140737374069323</v>
       </c>
       <c r="F46">
-        <v>-9.305465563245771e-5</v>
+        <v>0.00154293987880631</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1463,19 +1463,19 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>7.877236809590782e-6</v>
+        <v>0.0013713150393736503</v>
       </c>
       <c r="C47">
-        <v>7.903491312090182e-6</v>
+        <v>0.0012268543288419804</v>
       </c>
       <c r="D47">
-        <v>7.916606733211724e-6</v>
+        <v>0.0012370504002260617</v>
       </c>
       <c r="E47">
-        <v>7.929570743402394e-6</v>
+        <v>0.0013345124680544814</v>
       </c>
       <c r="F47">
-        <v>7.920311578617106e-6</v>
+        <v>-8.918345262159885e-9</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1483,19 +1483,19 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>9.900110659230514e-6</v>
+        <v>0.0004524429015939975</v>
       </c>
       <c r="C48">
-        <v>9.892543046976181e-6</v>
+        <v>0.000592044405570547</v>
       </c>
       <c r="D48">
-        <v>9.887774846979489e-6</v>
+        <v>0.0006810200770422861</v>
       </c>
       <c r="E48">
-        <v>9.877221582804596e-6</v>
+        <v>0.0008602912905415712</v>
       </c>
       <c r="F48">
-        <v>9.8369666787723e-6</v>
+        <v>-8.918550613658096e-9</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1503,19 +1503,19 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>7.167144649691226e-6</v>
+        <v>4.159894950410076e-8</v>
       </c>
       <c r="C49">
-        <v>7.141663629376297e-6</v>
+        <v>4.1599791410278856e-8</v>
       </c>
       <c r="D49">
-        <v>7.131605279617561e-6</v>
+        <v>4.160017238244907e-8</v>
       </c>
       <c r="E49">
-        <v>7.120572681687092e-6</v>
+        <v>4.16005326142097e-8</v>
       </c>
       <c r="F49">
-        <v>7.130377261789335e-6</v>
+        <v>0.004665508895185284</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1523,19 +1523,19 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>8.897892261574474e-6</v>
+        <v>4.159337281592296e-8</v>
       </c>
       <c r="C50">
-        <v>8.904198979781336e-6</v>
+        <v>4.1589594244711796e-8</v>
       </c>
       <c r="D50">
-        <v>8.908311026319314e-6</v>
+        <v>4.158872287967354e-8</v>
       </c>
       <c r="E50">
-        <v>8.917285645474704e-6</v>
+        <v>4.158788425774589e-8</v>
       </c>
       <c r="F50">
-        <v>8.950953762173813e-6</v>
+        <v>0.0023335088953943058</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1543,16 +1543,16 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.011663689012179963</v>
+        <v>0.012966455499037069</v>
       </c>
       <c r="C51">
-        <v>0.011663679788263947</v>
+        <v>0.014131923322182834</v>
       </c>
       <c r="D51">
-        <v>0.011663693611734584</v>
+        <v>0.015307077412742452</v>
       </c>
       <c r="E51">
-        <v>0.011663731364275882</v>
+        <v>0.016574820467359877</v>
       </c>
       <c r="F51">
         <v>0.01166375</v>
@@ -1563,16 +1563,16 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.005833663902745664</v>
+        <v>0.006263401974016596</v>
       </c>
       <c r="C52">
-        <v>0.005833688977608943</v>
+        <v>0.006825800380788358</v>
       </c>
       <c r="D52">
-        <v>0.005833705194212184</v>
+        <v>0.0074727256763754985</v>
       </c>
       <c r="E52">
-        <v>0.005833701938246927</v>
+        <v>0.00828995862566972</v>
       </c>
       <c r="F52">
         <v>0.005833624999999999</v>

</xml_diff>

<commit_message>
alpha = 1e-3 works again
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -851,76 +851,76 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.061731155791079025</v>
+        <v>0.06173114629133221</v>
       </c>
       <c r="C5">
-        <v>0.05729243497826494</v>
+        <v>0.0572924580189984</v>
       </c>
       <c r="D5">
-        <v>0.05427422584223315</v>
+        <v>0.05427437097296479</v>
       </c>
       <c r="E5">
-        <v>0.052936412038886646</v>
+        <v>0.05293621220309018</v>
       </c>
       <c r="F5">
-        <v>0.05319565852686628</v>
+        <v>0.053195715829821244</v>
       </c>
       <c r="G5">
-        <v>0.05405644160446478</v>
+        <v>0.05405661479838581</v>
       </c>
       <c r="H5">
-        <v>0.05570597584622493</v>
+        <v>0.055706056954738334</v>
       </c>
       <c r="I5">
-        <v>0.056979607687953064</v>
+        <v>0.05697964266758312</v>
       </c>
       <c r="J5">
-        <v>0.059345971184420254</v>
+        <v>0.05934596275255661</v>
       </c>
       <c r="K5">
-        <v>0.06177023363018112</v>
+        <v>0.061770210615367555</v>
       </c>
       <c r="L5">
-        <v>0.06204074440725385</v>
+        <v>0.06204071841054558</v>
       </c>
       <c r="M5">
-        <v>0.062242258136402426</v>
+        <v>0.06224222716344458</v>
       </c>
       <c r="N5">
-        <v>0.06238132333364854</v>
+        <v>0.062381283999564545</v>
       </c>
       <c r="O5">
-        <v>0.061412306717820754</v>
+        <v>0.061412239842530233</v>
       </c>
       <c r="P5">
-        <v>0.061939575781234234</v>
+        <v>0.06193946841493923</v>
       </c>
       <c r="Q5">
-        <v>0.0620195406066346</v>
+        <v>0.062019541464420534</v>
       </c>
       <c r="R5">
-        <v>0.06662726323375492</v>
+        <v>0.06662726716583452</v>
       </c>
       <c r="S5">
-        <v>0.07117864207112241</v>
+        <v>0.07117868709503243</v>
       </c>
       <c r="T5">
-        <v>0.07813608891967869</v>
+        <v>0.07813610371844927</v>
       </c>
       <c r="U5">
-        <v>0.08056137639923637</v>
+        <v>0.08056131707549531</v>
       </c>
       <c r="V5">
-        <v>0.0791752468385564</v>
+        <v>0.07917522417173717</v>
       </c>
       <c r="W5">
-        <v>0.07728281633700163</v>
+        <v>0.07728283375464502</v>
       </c>
       <c r="X5">
-        <v>0.07669496222574808</v>
+        <v>0.07669483002782823</v>
       </c>
       <c r="Y5">
-        <v>0.0689559184608287</v>
+        <v>0.06895605111911352</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -928,76 +928,76 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.0428014530590445</v>
+        <v>0.042801443560451874</v>
       </c>
       <c r="C6">
-        <v>0.03977587504531995</v>
+        <v>0.03977589808733105</v>
       </c>
       <c r="D6">
-        <v>0.03779751698394873</v>
+        <v>0.037797662115997346</v>
       </c>
       <c r="E6">
-        <v>0.0371529331386663</v>
+        <v>0.03715273330417834</v>
       </c>
       <c r="F6">
-        <v>0.03725220377226271</v>
+        <v>0.03725226107653093</v>
       </c>
       <c r="G6">
-        <v>0.03771304645342734</v>
+        <v>0.03771321964849193</v>
       </c>
       <c r="H6">
-        <v>0.03876941202890394</v>
+        <v>0.03876949313869838</v>
       </c>
       <c r="I6">
-        <v>0.03963651247814095</v>
+        <v>0.039636547458981444</v>
       </c>
       <c r="J6">
-        <v>0.04124972320892733</v>
+        <v>0.04124971477813585</v>
       </c>
       <c r="K6">
-        <v>0.04294089878058106</v>
+        <v>0.04294087576657016</v>
       </c>
       <c r="L6">
-        <v>0.043191621815563117</v>
+        <v>0.04319159581930361</v>
       </c>
       <c r="M6">
-        <v>0.04335987046069437</v>
+        <v>0.0433598394880687</v>
       </c>
       <c r="N6">
-        <v>0.04349232852404649</v>
+        <v>0.04349228919019694</v>
       </c>
       <c r="O6">
-        <v>0.04289659752970329</v>
+        <v>0.04289653065466126</v>
       </c>
       <c r="P6">
-        <v>0.04337386745646708</v>
+        <v>0.043373760090427475</v>
       </c>
       <c r="Q6">
-        <v>0.04308383105762742</v>
+        <v>0.04308383191541627</v>
       </c>
       <c r="R6">
-        <v>0.04623826864216082</v>
+        <v>0.04623827257424411</v>
       </c>
       <c r="S6">
-        <v>0.04931626883578449</v>
+        <v>0.049316313859699375</v>
       </c>
       <c r="T6">
-        <v>0.05304047375242899</v>
+        <v>0.053040488551201796</v>
       </c>
       <c r="U6">
-        <v>0.05389914472037901</v>
+        <v>0.05389908539663932</v>
       </c>
       <c r="V6">
-        <v>0.053312951506135416</v>
+        <v>0.05331292883931805</v>
       </c>
       <c r="W6">
-        <v>0.05272707424113511</v>
+        <v>0.0527270916587816</v>
       </c>
       <c r="X6">
-        <v>0.05403236353379804</v>
+        <v>0.05403223133659517</v>
       </c>
       <c r="Y6">
-        <v>0.04975958347715475</v>
+        <v>0.04975971613656475</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1082,76 +1082,76 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.0094649781690966</v>
+        <v>0.00946497816794242</v>
       </c>
       <c r="C8">
-        <v>0.008758386393607025</v>
+        <v>0.008758386392329386</v>
       </c>
       <c r="D8">
-        <v>0.008238447200432328</v>
+        <v>0.008238447199115352</v>
       </c>
       <c r="E8">
-        <v>0.007891823739670617</v>
+        <v>0.007891823738362107</v>
       </c>
       <c r="F8">
-        <v>0.007971813580380826</v>
+        <v>0.007971813579067568</v>
       </c>
       <c r="G8">
-        <v>0.00817178867727363</v>
+        <v>0.008171788676130068</v>
       </c>
       <c r="H8">
-        <v>0.008351694523218996</v>
+        <v>0.008351694521937954</v>
       </c>
       <c r="I8">
-        <v>0.008438279394409678</v>
+        <v>0.008438279393199239</v>
       </c>
       <c r="J8">
-        <v>0.008698179371687452</v>
+        <v>0.008698179370615294</v>
       </c>
       <c r="K8">
-        <v>0.008831361097155757</v>
+        <v>0.008831361096353097</v>
       </c>
       <c r="L8">
-        <v>0.008491204112278144</v>
+        <v>0.00849120411182938</v>
       </c>
       <c r="M8">
-        <v>0.008391156022731796</v>
+        <v>0.008391156022399624</v>
       </c>
       <c r="N8">
-        <v>0.008277781156350302</v>
+        <v>0.008277781156115847</v>
       </c>
       <c r="O8">
-        <v>0.008091134142985585</v>
+        <v>0.008091134142737093</v>
       </c>
       <c r="P8">
-        <v>0.008127801961436412</v>
+        <v>0.008127801961181012</v>
       </c>
       <c r="Q8">
-        <v>0.008417815241098126</v>
+        <v>0.008417815241095212</v>
       </c>
       <c r="R8">
-        <v>0.009377839951684407</v>
+        <v>0.009377839951680704</v>
       </c>
       <c r="S8">
-        <v>0.010464607533433246</v>
+        <v>0.010464607533428377</v>
       </c>
       <c r="T8">
-        <v>0.01243135502666498</v>
+        <v>0.012431355026662759</v>
       </c>
       <c r="U8">
-        <v>0.013331389409204036</v>
+        <v>0.013331389409202664</v>
       </c>
       <c r="V8">
-        <v>0.012931402845769184</v>
+        <v>0.012931402845767334</v>
       </c>
       <c r="W8">
-        <v>0.01227809765976293</v>
+        <v>0.012278097659759834</v>
       </c>
       <c r="X8">
-        <v>0.011331490170803687</v>
+        <v>0.011331490170086706</v>
       </c>
       <c r="Y8">
-        <v>0.009598298376101344</v>
+        <v>0.009598298374976165</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1159,76 +1159,76 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.004733857998613808</v>
+        <v>0.004733857998613734</v>
       </c>
       <c r="C9">
-        <v>0.004380465595063716</v>
+        <v>0.004380465595063637</v>
       </c>
       <c r="D9">
-        <v>0.00412042418079558</v>
+        <v>0.0041204241807955835</v>
       </c>
       <c r="E9">
-        <v>0.003947064205190556</v>
+        <v>0.0039470642051900925</v>
       </c>
       <c r="F9">
-        <v>0.003987070284739588</v>
+        <v>0.003987070284739433</v>
       </c>
       <c r="G9">
-        <v>0.004087085663962383</v>
+        <v>0.004087085663962407</v>
       </c>
       <c r="H9">
-        <v>0.004293784929921202</v>
+        <v>0.004293784929921183</v>
       </c>
       <c r="I9">
-        <v>0.004453810923105984</v>
+        <v>0.004453810923105943</v>
       </c>
       <c r="J9">
-        <v>0.004700518953860356</v>
+        <v>0.004700518953860288</v>
       </c>
       <c r="K9">
-        <v>0.0050005713724417195</v>
+        <v>0.005000571372441652</v>
       </c>
       <c r="L9">
-        <v>0.005180603937008272</v>
+        <v>0.00518060393700821</v>
       </c>
       <c r="M9">
-        <v>0.005247282877036797</v>
+        <v>0.005247282877036728</v>
       </c>
       <c r="N9">
-        <v>0.005307294021685612</v>
+        <v>0.005307294021685526</v>
       </c>
       <c r="O9">
-        <v>0.005213943395349135</v>
+        <v>0.005213943395348996</v>
       </c>
       <c r="P9">
-        <v>0.0052206112903810924</v>
+        <v>0.005220611290380872</v>
       </c>
       <c r="Q9">
-        <v>0.00526061867734947</v>
+        <v>0.0052606186773494715</v>
       </c>
       <c r="R9">
-        <v>0.005507331829556263</v>
+        <v>0.0055073318295562725</v>
       </c>
       <c r="S9">
-        <v>0.005700702693597541</v>
+        <v>0.005700702693597648</v>
       </c>
       <c r="T9">
-        <v>0.006334165707464373</v>
+        <v>0.006334165707464417</v>
       </c>
       <c r="U9">
-        <v>0.006667571439556789</v>
+        <v>0.006667571439556595</v>
       </c>
       <c r="V9">
-        <v>0.006467527656719374</v>
+        <v>0.006467527656719305</v>
       </c>
       <c r="W9">
-        <v>0.0061407916939465075</v>
+        <v>0.006140791693946556</v>
       </c>
       <c r="X9">
-        <v>0.00566736283149592</v>
+        <v>0.005667362831495597</v>
       </c>
       <c r="Y9">
-        <v>0.0048005361817412455</v>
+        <v>0.004800536181741414</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1236,76 +1236,76 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.009594347083501705</v>
+        <v>0.009594357663375656</v>
       </c>
       <c r="C10">
-        <v>0.008996241625198973</v>
+        <v>0.008996286661527035</v>
       </c>
       <c r="D10">
-        <v>0.008747137947338106</v>
+        <v>0.008747280970884284</v>
       </c>
       <c r="E10">
-        <v>0.009156257780388283</v>
+        <v>0.009155933770505099</v>
       </c>
       <c r="F10">
-        <v>0.009013819848550911</v>
+        <v>0.009013798834025439</v>
       </c>
       <c r="G10">
-        <v>0.008855293282347063</v>
+        <v>0.008855442696598565</v>
       </c>
       <c r="H10">
-        <v>0.008989597656786039</v>
+        <v>0.00898967775354143</v>
       </c>
       <c r="I10">
-        <v>0.009223712888577894</v>
+        <v>0.009223753030530968</v>
       </c>
       <c r="J10">
-        <v>0.009617922067986947</v>
+        <v>0.009617928537382501</v>
       </c>
       <c r="K10">
-        <v>0.010161575144435546</v>
+        <v>0.010161569894650538</v>
       </c>
       <c r="L10">
-        <v>0.010523489450265102</v>
+        <v>0.010523480313139513</v>
       </c>
       <c r="M10">
-        <v>0.010670778387854277</v>
+        <v>0.010670763898993851</v>
       </c>
       <c r="N10">
-        <v>0.01081459877811948</v>
+        <v>0.010814573722841773</v>
       </c>
       <c r="O10">
-        <v>0.01074372744554255</v>
+        <v>0.010743672538856797</v>
       </c>
       <c r="P10">
-        <v>0.010978540785405399</v>
+        <v>0.010978521623073683</v>
       </c>
       <c r="Q10">
-        <v>0.010472452159001682</v>
+        <v>0.010472452962352136</v>
       </c>
       <c r="R10">
-        <v>0.010963558531569875</v>
+        <v>0.01096356239448917</v>
       </c>
       <c r="S10">
-        <v>0.011292199924767831</v>
+        <v>0.011292244719964172</v>
       </c>
       <c r="T10">
-        <v>0.010121454630711</v>
+        <v>0.010121448489469284</v>
       </c>
       <c r="U10">
-        <v>0.009472217018930085</v>
+        <v>0.009472186158058648</v>
       </c>
       <c r="V10">
-        <v>0.009914247048019945</v>
+        <v>0.009914262326124119</v>
       </c>
       <c r="W10">
-        <v>0.010368022022235097</v>
+        <v>0.010367994305393282</v>
       </c>
       <c r="X10">
-        <v>0.013392722769334326</v>
+        <v>0.013392605141400893</v>
       </c>
       <c r="Y10">
-        <v>0.013920853784304717</v>
+        <v>0.013920971644932337</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1313,76 +1313,76 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.01900337883868342</v>
+        <v>0.019003358763453247</v>
       </c>
       <c r="C11">
-        <v>0.017636591451548837</v>
+        <v>0.017636569453845334</v>
       </c>
       <c r="D11">
-        <v>0.016687743389957432</v>
+        <v>0.01668774547006055</v>
       </c>
       <c r="E11">
-        <v>0.016154153696164714</v>
+        <v>0.016154277913820216</v>
       </c>
       <c r="F11">
-        <v>0.01627584648315796</v>
+        <v>0.016275924791880954</v>
       </c>
       <c r="G11">
-        <v>0.01659513122794062</v>
+        <v>0.016595154974473503</v>
       </c>
       <c r="H11">
-        <v>0.016896987253782567</v>
+        <v>0.01689698825103955</v>
       </c>
       <c r="I11">
-        <v>0.017049791513033145</v>
+        <v>0.017049786345542276</v>
       </c>
       <c r="J11">
-        <v>0.017528432308766828</v>
+        <v>0.017528417411393528</v>
       </c>
       <c r="K11">
-        <v>0.01777553384117394</v>
+        <v>0.017775516082876183</v>
       </c>
       <c r="L11">
-        <v>0.017124205104432487</v>
+        <v>0.01712418825174035</v>
       </c>
       <c r="M11">
-        <v>0.01694507943689391</v>
+        <v>0.01694506296072802</v>
       </c>
       <c r="N11">
-        <v>0.01675362492532631</v>
+        <v>0.016753610656320042</v>
       </c>
       <c r="O11">
-        <v>0.01650892035886614</v>
+        <v>0.016508908406540488</v>
       </c>
       <c r="P11">
-        <v>0.016731265770958133</v>
+        <v>0.01673117759331875</v>
       </c>
       <c r="Q11">
-        <v>0.016827441874359972</v>
+        <v>0.016827441928582803</v>
       </c>
       <c r="R11">
-        <v>0.01875002521623441</v>
+        <v>0.018750025284345762</v>
       </c>
       <c r="S11">
-        <v>0.020918594307114968</v>
+        <v>0.020918594523088863</v>
       </c>
       <c r="T11">
-        <v>0.023912400465399913</v>
+        <v>0.02391242140094724</v>
       </c>
       <c r="U11">
-        <v>0.024419981820803825</v>
+        <v>0.024419953375940565</v>
       </c>
       <c r="V11">
-        <v>0.023991980053788057</v>
+        <v>0.023991942115673442</v>
       </c>
       <c r="W11">
-        <v>0.023932562187210012</v>
+        <v>0.023932607316467288</v>
       </c>
       <c r="X11">
-        <v>0.023632802304972604</v>
+        <v>0.023632787775337945</v>
       </c>
       <c r="Y11">
-        <v>0.021433174050625375</v>
+        <v>0.0214331888115743</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1390,76 +1390,76 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.004733944684352269</v>
+        <v>0.004733944684351967</v>
       </c>
       <c r="C12">
-        <v>0.004380539806695971</v>
+        <v>0.004380539806695589</v>
       </c>
       <c r="D12">
-        <v>0.004120489833860221</v>
+        <v>0.004120489833859971</v>
       </c>
       <c r="E12">
-        <v>0.003947124445115764</v>
+        <v>0.003947124445115338</v>
       </c>
       <c r="F12">
-        <v>0.003987131753113812</v>
+        <v>0.00398713175311362</v>
       </c>
       <c r="G12">
-        <v>0.004087150257974141</v>
+        <v>0.004087150257974001</v>
       </c>
       <c r="H12">
-        <v>0.004293856228126987</v>
+        <v>0.004293856228126779</v>
       </c>
       <c r="I12">
-        <v>0.004453887639239105</v>
+        <v>0.004453887639238891</v>
       </c>
       <c r="J12">
-        <v>0.004700604413744758</v>
+        <v>0.004700604413744504</v>
       </c>
       <c r="K12">
-        <v>0.005000668103194669</v>
+        <v>0.005000668103194427</v>
       </c>
       <c r="L12">
-        <v>0.005180707765902317</v>
+        <v>0.0051807077659021</v>
       </c>
       <c r="M12">
-        <v>0.0052473894004732196</v>
+        <v>0.005247389400472997</v>
       </c>
       <c r="N12">
-        <v>0.005307403001270388</v>
+        <v>0.005307403001270161</v>
       </c>
       <c r="O12">
-        <v>0.005214048570390699</v>
+        <v>0.005214048570390423</v>
       </c>
       <c r="P12">
-        <v>0.00522071673611944</v>
+        <v>0.005220716736118486</v>
       </c>
       <c r="Q12">
-        <v>0.005260725741660261</v>
+        <v>0.0052607257416602635</v>
       </c>
       <c r="R12">
-        <v>0.005507449188452209</v>
+        <v>0.005507449188452221</v>
       </c>
       <c r="S12">
-        <v>0.0057008284582724155</v>
+        <v>0.005700828458272557</v>
       </c>
       <c r="T12">
-        <v>0.006334321031282821</v>
+        <v>0.006334321031283109</v>
       </c>
       <c r="U12">
-        <v>0.006667743565651424</v>
+        <v>0.006667743565650826</v>
       </c>
       <c r="V12">
-        <v>0.006467689596016302</v>
+        <v>0.006467689596015775</v>
       </c>
       <c r="W12">
-        <v>0.006140937671729384</v>
+        <v>0.006140937671729916</v>
       </c>
       <c r="X12">
-        <v>0.005667487153135641</v>
+        <v>0.005667487153135075</v>
       </c>
       <c r="Y12">
-        <v>0.004800625347031247</v>
+        <v>0.004800625347031485</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1467,76 +1467,76 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.0047339112441354666</v>
+        <v>0.004733911244135191</v>
       </c>
       <c r="C13">
-        <v>0.004380511175175346</v>
+        <v>0.004380511175174999</v>
       </c>
       <c r="D13">
-        <v>0.004120464502219148</v>
+        <v>0.004120464502218921</v>
       </c>
       <c r="E13">
-        <v>0.003947101200943006</v>
+        <v>0.0039471012009426164</v>
       </c>
       <c r="F13">
-        <v>0.003987108035197828</v>
+        <v>0.003987108035197653</v>
       </c>
       <c r="G13">
-        <v>0.004087125334736079</v>
+        <v>0.004087125334735951</v>
       </c>
       <c r="H13">
-        <v>0.004293828719264392</v>
+        <v>0.004293828719264202</v>
       </c>
       <c r="I13">
-        <v>0.0044538580408942435</v>
+        <v>0.004453858040894048</v>
       </c>
       <c r="J13">
-        <v>0.004700571443942833</v>
+        <v>0.0047005714439426</v>
       </c>
       <c r="K13">
-        <v>0.00500063078772356</v>
+        <v>0.005000630787723339</v>
       </c>
       <c r="L13">
-        <v>0.005180667713682803</v>
+        <v>0.005180667713682605</v>
       </c>
       <c r="M13">
-        <v>0.005247348309826468</v>
+        <v>0.005247348309826264</v>
       </c>
       <c r="N13">
-        <v>0.005307360964462921</v>
+        <v>0.005307360964462714</v>
       </c>
       <c r="O13">
-        <v>0.005214008000099942</v>
+        <v>0.00521400800009969</v>
       </c>
       <c r="P13">
-        <v>0.005220676061783192</v>
+        <v>0.005220676061782324</v>
       </c>
       <c r="Q13">
-        <v>0.005260684442053964</v>
+        <v>0.005260684442053966</v>
       </c>
       <c r="R13">
-        <v>0.005507403921793306</v>
+        <v>0.005507403921793317</v>
       </c>
       <c r="S13">
-        <v>0.005700779954370407</v>
+        <v>0.005700779954370535</v>
       </c>
       <c r="T13">
-        <v>0.006334261140802833</v>
+        <v>0.006334261140803094</v>
       </c>
       <c r="U13">
-        <v>0.006667677201011552</v>
+        <v>0.006667677201011006</v>
       </c>
       <c r="V13">
-        <v>0.0064676271559561665</v>
+        <v>0.006467627155955686</v>
       </c>
       <c r="W13">
-        <v>0.006140881383576005</v>
+        <v>0.006140881383576488</v>
       </c>
       <c r="X13">
-        <v>0.005667439211996144</v>
+        <v>0.00566743921199563</v>
       </c>
       <c r="Y13">
-        <v>0.004800590955142506</v>
+        <v>0.004800590955142724</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1544,76 +1544,76 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.004733623133315053</v>
+        <v>0.00473362313331501</v>
       </c>
       <c r="C14">
-        <v>0.004380264493047436</v>
+        <v>0.0043802644930473825</v>
       </c>
       <c r="D14">
-        <v>0.004120246250009962</v>
+        <v>0.004120246250009926</v>
       </c>
       <c r="E14">
-        <v>0.003946900933301193</v>
+        <v>0.003946900933301131</v>
       </c>
       <c r="F14">
-        <v>0.00398690368601738</v>
+        <v>0.003986903686017353</v>
       </c>
       <c r="G14">
-        <v>0.0040869106011132686</v>
+        <v>0.004086910601113249</v>
       </c>
       <c r="H14">
-        <v>0.004293591709308282</v>
+        <v>0.004293591709308252</v>
       </c>
       <c r="I14">
-        <v>0.004453603029186217</v>
+        <v>0.004453603029186188</v>
       </c>
       <c r="J14">
-        <v>0.004700287385902508</v>
+        <v>0.0047002873859024715</v>
       </c>
       <c r="K14">
-        <v>0.005000309290437494</v>
+        <v>0.00500030929043746</v>
       </c>
       <c r="L14">
-        <v>0.005180322638640544</v>
+        <v>0.005180322638640513</v>
       </c>
       <c r="M14">
-        <v>0.005246994288509893</v>
+        <v>0.0052469942885098615</v>
       </c>
       <c r="N14">
-        <v>0.005306998791782146</v>
+        <v>0.005306998791782114</v>
       </c>
       <c r="O14">
-        <v>0.005213658461760528</v>
+        <v>0.005213658461760489</v>
       </c>
       <c r="P14">
-        <v>0.005220325627069598</v>
+        <v>0.005220325627069463</v>
       </c>
       <c r="Q14">
-        <v>0.005260328620507731</v>
+        <v>0.005260328620507732</v>
       </c>
       <c r="R14">
-        <v>0.00550701392339332</v>
+        <v>0.005507013923393322</v>
       </c>
       <c r="S14">
-        <v>0.005700362066720761</v>
+        <v>0.005700362066720781</v>
       </c>
       <c r="T14">
-        <v>0.006333745157494132</v>
+        <v>0.006333745157494172</v>
       </c>
       <c r="U14">
-        <v>0.00666710544337898</v>
+        <v>0.006667105443378895</v>
       </c>
       <c r="V14">
-        <v>0.0064670892081757254</v>
+        <v>0.006467089208175651</v>
       </c>
       <c r="W14">
-        <v>0.00614039643422123</v>
+        <v>0.006140396434221306</v>
       </c>
       <c r="X14">
-        <v>0.00566702617260611</v>
+        <v>0.0056670261726060305</v>
       </c>
       <c r="Y14">
-        <v>0.00480029464536447</v>
+        <v>0.004800294645364505</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -1621,76 +1621,76 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.011262602765156027</v>
+        <v>0.011262585310224699</v>
       </c>
       <c r="C15">
-        <v>0.009713034713661993</v>
+        <v>0.009712995860138731</v>
       </c>
       <c r="D15">
-        <v>0.008588594541377595</v>
+        <v>0.008588524844934255</v>
       </c>
       <c r="E15">
-        <v>0.00785133593681851</v>
+        <v>0.007851234640988955</v>
       </c>
       <c r="F15">
-        <v>0.008020359997043276</v>
+        <v>0.008020266865080804</v>
       </c>
       <c r="G15">
-        <v>0.008445937535877336</v>
+        <v>0.008445862443217898</v>
       </c>
       <c r="H15">
-        <v>0.009354469858085544</v>
+        <v>0.009354423186373497</v>
       </c>
       <c r="I15">
-        <v>0.010107445083206509</v>
+        <v>0.010107414051398823</v>
       </c>
       <c r="J15">
-        <v>0.011287083879678288</v>
+        <v>0.011287067379352377</v>
       </c>
       <c r="K15">
-        <v>0.012938453314103825</v>
+        <v>0.012938446488027345</v>
       </c>
       <c r="L15">
-        <v>0.014641030809718854</v>
+        <v>0.014641028105134794</v>
       </c>
       <c r="M15">
-        <v>0.015402564796279786</v>
+        <v>0.015402562944672321</v>
       </c>
       <c r="N15">
-        <v>0.016272675163983442</v>
+        <v>0.016272673931691625</v>
       </c>
       <c r="O15">
-        <v>0.01585539921095027</v>
+        <v>0.01585539775176105</v>
       </c>
       <c r="P15">
-        <v>0.01581697940752414</v>
+        <v>0.015816977835937163</v>
       </c>
       <c r="Q15">
-        <v>0.015360503555678027</v>
+        <v>0.015360503554972973</v>
       </c>
       <c r="R15">
-        <v>0.015628683533786842</v>
+        <v>0.015628683535162013</v>
       </c>
       <c r="S15">
-        <v>0.01577036803105085</v>
+        <v>0.01577036806178318</v>
       </c>
       <c r="T15">
-        <v>0.01832083120586763</v>
+        <v>0.018320831222193527</v>
       </c>
       <c r="U15">
-        <v>0.01980123868876438</v>
+        <v>0.019801238636827808</v>
       </c>
       <c r="V15">
-        <v>0.01890119696511603</v>
+        <v>0.018901196937563192</v>
       </c>
       <c r="W15">
-        <v>0.017431840038024855</v>
+        <v>0.017431840062789392</v>
       </c>
       <c r="X15">
-        <v>0.015411628239561471</v>
+        <v>0.01541162541920933</v>
       </c>
       <c r="Y15">
-        <v>0.011561446956938089</v>
+        <v>0.011561430963618311</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -1775,76 +1775,76 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.0021326132521390087</v>
+        <v>0.002132556301988195</v>
       </c>
       <c r="C17">
-        <v>0.001819039518058132</v>
+        <v>0.0018189625943495836</v>
       </c>
       <c r="D17">
-        <v>0.001597177297581881</v>
+        <v>0.0015970837212705756</v>
       </c>
       <c r="E17">
-        <v>0.0014545600718930698</v>
+        <v>0.0014544550401362098</v>
       </c>
       <c r="F17">
-        <v>0.0014870521734344712</v>
+        <v>0.0014869497807992397</v>
       </c>
       <c r="G17">
-        <v>0.0015693921202927434</v>
+        <v>0.0015693084307062172</v>
       </c>
       <c r="H17">
-        <v>0.0017523883339923751</v>
+        <v>0.0017523077469673253</v>
       </c>
       <c r="I17">
-        <v>0.0019172254709967009</v>
+        <v>0.001917157629195325</v>
       </c>
       <c r="J17">
-        <v>0.0021824508329932207</v>
+        <v>0.002182399748626265</v>
       </c>
       <c r="K17">
-        <v>0.0026121234554821984</v>
+        <v>0.0026120929256859835</v>
       </c>
       <c r="L17">
-        <v>0.0032174320413162487</v>
+        <v>0.003217419002824309</v>
       </c>
       <c r="M17">
-        <v>0.0035077405233872594</v>
+        <v>0.0035077319299388404</v>
       </c>
       <c r="N17">
-        <v>0.0038607087086561594</v>
+        <v>0.0038607033728156044</v>
       </c>
       <c r="O17">
-        <v>0.0037698377891419517</v>
+        <v>0.0037698319547875897</v>
       </c>
       <c r="P17">
-        <v>0.0037427534834809585</v>
+        <v>0.0037427474334845406</v>
       </c>
       <c r="Q17">
-        <v>0.0034270468071159743</v>
+        <v>0.003427046745302235</v>
       </c>
       <c r="R17">
-        <v>0.0032525807080461054</v>
+        <v>0.0032525806248035532</v>
       </c>
       <c r="S17">
-        <v>0.0030815144314733974</v>
+        <v>0.003081514315098725</v>
       </c>
       <c r="T17">
-        <v>0.003562069097984366</v>
+        <v>0.003562069052952501</v>
       </c>
       <c r="U17">
-        <v>0.003884400441293996</v>
+        <v>0.003884400416020618</v>
       </c>
       <c r="V17">
-        <v>0.0036851780667626387</v>
+        <v>0.0036851780306577553</v>
       </c>
       <c r="W17">
-        <v>0.0033600105903554976</v>
+        <v>0.0033600105233111766</v>
       </c>
       <c r="X17">
-        <v>0.003002611861203149</v>
+        <v>0.0030025887799725284</v>
       </c>
       <c r="Y17">
-        <v>0.002193030980451837</v>
+        <v>0.0021929773586243056</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -1852,76 +1852,76 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.002366722119420683</v>
+        <v>0.002366722119420608</v>
       </c>
       <c r="C18">
-        <v>0.002190031123450955</v>
+        <v>0.002190031123450875</v>
       </c>
       <c r="D18">
-        <v>0.002060015302619364</v>
+        <v>0.0020600153026193676</v>
       </c>
       <c r="E18">
-        <v>0.0019733390698117243</v>
+        <v>0.0019733390698112546</v>
       </c>
       <c r="F18">
-        <v>0.0019933412077326822</v>
+        <v>0.0019933412077325252</v>
       </c>
       <c r="G18">
-        <v>0.0020433467354658195</v>
+        <v>0.0020433467354658437</v>
       </c>
       <c r="H18">
-        <v>0.0021466923200154637</v>
+        <v>0.002146692320015444</v>
       </c>
       <c r="I18">
-        <v>0.002226702570654401</v>
+        <v>0.002226702570654359</v>
       </c>
       <c r="J18">
-        <v>0.0023500530167931757</v>
+        <v>0.002350053016793107</v>
       </c>
       <c r="K18">
-        <v>0.0025000759707755438</v>
+        <v>0.0025000759707754757</v>
       </c>
       <c r="L18">
-        <v>0.0025900908725139545</v>
+        <v>0.002590090872513891</v>
       </c>
       <c r="M18">
-        <v>0.002623429940460217</v>
+        <v>0.0026234299404601464</v>
       </c>
       <c r="N18">
-        <v>0.002653435201646138</v>
+        <v>0.0026534352016460505</v>
       </c>
       <c r="O18">
-        <v>0.002606760394646658</v>
+        <v>0.0026067603946465174</v>
       </c>
       <c r="P18">
-        <v>0.0026100943024851145</v>
+        <v>0.002610094302484891</v>
       </c>
       <c r="Q18">
-        <v>0.00263009776653253</v>
+        <v>0.0026300977665325315</v>
       </c>
       <c r="R18">
-        <v>0.00275345340740365</v>
+        <v>0.002753453407403659</v>
       </c>
       <c r="S18">
-        <v>0.002850138670135502</v>
+        <v>0.0028501386701356105</v>
       </c>
       <c r="T18">
-        <v>0.003166873086426503</v>
+        <v>0.0031668730864265466</v>
       </c>
       <c r="U18">
-        <v>0.003333579615957442</v>
+        <v>0.0033335796159572463</v>
       </c>
       <c r="V18">
-        <v>0.003233555349740796</v>
+        <v>0.003233555349740726</v>
       </c>
       <c r="W18">
-        <v>0.003070184629154009</v>
+        <v>0.003070184629154058</v>
       </c>
       <c r="X18">
-        <v>0.002833468738464861</v>
+        <v>0.002833468738464532</v>
       </c>
       <c r="Y18">
-        <v>0.0024000604196357943</v>
+        <v>0.0024000604196359647</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -1929,76 +1929,76 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.0017166348390261986</v>
+        <v>0.0017166305519427246</v>
       </c>
       <c r="C19">
-        <v>0.0013771183610542766</v>
+        <v>0.0013771098371934596</v>
       </c>
       <c r="D19">
-        <v>0.0011310123151536745</v>
+        <v>0.0011309982326361742</v>
       </c>
       <c r="E19">
-        <v>0.0009694555455608127</v>
+        <v>0.0009694363322106775</v>
       </c>
       <c r="F19">
-        <v>0.001006531074080116</v>
+        <v>0.0010065130801263568</v>
       </c>
       <c r="G19">
-        <v>0.0010997701934542157</v>
+        <v>0.001099755141655008</v>
       </c>
       <c r="H19">
-        <v>0.001294484794534733</v>
+        <v>0.0012944747262608595</v>
       </c>
       <c r="I19">
-        <v>0.0014465858285965013</v>
+        <v>0.0014465786316822185</v>
       </c>
       <c r="J19">
-        <v>0.0016833486225225707</v>
+        <v>0.0016833443498209325</v>
       </c>
       <c r="K19">
-        <v>0.0019730923516002715</v>
+        <v>0.0019730902318151147</v>
       </c>
       <c r="L19">
-        <v>0.0021455596560317116</v>
+        <v>0.002145558576331036</v>
       </c>
       <c r="M19">
-        <v>0.002209443549133674</v>
+        <v>0.0022094427359246886</v>
       </c>
       <c r="N19">
-        <v>0.002266621160246674</v>
+        <v>0.002266620566783339</v>
       </c>
       <c r="O19">
-        <v>0.002174794853944395</v>
+        <v>0.0021747941516446147</v>
       </c>
       <c r="P19">
-        <v>0.002181587149352187</v>
+        <v>0.002181586408484786</v>
       </c>
       <c r="Q19">
-        <v>0.0021752753943110495</v>
+        <v>0.002175275393828362</v>
       </c>
       <c r="R19">
-        <v>0.0024217621360120346</v>
+        <v>0.002421762136024393</v>
       </c>
       <c r="S19">
-        <v>0.002614991470923738</v>
+        <v>0.0026149914765346677</v>
       </c>
       <c r="T19">
-        <v>0.0032469530601239886</v>
+        <v>0.003246953059250751</v>
       </c>
       <c r="U19">
-        <v>0.003579669420398561</v>
+        <v>0.00357966941695784</v>
       </c>
       <c r="V19">
-        <v>0.0033800375158464947</v>
+        <v>0.0033800375175084907</v>
       </c>
       <c r="W19">
-        <v>0.003054022425947586</v>
+        <v>0.0030540224223885577</v>
       </c>
       <c r="X19">
-        <v>0.002628476947566688</v>
+        <v>0.002628475975867827</v>
       </c>
       <c r="Y19">
-        <v>0.0017816773784075457</v>
+        <v>0.0017816727963679462</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2006,76 +2006,76 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.0024342814778848722</v>
+        <v>0.002434268316658558</v>
       </c>
       <c r="C20">
-        <v>0.0017559143385303287</v>
+        <v>0.0017558840019390263</v>
       </c>
       <c r="D20">
-        <v>0.001268621602654504</v>
+        <v>0.0012685659306243054</v>
       </c>
       <c r="E20">
-        <v>0.0009532940187764477</v>
+        <v>0.0009532120227600926</v>
       </c>
       <c r="F20">
-        <v>0.0010251776493116714</v>
+        <v>0.0010251024906983877</v>
       </c>
       <c r="G20">
-        <v>0.0012072618173762308</v>
+        <v>0.0012072017063794824</v>
       </c>
       <c r="H20">
-        <v>0.0016104924499984034</v>
+        <v>0.0016104558142704512</v>
       </c>
       <c r="I20">
-        <v>0.0019708676574101015</v>
+        <v>0.001970843809466825</v>
       </c>
       <c r="J20">
-        <v>0.002542808408871168</v>
+        <v>0.002542796187003667</v>
       </c>
       <c r="K20">
-        <v>0.0034533352306899082</v>
+        <v>0.003453330536527349</v>
       </c>
       <c r="L20">
-        <v>0.0047130227564997264</v>
+        <v>0.004713021144795998</v>
       </c>
       <c r="M20">
-        <v>0.005310446018342554</v>
+        <v>0.0053104449954921055</v>
       </c>
       <c r="N20">
-        <v>0.006033143328448278</v>
+        <v>0.006033142709190639</v>
       </c>
       <c r="O20">
-        <v>0.005848083907988043</v>
+        <v>0.005848083183896743</v>
       </c>
       <c r="P20">
-        <v>0.005792639133496049</v>
+        <v>0.005792638356111833</v>
       </c>
       <c r="Q20">
-        <v>0.005282697213787317</v>
+        <v>0.005282697213123922</v>
       </c>
       <c r="R20">
-        <v>0.004932668455492441</v>
+        <v>0.004932668454701581</v>
       </c>
       <c r="S20">
-        <v>0.004589358636725663</v>
+        <v>0.004589358635771898</v>
       </c>
       <c r="T20">
-        <v>0.005555037531777364</v>
+        <v>0.005555037539836768</v>
       </c>
       <c r="U20">
-        <v>0.006201809761446067</v>
+        <v>0.006201809749787842</v>
       </c>
       <c r="V20">
-        <v>0.005802002363043316</v>
+        <v>0.00580200234775524</v>
       </c>
       <c r="W20">
-        <v>0.005149386165471059</v>
+        <v>0.005149386183092092</v>
       </c>
       <c r="X20">
-        <v>0.004264368624988044</v>
+        <v>0.00426436685742628</v>
       </c>
       <c r="Y20">
-        <v>0.0025642891133079862</v>
+        <v>0.002564277624621613</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2083,76 +2083,76 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.0023668097228949033</v>
+        <v>0.0023668097228945967</v>
       </c>
       <c r="C21">
-        <v>0.0021901061207224445</v>
+        <v>0.002190106120722058</v>
       </c>
       <c r="D21">
-        <v>0.0020600816506969716</v>
+        <v>0.002060081650696719</v>
       </c>
       <c r="E21">
-        <v>0.001973399947433947</v>
+        <v>0.0019733999474335143</v>
       </c>
       <c r="F21">
-        <v>0.001993403326810941</v>
+        <v>0.001993403326810746</v>
       </c>
       <c r="G21">
-        <v>0.0020434120132769716</v>
+        <v>0.00204341201327683</v>
       </c>
       <c r="H21">
-        <v>0.0021467643730040007</v>
+        <v>0.0021467643730037895</v>
       </c>
       <c r="I21">
-        <v>0.002226780098935475</v>
+        <v>0.002226780098935258</v>
       </c>
       <c r="J21">
-        <v>0.002350139381411252</v>
+        <v>0.0023501393814109946</v>
       </c>
       <c r="K21">
-        <v>0.0025001737256092676</v>
+        <v>0.0025001737256090217</v>
       </c>
       <c r="L21">
-        <v>0.002590195800651615</v>
+        <v>0.002590195800651395</v>
       </c>
       <c r="M21">
-        <v>0.0026235375916776283</v>
+        <v>0.0026235375916774015</v>
       </c>
       <c r="N21">
-        <v>0.002653545335028303</v>
+        <v>0.002653545335028072</v>
       </c>
       <c r="O21">
-        <v>0.0026068666831954627</v>
+        <v>0.0026068666831951834</v>
       </c>
       <c r="P21">
-        <v>0.002610200864600263</v>
+        <v>0.0026102008645992967</v>
       </c>
       <c r="Q21">
-        <v>0.0026302059643476235</v>
+        <v>0.002630205964347626</v>
       </c>
       <c r="R21">
-        <v>0.0027535720088348184</v>
+        <v>0.0027535720088348306</v>
       </c>
       <c r="S21">
-        <v>0.0028502657663909935</v>
+        <v>0.0028502657663911366</v>
       </c>
       <c r="T21">
-        <v>0.0031670300549308792</v>
+        <v>0.0031670300549311715</v>
       </c>
       <c r="U21">
-        <v>0.003333753564700527</v>
+        <v>0.0033337535646999193</v>
       </c>
       <c r="V21">
-        <v>0.003233719003786693</v>
+        <v>0.003233719003786159</v>
       </c>
       <c r="W21">
-        <v>0.0030703321526450605</v>
+        <v>0.0030703321526455987</v>
       </c>
       <c r="X21">
-        <v>0.002833594376466316</v>
+        <v>0.0028335943764657427</v>
       </c>
       <c r="Y21">
-        <v>0.00240015052895954</v>
+        <v>0.0024001505289597816</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2160,76 +2160,76 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.002366831248137809</v>
+        <v>0.0023668312481374856</v>
       </c>
       <c r="C22">
-        <v>0.0021901245509444336</v>
+        <v>0.002190124550944025</v>
       </c>
       <c r="D22">
-        <v>0.002060097956971777</v>
+        <v>0.0020600979569715093</v>
       </c>
       <c r="E22">
-        <v>0.001973414910102112</v>
+        <v>0.001973414910101654</v>
       </c>
       <c r="F22">
-        <v>0.0019934185944071097</v>
+        <v>0.0019934185944069037</v>
       </c>
       <c r="G22">
-        <v>0.0020434280566829595</v>
+        <v>0.00204342805668281</v>
       </c>
       <c r="H22">
-        <v>0.0021467820806383995</v>
+        <v>0.0021467820806381765</v>
       </c>
       <c r="I22">
-        <v>0.0022267991514407486</v>
+        <v>0.002226799151440519</v>
       </c>
       <c r="J22">
-        <v>0.002350160603884458</v>
+        <v>0.0023501606038841857</v>
       </c>
       <c r="K22">
-        <v>0.0025001977450279707</v>
+        <v>0.0025001977450277105</v>
       </c>
       <c r="L22">
-        <v>0.002590221581457899</v>
+        <v>0.0025902215814576665</v>
       </c>
       <c r="M22">
-        <v>0.0026235640408160893</v>
+        <v>0.0026235640408158495</v>
       </c>
       <c r="N22">
-        <v>0.002653572393113448</v>
+        <v>0.002653572393113204</v>
       </c>
       <c r="O22">
-        <v>0.0026068927974329512</v>
+        <v>0.0026068927974326563</v>
       </c>
       <c r="P22">
-        <v>0.0026102270458014444</v>
+        <v>0.002610227045800423</v>
       </c>
       <c r="Q22">
-        <v>0.0026302325479721778</v>
+        <v>0.0026302325479721812</v>
       </c>
       <c r="R22">
-        <v>0.0027536011456254176</v>
+        <v>0.00275360114562543</v>
       </c>
       <c r="S22">
-        <v>0.002850296986615404</v>
+        <v>0.0028502969866155553</v>
       </c>
       <c r="T22">
-        <v>0.0031670686031453443</v>
+        <v>0.0031670686031456522</v>
       </c>
       <c r="U22">
-        <v>0.003333796279310228</v>
+        <v>0.003333796279309586</v>
       </c>
       <c r="V22">
-        <v>0.0032337591927753045</v>
+        <v>0.00323375919277474</v>
       </c>
       <c r="W22">
-        <v>0.0030703683825672214</v>
+        <v>0.0030703683825677903</v>
       </c>
       <c r="X22">
-        <v>0.002833625234508219</v>
+        <v>0.002833625234507613</v>
       </c>
       <c r="Y22">
-        <v>0.0024001726667179004</v>
+        <v>0.002400172666718156</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2237,76 +2237,76 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.002366539014905021</v>
+        <v>0.0023665390149049336</v>
       </c>
       <c r="C23">
-        <v>0.0021898743391835333</v>
+        <v>0.0021898743391834223</v>
       </c>
       <c r="D23">
-        <v>0.00205987658191699</v>
+        <v>0.002059876581916917</v>
       </c>
       <c r="E23">
-        <v>0.0019732117769455508</v>
+        <v>0.0019732117769454263</v>
       </c>
       <c r="F23">
-        <v>0.0019932113213115207</v>
+        <v>0.001993211321311465</v>
       </c>
       <c r="G23">
-        <v>0.0020432102505599818</v>
+        <v>0.0020432102505599414</v>
       </c>
       <c r="H23">
-        <v>0.0021465416794428527</v>
+        <v>0.0021465416794427925</v>
       </c>
       <c r="I23">
-        <v>0.002226540490916551</v>
+        <v>0.002226540490916488</v>
       </c>
       <c r="J23">
-        <v>0.002349872481420663</v>
+        <v>0.0023498724814205894</v>
       </c>
       <c r="K23">
-        <v>0.0024998716476217547</v>
+        <v>0.0024998716476216844</v>
       </c>
       <c r="L23">
-        <v>0.002589871568934909</v>
+        <v>0.0025898715689348455</v>
       </c>
       <c r="M23">
-        <v>0.0026232049540116775</v>
+        <v>0.0026232049540116124</v>
       </c>
       <c r="N23">
-        <v>0.0026532050383116447</v>
+        <v>0.0026532050383115784</v>
       </c>
       <c r="O23">
-        <v>0.002606538257750048</v>
+        <v>0.0026065382577499683</v>
       </c>
       <c r="P23">
-        <v>0.0026098715969186575</v>
+        <v>0.00260987159691838</v>
       </c>
       <c r="Q23">
-        <v>0.0026298716351796556</v>
+        <v>0.0026298716351796565</v>
       </c>
       <c r="R23">
-        <v>0.0027532055669621572</v>
+        <v>0.0027532055669621603</v>
       </c>
       <c r="S23">
-        <v>0.002849873119651217</v>
+        <v>0.0028498731196512582</v>
       </c>
       <c r="T23">
-        <v>0.0031665452369276166</v>
+        <v>0.0031665452369277</v>
       </c>
       <c r="U23">
-        <v>0.0033332163407258386</v>
+        <v>0.003333216340725664</v>
       </c>
       <c r="V23">
-        <v>0.0032332135478088156</v>
+        <v>0.003233213547808662</v>
       </c>
       <c r="W23">
-        <v>0.003069876494350455</v>
+        <v>0.00306987649435061</v>
       </c>
       <c r="X23">
-        <v>0.0028332062851746075</v>
+        <v>0.002833206285174443</v>
       </c>
       <c r="Y23">
-        <v>0.002399872117213311</v>
+        <v>0.0023998721172133804</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2314,76 +2314,76 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.0018463432007438157</v>
+        <v>0.0018463421277981433</v>
       </c>
       <c r="C24">
-        <v>0.0015802016275109102</v>
+        <v>0.0015802027502797025</v>
       </c>
       <c r="D24">
-        <v>0.001416124289907533</v>
+        <v>0.0014161337051687855</v>
       </c>
       <c r="E24">
-        <v>0.0013584348953210711</v>
+        <v>0.0013584208848756822</v>
       </c>
       <c r="F24">
-        <v>0.0013682810050738327</v>
+        <v>0.0013682843438753208</v>
       </c>
       <c r="G24">
-        <v>0.0014077741190278061</v>
+        <v>0.0014077854839831775</v>
       </c>
       <c r="H24">
-        <v>0.0014992466451232151</v>
+        <v>0.0014992518773795825</v>
       </c>
       <c r="I24">
-        <v>0.0015771448816424632</v>
+        <v>0.001577146996257638</v>
       </c>
       <c r="J24">
-        <v>0.0017239220046128894</v>
+        <v>0.0017239210717937717</v>
       </c>
       <c r="K24">
-        <v>0.0018958356017431848</v>
+        <v>0.0018958336364028876</v>
       </c>
       <c r="L24">
-        <v>0.0019604514767283627</v>
+        <v>0.0019604493410998974</v>
       </c>
       <c r="M24">
-        <v>0.001995738019485965</v>
+        <v>0.001995735500086282</v>
       </c>
       <c r="N24">
-        <v>0.0020325512481199756</v>
+        <v>0.0020325480768637154</v>
       </c>
       <c r="O24">
-        <v>0.0019713940254418756</v>
+        <v>0.0019713887108367837</v>
       </c>
       <c r="P24">
-        <v>0.0020089498081913583</v>
+        <v>0.0020089411657370467</v>
       </c>
       <c r="Q24">
-        <v>0.001972062714244751</v>
+        <v>0.00197206278570875</v>
       </c>
       <c r="R24">
-        <v>0.002245482441044153</v>
+        <v>0.00224548279002488</v>
       </c>
       <c r="S24">
-        <v>0.0025269012271188556</v>
+        <v>0.0025269054523356393</v>
       </c>
       <c r="T24">
-        <v>0.0029681820622423616</v>
+        <v>0.002968183543242613</v>
       </c>
       <c r="U24">
-        <v>0.003107919897294558</v>
+        <v>0.00310791392813711</v>
       </c>
       <c r="V24">
-        <v>0.003015855838800589</v>
+        <v>0.003015853582112814</v>
       </c>
       <c r="W24">
-        <v>0.0029069777155188185</v>
+        <v>0.0029069794497548667</v>
       </c>
       <c r="X24">
-        <v>0.0029757009057007106</v>
+        <v>0.0029756877656410483</v>
       </c>
       <c r="Y24">
-        <v>0.002459782790926057</v>
+        <v>0.0024597953338401355</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -2418,7 +2418,7 @@
         <v>0.00010408517296007847</v>
       </c>
       <c r="K25">
-        <v>0.00011779779462322102</v>
+        <v>0.00011779779462322103</v>
       </c>
       <c r="L25">
         <v>0.00012643260026237716</v>
@@ -2436,7 +2436,7 @@
         <v>0.0001283929240206722</v>
       </c>
       <c r="Q25">
-        <v>0.00013036833083050954</v>
+        <v>0.0001303683308305095</v>
       </c>
       <c r="R25">
         <v>0.00014288330304167542</v>
@@ -2468,76 +2468,76 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>8.871010373416832e-5</v>
+        <v>8.870995275787644e-5</v>
       </c>
       <c r="C26">
-        <v>7.539703140005237e-5</v>
+        <v>7.539686427426897e-5</v>
       </c>
       <c r="D26">
-        <v>6.634599422401234e-5</v>
+        <v>6.634582195276093e-5</v>
       </c>
       <c r="E26">
-        <v>6.0660968617233e-5</v>
+        <v>6.0660797453363474e-5</v>
       </c>
       <c r="F26">
-        <v>6.194821456782078e-5</v>
+        <v>6.194804278306645e-5</v>
       </c>
       <c r="G26">
-        <v>6.523109486331509e-5</v>
+        <v>6.52309452758584e-5</v>
       </c>
       <c r="H26">
-        <v>6.861195740328034e-5</v>
+        <v>6.861178983234295e-5</v>
       </c>
       <c r="I26">
-        <v>7.055723163475032e-5</v>
+        <v>7.055707329912641e-5</v>
       </c>
       <c r="J26">
-        <v>7.57865888499283e-5</v>
+        <v>7.578644860295506e-5</v>
       </c>
       <c r="K26">
-        <v>7.993654141797934e-5</v>
+        <v>7.993643642350706e-5</v>
       </c>
       <c r="L26">
-        <v>7.771477952638293e-5</v>
+        <v>7.771472082418952e-5</v>
       </c>
       <c r="M26">
-        <v>7.796468259998801e-5</v>
+        <v>7.79646391492745e-5</v>
       </c>
       <c r="N26">
-        <v>7.86362021847881e-5</v>
+        <v>7.863617151641397e-5</v>
       </c>
       <c r="O26">
-        <v>7.510263157795599e-5</v>
+        <v>7.510259907322417e-5</v>
       </c>
       <c r="P26">
-        <v>7.547130816098041e-5</v>
+        <v>7.547127475243896e-5</v>
       </c>
       <c r="Q26">
-        <v>7.786243847789808e-5</v>
+        <v>7.786243809684615e-5</v>
       </c>
       <c r="R26">
-        <v>9.286752800412666e-5</v>
+        <v>9.286752751972836e-5</v>
       </c>
       <c r="S26">
-        <v>0.00011217243634386979</v>
+        <v>0.00011217243570701032</v>
       </c>
       <c r="T26">
-        <v>0.00015762741326456184</v>
+        <v>0.00015762741297384403</v>
       </c>
       <c r="U26">
-        <v>0.00018174616808304303</v>
+        <v>0.00018174616790348633</v>
       </c>
       <c r="V26">
-        <v>0.00017042295780425435</v>
+        <v>0.00017042295756220188</v>
       </c>
       <c r="W26">
-        <v>0.00015273951469505344</v>
+        <v>0.00015273951428984445</v>
       </c>
       <c r="X26">
-        <v>0.00012952249689641282</v>
+        <v>0.0001295224031093473</v>
       </c>
       <c r="Y26">
-        <v>9.135334639455344e-5</v>
+        <v>9.13531992117498e-5</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -2545,76 +2545,76 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2.6412738579846764e-5</v>
+        <v>2.641273857305455e-5</v>
       </c>
       <c r="C27">
-        <v>2.26155635504479e-5</v>
+        <v>2.261556354318418e-5</v>
       </c>
       <c r="D27">
-        <v>2.0009652965345745e-5</v>
+        <v>2.000965296562622e-5</v>
       </c>
       <c r="E27">
-        <v>1.8361086154444384e-5</v>
+        <v>1.83610861119352e-5</v>
       </c>
       <c r="F27">
-        <v>1.873522705978195e-5</v>
+        <v>1.8735227045578088e-5</v>
       </c>
       <c r="G27">
-        <v>1.9687119482888837e-5</v>
+        <v>1.9687119485069398e-5</v>
       </c>
       <c r="H27">
-        <v>2.1729160386223682e-5</v>
+        <v>2.1729160384441488e-5</v>
       </c>
       <c r="I27">
-        <v>2.3379339460364658e-5</v>
+        <v>2.3379339456570913e-5</v>
       </c>
       <c r="J27">
-        <v>2.60417888238293e-5</v>
+        <v>2.6041788817579974e-5</v>
       </c>
       <c r="K27">
-        <v>2.9473497034142905e-5</v>
+        <v>2.9473497027944667e-5</v>
       </c>
       <c r="L27">
-        <v>3.163463499191345e-5</v>
+        <v>3.163463498624165e-5</v>
       </c>
       <c r="M27">
-        <v>3.245453698108581e-5</v>
+        <v>3.2454536974670835e-5</v>
       </c>
       <c r="N27">
-        <v>3.3201493631826254e-5</v>
+        <v>3.3201493623924386e-5</v>
       </c>
       <c r="O27">
-        <v>3.204351540339092e-5</v>
+        <v>3.2043515390662004e-5</v>
       </c>
       <c r="P27">
-        <v>3.2125599982926367e-5</v>
+        <v>3.2125599962726515e-5</v>
       </c>
       <c r="Q27">
-        <v>3.2619646067336335e-5</v>
+        <v>3.261964606749517e-5</v>
       </c>
       <c r="R27">
-        <v>3.575179069141819e-5</v>
+        <v>3.575179069221809e-5</v>
       </c>
       <c r="S27">
-        <v>3.830723923438699e-5</v>
+        <v>3.830723924420726e-5</v>
       </c>
       <c r="T27">
-        <v>4.729622222854707e-5</v>
+        <v>4.7296222232535775e-5</v>
       </c>
       <c r="U27">
-        <v>5.240748706417243e-5</v>
+        <v>5.240748704646281e-5</v>
       </c>
       <c r="V27">
-        <v>4.9309217800631966e-5</v>
+        <v>4.930921779426104e-5</v>
       </c>
       <c r="W27">
-        <v>4.4451930969626156e-5</v>
+        <v>4.445193097404121e-5</v>
       </c>
       <c r="X27">
-        <v>3.7861329383162356e-5</v>
+        <v>3.786132935346242e-5</v>
       </c>
       <c r="Y27">
-        <v>2.7163224156548375e-5</v>
+        <v>2.7163224171978192e-5</v>
       </c>
     </row>
     <row r="28" spans="1:25">
@@ -2622,76 +2622,76 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>8.956919837473248e-5</v>
+        <v>8.95693843438484e-5</v>
       </c>
       <c r="C28">
-        <v>7.809384857377952e-5</v>
+        <v>7.809459765198285e-5</v>
       </c>
       <c r="D28">
-        <v>7.333797725537357e-5</v>
+        <v>7.334033775303703e-5</v>
       </c>
       <c r="E28">
-        <v>7.943857267655233e-5</v>
+        <v>7.943405901815051e-5</v>
       </c>
       <c r="F28">
-        <v>7.731452222171268e-5</v>
+        <v>7.731455807598618e-5</v>
       </c>
       <c r="G28">
-        <v>7.503836323028164e-5</v>
+        <v>7.504087684466095e-5</v>
       </c>
       <c r="H28">
-        <v>7.777647464530239e-5</v>
+        <v>7.777782052175033e-5</v>
       </c>
       <c r="I28">
-        <v>8.218749574042518e-5</v>
+        <v>8.218819185227767e-5</v>
       </c>
       <c r="J28">
-        <v>8.988477530036526e-5</v>
+        <v>8.98849089203474e-5</v>
       </c>
       <c r="K28">
-        <v>0.00010102378969589426</v>
+        <v>0.0001010237182317479</v>
       </c>
       <c r="L28">
-        <v>0.00010875301550502948</v>
+        <v>0.00010875287311219125</v>
       </c>
       <c r="M28">
-        <v>0.00011195634782682413</v>
+        <v>0.00011195610912586112</v>
       </c>
       <c r="N28">
-        <v>0.00011510622497300928</v>
+        <v>0.00011510579649084599</v>
       </c>
       <c r="O28">
-        <v>0.00011326332838902015</v>
+        <v>0.0001132623587180167</v>
       </c>
       <c r="P28">
-        <v>0.00011803563599812032</v>
+        <v>0.00011803530064702117</v>
       </c>
       <c r="Q28">
-        <v>0.00010788231960103775</v>
+        <v>0.00010788233706276635</v>
       </c>
       <c r="R28">
-        <v>0.0001188799911518216</v>
+        <v>0.00011888007672745649</v>
       </c>
       <c r="S28">
-        <v>0.00012669035393722146</v>
+        <v>0.00012669134184615963</v>
       </c>
       <c r="T28">
-        <v>0.00010655497782074299</v>
+        <v>0.00010655486296455761</v>
       </c>
       <c r="U28">
-        <v>9.66984681140738e-5</v>
+        <v>9.669793835323105e-5</v>
       </c>
       <c r="V28">
-        <v>0.00010347285432105884</v>
+        <v>0.0001034731400243381</v>
       </c>
       <c r="W28">
-        <v>0.00011017031550363163</v>
+        <v>0.00011016977985867443</v>
       </c>
       <c r="X28">
-        <v>0.00017562448546552836</v>
+        <v>0.0001756216638967524</v>
       </c>
       <c r="Y28">
-        <v>0.0001856927476084797</v>
+        <v>0.00018569598612568053</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -2699,76 +2699,76 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.00034610888118359167</v>
+        <v>0.0003461081265245712</v>
       </c>
       <c r="C29">
-        <v>0.0002961922359402949</v>
+        <v>0.00029619145543245814</v>
       </c>
       <c r="D29">
-        <v>0.000264078938140603</v>
+        <v>0.00026407895888504114</v>
       </c>
       <c r="E29">
-        <v>0.00024686270568471935</v>
+        <v>0.0002468664478591871</v>
       </c>
       <c r="F29">
-        <v>0.0002507295208697721</v>
+        <v>0.00025073189054402754</v>
       </c>
       <c r="G29">
-        <v>0.0002610257699103788</v>
+        <v>0.0002610264732759833</v>
       </c>
       <c r="H29">
-        <v>0.0002716434136170716</v>
+        <v>0.00027164339529887454</v>
       </c>
       <c r="I29">
-        <v>0.0002777588679664852</v>
+        <v>0.0002777586530995801</v>
       </c>
       <c r="J29">
-        <v>0.00029580786053430135</v>
+        <v>0.00029580732913763965</v>
       </c>
       <c r="K29">
-        <v>0.0003091918508938317</v>
+        <v>0.00030919123220410615</v>
       </c>
       <c r="L29">
-        <v>0.0002974646300061752</v>
+        <v>0.0002974640722703857</v>
       </c>
       <c r="M29">
-        <v>0.000297359559325326</v>
+        <v>0.00029735902164500927</v>
       </c>
       <c r="N29">
-        <v>0.00029900929098598627</v>
+        <v>0.0002990088298206349</v>
       </c>
       <c r="O29">
-        <v>0.000289259324413313</v>
+        <v>0.0002892589421411053</v>
       </c>
       <c r="P29">
-        <v>0.00029561629509603274</v>
+        <v>0.0002956135231291228</v>
       </c>
       <c r="Q29">
-        <v>0.00029333727573352614</v>
+        <v>0.00029333727745617946</v>
       </c>
       <c r="R29">
-        <v>0.00035447438830276534</v>
+        <v>0.00035447439072222445</v>
       </c>
       <c r="S29">
-        <v>0.000432522004852488</v>
+        <v>0.0004325220136146411</v>
       </c>
       <c r="T29">
-        <v>0.0005683569036945164</v>
+        <v>0.0005683578539228638</v>
       </c>
       <c r="U29">
-        <v>0.000598676603923119</v>
+        <v>0.0005986753030599317</v>
       </c>
       <c r="V29">
-        <v>0.0005745994255574303</v>
+        <v>0.0005745977235727924</v>
       </c>
       <c r="W29">
-        <v>0.0005651615075885344</v>
+        <v>0.000565163560772316</v>
       </c>
       <c r="X29">
-        <v>0.0005438455478275318</v>
+        <v>0.0005438449431188449</v>
       </c>
       <c r="Y29">
-        <v>0.0004393811571850161</v>
+        <v>0.0004393817729784901</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -2776,76 +2776,76 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>2.6423231734095178e-5</v>
+        <v>2.642323171277249e-5</v>
       </c>
       <c r="C30">
-        <v>2.2623708778208756e-5</v>
+        <v>2.2623708751307765e-5</v>
       </c>
       <c r="D30">
-        <v>2.0016335929638103e-5</v>
+        <v>2.001633591201768e-5</v>
       </c>
       <c r="E30">
-        <v>1.8366931007913304e-5</v>
+        <v>1.8366930977778487e-5</v>
       </c>
       <c r="F30">
-        <v>1.874125798896089e-5</v>
+        <v>1.8741257975390062e-5</v>
       </c>
       <c r="G30">
-        <v>1.969363844431858e-5</v>
+        <v>1.969363843444719e-5</v>
       </c>
       <c r="H30">
-        <v>2.1736651602982156e-5</v>
+        <v>2.1736651588273324e-5</v>
       </c>
       <c r="I30">
-        <v>2.3387633921547997e-5</v>
+        <v>2.3387633906461294e-5</v>
       </c>
       <c r="J30">
-        <v>2.605154158266638e-5</v>
+        <v>2.605154156471858e-5</v>
       </c>
       <c r="K30">
-        <v>2.948518542236869e-5</v>
+        <v>2.948518540524454e-5</v>
       </c>
       <c r="L30">
-        <v>3.164755976459512e-5</v>
+        <v>3.164755974929476e-5</v>
       </c>
       <c r="M30">
-        <v>3.246804495764061e-5</v>
+        <v>3.246804494186662e-5</v>
       </c>
       <c r="N30">
-        <v>3.321562707156864e-5</v>
+        <v>3.321562705552035e-5</v>
       </c>
       <c r="O30">
-        <v>3.205689989491816e-5</v>
+        <v>3.205689987548853e-5</v>
       </c>
       <c r="P30">
-        <v>3.2139108614011704e-5</v>
+        <v>3.2139108546760154e-5</v>
       </c>
       <c r="Q30">
-        <v>3.263314853702478e-5</v>
+        <v>3.263314853721248e-5</v>
       </c>
       <c r="R30">
-        <v>3.576759457510009e-5</v>
+        <v>3.576759457594031e-5</v>
       </c>
       <c r="S30">
-        <v>3.832538984586848e-5</v>
+        <v>3.832538985583363e-5</v>
       </c>
       <c r="T30">
-        <v>4.732200578825708e-5</v>
+        <v>4.732200580855587e-5</v>
       </c>
       <c r="U30">
-        <v>5.243722455485018e-5</v>
+        <v>5.2437224512569966e-5</v>
       </c>
       <c r="V30">
-        <v>4.933642824175358e-5</v>
+        <v>4.933642820456883e-5</v>
       </c>
       <c r="W30">
-        <v>4.447579716832983e-5</v>
+        <v>4.447579720578403e-5</v>
       </c>
       <c r="X30">
-        <v>3.78807433344948e-5</v>
+        <v>3.788074329459509e-5</v>
       </c>
       <c r="Y30">
-        <v>2.717517783442297e-5</v>
+        <v>2.7175177851255814e-5</v>
       </c>
     </row>
     <row r="31" spans="1:25">
@@ -2853,76 +2853,76 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>2.6423029197905562e-5</v>
+        <v>2.642302917658321e-5</v>
       </c>
       <c r="C31">
-        <v>2.262354832421861e-5</v>
+        <v>2.2623548297318e-5</v>
       </c>
       <c r="D31">
-        <v>2.001620240286159e-5</v>
+        <v>2.0016202385241408e-5</v>
       </c>
       <c r="E31">
-        <v>1.8366813642872603e-5</v>
+        <v>1.836681361273816e-5</v>
       </c>
       <c r="F31">
-        <v>1.8741137017295576e-5</v>
+        <v>1.8741137003724926e-5</v>
       </c>
       <c r="G31">
-        <v>1.9693508133928193e-5</v>
+        <v>1.9693508124056932e-5</v>
       </c>
       <c r="H31">
-        <v>2.173650049496531e-5</v>
+        <v>2.1736500480256684e-5</v>
       </c>
       <c r="I31">
-        <v>2.3387465272236796e-5</v>
+        <v>2.338746525715032e-5</v>
       </c>
       <c r="J31">
-        <v>2.6051343308206175e-5</v>
+        <v>2.6051343290258638e-5</v>
       </c>
       <c r="K31">
-        <v>2.948494667631304e-5</v>
+        <v>2.948494665918917e-5</v>
       </c>
       <c r="L31">
-        <v>3.164729427371748e-5</v>
+        <v>3.164729425841736e-5</v>
       </c>
       <c r="M31">
-        <v>3.246776907278177e-5</v>
+        <v>3.246776905700805e-5</v>
       </c>
       <c r="N31">
-        <v>3.3215341600365094e-5</v>
+        <v>3.321534158431709e-5</v>
       </c>
       <c r="O31">
-        <v>3.205662923338843e-5</v>
+        <v>3.205662921395913e-5</v>
       </c>
       <c r="P31">
-        <v>3.21388369099371e-5</v>
+        <v>3.213883684268669e-5</v>
       </c>
       <c r="Q31">
-        <v>3.263287054566063e-5</v>
+        <v>3.263287054584834e-5</v>
       </c>
       <c r="R31">
-        <v>3.576727557534293e-5</v>
+        <v>3.576727557618313e-5</v>
       </c>
       <c r="S31">
-        <v>3.832503601278821e-5</v>
+        <v>3.832503602275316e-5</v>
       </c>
       <c r="T31">
-        <v>4.732152028118966e-5</v>
+        <v>4.7321520301488034e-5</v>
       </c>
       <c r="U31">
-        <v>5.2436658220310373e-5</v>
+        <v>5.2436658178031056e-5</v>
       </c>
       <c r="V31">
-        <v>4.933591140086813e-5</v>
+        <v>4.933591136368415e-5</v>
       </c>
       <c r="W31">
-        <v>4.447535480382636e-5</v>
+        <v>4.4475354841279796e-5</v>
       </c>
       <c r="X31">
-        <v>3.788039563075038e-5</v>
+        <v>3.7880395590851414e-5</v>
       </c>
       <c r="Y31">
-        <v>2.7174966582064037e-5</v>
+        <v>2.7174966598896628e-5</v>
       </c>
     </row>
     <row r="32" spans="1:25">
@@ -2930,76 +2930,76 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>2.6423029197905566e-5</v>
+        <v>2.6423029176583205e-5</v>
       </c>
       <c r="C32">
-        <v>2.2623548324218614e-5</v>
+        <v>2.2623548297318e-5</v>
       </c>
       <c r="D32">
-        <v>2.0016202402861594e-5</v>
+        <v>2.0016202385241408e-5</v>
       </c>
       <c r="E32">
-        <v>1.83668136428726e-5</v>
+        <v>1.836681361273816e-5</v>
       </c>
       <c r="F32">
-        <v>1.8741137017295573e-5</v>
+        <v>1.8741137003724926e-5</v>
       </c>
       <c r="G32">
-        <v>1.9693508133928193e-5</v>
+        <v>1.9693508124056932e-5</v>
       </c>
       <c r="H32">
-        <v>2.173650049496531e-5</v>
+        <v>2.1736500480256684e-5</v>
       </c>
       <c r="I32">
-        <v>2.33874652722368e-5</v>
+        <v>2.3387465257150323e-5</v>
       </c>
       <c r="J32">
-        <v>2.6051343308206172e-5</v>
+        <v>2.6051343290258645e-5</v>
       </c>
       <c r="K32">
-        <v>2.948494667631305e-5</v>
+        <v>2.948494665918917e-5</v>
       </c>
       <c r="L32">
-        <v>3.164729427371747e-5</v>
+        <v>3.164729425841736e-5</v>
       </c>
       <c r="M32">
-        <v>3.246776907278176e-5</v>
+        <v>3.2467769057008044e-5</v>
       </c>
       <c r="N32">
-        <v>3.32153416003651e-5</v>
+        <v>3.3215341584317085e-5</v>
       </c>
       <c r="O32">
-        <v>3.205662923338843e-5</v>
+        <v>3.205662921395912e-5</v>
       </c>
       <c r="P32">
-        <v>3.21388369099371e-5</v>
+        <v>3.213883684268669e-5</v>
       </c>
       <c r="Q32">
-        <v>3.263287054566064e-5</v>
+        <v>3.263287054584834e-5</v>
       </c>
       <c r="R32">
-        <v>3.5767275575342925e-5</v>
+        <v>3.5767275576183135e-5</v>
       </c>
       <c r="S32">
-        <v>3.832503601278821e-5</v>
+        <v>3.832503602275317e-5</v>
       </c>
       <c r="T32">
-        <v>4.732152028118967e-5</v>
+        <v>4.732152030148804e-5</v>
       </c>
       <c r="U32">
-        <v>5.2436658220310373e-5</v>
+        <v>5.243665817803106e-5</v>
       </c>
       <c r="V32">
-        <v>4.933591140086813e-5</v>
+        <v>4.9335911363684146e-5</v>
       </c>
       <c r="W32">
-        <v>4.4475354803826364e-5</v>
+        <v>4.4475354841279796e-5</v>
       </c>
       <c r="X32">
-        <v>3.7880395630750386e-5</v>
+        <v>3.788039559085141e-5</v>
       </c>
       <c r="Y32">
-        <v>2.7174966582064037e-5</v>
+        <v>2.717496659889663e-5</v>
       </c>
     </row>
     <row r="33" spans="1:25">
@@ -3084,76 +3084,76 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1.0605028727645458</v>
+        <v>1.0605028730372357</v>
       </c>
       <c r="C34">
-        <v>1.060540238036113</v>
+        <v>1.0605402383767157</v>
       </c>
       <c r="D34">
-        <v>1.0605660434700315</v>
+        <v>1.060566043455185</v>
       </c>
       <c r="E34">
-        <v>1.060579028954718</v>
+        <v>1.0605790314098342</v>
       </c>
       <c r="F34">
-        <v>1.0605763443631147</v>
+        <v>1.0605763451670671</v>
       </c>
       <c r="G34">
-        <v>1.06056831341115</v>
+        <v>1.0605683132937054</v>
       </c>
       <c r="H34">
-        <v>1.0605507314387546</v>
+        <v>1.060550731525747</v>
       </c>
       <c r="I34">
-        <v>1.0605362105669152</v>
+        <v>1.0605362107390017</v>
       </c>
       <c r="J34">
-        <v>1.0605119258157452</v>
+        <v>1.0605119260702176</v>
       </c>
       <c r="K34">
-        <v>1.0604813495407832</v>
+        <v>1.0604813497637766</v>
       </c>
       <c r="L34">
-        <v>1.060458825857721</v>
+        <v>1.0604588260478272</v>
       </c>
       <c r="M34">
-        <v>1.0604484132414718</v>
+        <v>1.0604484134510526</v>
       </c>
       <c r="N34">
-        <v>1.0604368764942464</v>
+        <v>1.0604368767465926</v>
       </c>
       <c r="O34">
-        <v>1.0604456176901353</v>
+        <v>1.060445618111326</v>
       </c>
       <c r="P34">
-        <v>1.060443214476612</v>
+        <v>1.0604432151432996</v>
       </c>
       <c r="Q34">
-        <v>1.0604505965083242</v>
+        <v>1.0604505965031616</v>
       </c>
       <c r="R34">
-        <v>1.060428269868049</v>
+        <v>1.0604282698443277</v>
       </c>
       <c r="S34">
-        <v>1.0604079660043875</v>
+        <v>1.0604079657325955</v>
       </c>
       <c r="T34">
-        <v>1.06035404081131</v>
+        <v>1.0603540407219032</v>
       </c>
       <c r="U34">
-        <v>1.0603305953107414</v>
+        <v>1.060330595668978</v>
       </c>
       <c r="V34">
-        <v>1.0603452360907133</v>
+        <v>1.060345236227687</v>
       </c>
       <c r="W34">
-        <v>1.0603669009956453</v>
+        <v>1.0603669008903476</v>
       </c>
       <c r="X34">
-        <v>1.0603839645778044</v>
+        <v>1.0603839654094895</v>
       </c>
       <c r="Y34">
-        <v>1.060457237479622</v>
+        <v>1.0604572368773297</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -3238,76 +3238,76 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1.0603472943574588</v>
+        <v>1.0603472946301489</v>
       </c>
       <c r="C36">
-        <v>1.0603962736687647</v>
+        <v>1.0603962740093673</v>
       </c>
       <c r="D36">
-        <v>1.060430625237463</v>
+        <v>1.0604306252226163</v>
       </c>
       <c r="E36">
-        <v>1.0604493081239388</v>
+        <v>1.0604493105790551</v>
       </c>
       <c r="F36">
-        <v>1.0604453087488261</v>
+        <v>1.060445309552779</v>
       </c>
       <c r="G36">
-        <v>1.060433990834099</v>
+        <v>1.060433990716654</v>
       </c>
       <c r="H36">
-        <v>1.0604096157872847</v>
+        <v>1.0604096158742773</v>
       </c>
       <c r="I36">
-        <v>1.0603898357443542</v>
+        <v>1.060389835916441</v>
       </c>
       <c r="J36">
-        <v>1.0603574430758542</v>
+        <v>1.0603574433303264</v>
       </c>
       <c r="K36">
-        <v>1.0603170057736582</v>
+        <v>1.0603170059966516</v>
       </c>
       <c r="L36">
-        <v>1.0602885654496246</v>
+        <v>1.060288565639731</v>
       </c>
       <c r="M36">
-        <v>1.0602759614801687</v>
+        <v>1.0602759616897495</v>
       </c>
       <c r="N36">
-        <v>1.0602624525128757</v>
+        <v>1.0602624527652216</v>
       </c>
       <c r="O36">
-        <v>1.060274261605694</v>
+        <v>1.0602742620268846</v>
       </c>
       <c r="P36">
-        <v>1.0602716392568272</v>
+        <v>1.0602716399235146</v>
       </c>
       <c r="Q36">
-        <v>1.0602777064761075</v>
+        <v>1.060277706470945</v>
       </c>
       <c r="R36">
-        <v>1.0602472718052063</v>
+        <v>1.0602472717814848</v>
       </c>
       <c r="S36">
-        <v>1.0602206129743739</v>
+        <v>1.060220612702582</v>
       </c>
       <c r="T36">
-        <v>1.060145869636399</v>
+        <v>1.060145869546992</v>
       </c>
       <c r="U36">
-        <v>1.0601114671257494</v>
+        <v>1.0601114674839862</v>
       </c>
       <c r="V36">
-        <v>1.0601326821193706</v>
+        <v>1.0601326822563444</v>
       </c>
       <c r="W36">
-        <v>1.0601650848575772</v>
+        <v>1.0601650847522797</v>
       </c>
       <c r="X36">
-        <v>1.0601977072330675</v>
+        <v>1.060197708064753</v>
       </c>
       <c r="Y36">
-        <v>1.0602994677360722</v>
+        <v>1.0602994671337798</v>
       </c>
     </row>
     <row r="37" spans="1:25">
@@ -3315,76 +3315,76 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1.060423810274293</v>
+        <v>1.060423810536081</v>
       </c>
       <c r="C37">
-        <v>1.0604689736567727</v>
+        <v>1.0604689738309303</v>
       </c>
       <c r="D37">
-        <v>1.0604993191988077</v>
+        <v>1.0604993184950813</v>
       </c>
       <c r="E37">
-        <v>1.0605118309381765</v>
+        <v>1.0605118355848488</v>
       </c>
       <c r="F37">
-        <v>1.060509547911408</v>
+        <v>1.0605095490642267</v>
       </c>
       <c r="G37">
-        <v>1.060501322369437</v>
+        <v>1.0605013215365304</v>
       </c>
       <c r="H37">
-        <v>1.0604805270371935</v>
+        <v>1.0604805267653254</v>
       </c>
       <c r="I37">
-        <v>1.0604627167258271</v>
+        <v>1.0604627167446141</v>
       </c>
       <c r="J37">
-        <v>1.0604331319597247</v>
+        <v>1.0604331322279124</v>
       </c>
       <c r="K37">
-        <v>1.0603957003728486</v>
+        <v>1.0603957006536722</v>
       </c>
       <c r="L37">
-        <v>1.0603688650717629</v>
+        <v>1.0603688653303096</v>
       </c>
       <c r="M37">
-        <v>1.0603567755765797</v>
+        <v>1.060356775883592</v>
       </c>
       <c r="N37">
-        <v>1.0603436656451972</v>
+        <v>1.0603436660559968</v>
       </c>
       <c r="O37">
-        <v>1.0603539676680265</v>
+        <v>1.0603539684290704</v>
       </c>
       <c r="P37">
-        <v>1.0603500643068318</v>
+        <v>1.0603500650982467</v>
       </c>
       <c r="Q37">
-        <v>1.0603605768003972</v>
+        <v>1.0603605767903952</v>
       </c>
       <c r="R37">
-        <v>1.060332245738811</v>
+        <v>1.06033224569179</v>
       </c>
       <c r="S37">
-        <v>1.060307574726369</v>
+        <v>1.0603075741843224</v>
       </c>
       <c r="T37">
-        <v>1.0602529111951373</v>
+        <v>1.0602529111427836</v>
       </c>
       <c r="U37">
-        <v>1.0602292752479283</v>
+        <v>1.060229275792354</v>
       </c>
       <c r="V37">
-        <v>1.060243713725644</v>
+        <v>1.0602437137704437</v>
       </c>
       <c r="W37">
-        <v>1.060266665367841</v>
+        <v>1.0602666654297668</v>
       </c>
       <c r="X37">
-        <v>1.0602707375186733</v>
+        <v>1.0602707390718225</v>
       </c>
       <c r="Y37">
-        <v>1.060351276584935</v>
+        <v>1.060351275328342</v>
       </c>
     </row>
     <row r="38" spans="1:25">
@@ -3392,76 +3392,76 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>1.0601284816511936</v>
+        <v>1.0601284825065753</v>
       </c>
       <c r="C38">
-        <v>1.0602016695331962</v>
+        <v>1.0602016707937043</v>
       </c>
       <c r="D38">
-        <v>1.060252633293587</v>
+        <v>1.06025263422685</v>
       </c>
       <c r="E38">
-        <v>1.060280497012148</v>
+        <v>1.0602804987514334</v>
       </c>
       <c r="F38">
-        <v>1.0602744197709357</v>
+        <v>1.060274420538559</v>
       </c>
       <c r="G38">
-        <v>1.0602576027890407</v>
+        <v>1.0602576033204567</v>
       </c>
       <c r="H38">
-        <v>1.060227628509897</v>
+        <v>1.060227629227281</v>
       </c>
       <c r="I38">
-        <v>1.0602040717282437</v>
+        <v>1.0602040724120882</v>
       </c>
       <c r="J38">
-        <v>1.0601613297485606</v>
+        <v>1.0601613304788526</v>
       </c>
       <c r="K38">
-        <v>1.0601103465528894</v>
+        <v>1.0601103471684774</v>
       </c>
       <c r="L38">
-        <v>1.0600769061108561</v>
+        <v>1.0600769066232703</v>
       </c>
       <c r="M38">
-        <v>1.0600590537514603</v>
+        <v>1.0600590542663735</v>
       </c>
       <c r="N38">
-        <v>1.0600380774649707</v>
+        <v>1.060038077977034</v>
       </c>
       <c r="O38">
-        <v>1.0600543567709606</v>
+        <v>1.0600543574133336</v>
       </c>
       <c r="P38">
-        <v>1.0600490573951393</v>
+        <v>1.0600490596128846</v>
       </c>
       <c r="Q38">
-        <v>1.0600637785412506</v>
+        <v>1.0600637785351545</v>
       </c>
       <c r="R38">
-        <v>1.0600141223255317</v>
+        <v>1.0600141223006367</v>
       </c>
       <c r="S38">
-        <v>1.0599620829185792</v>
+        <v>1.0599620826430394</v>
       </c>
       <c r="T38">
-        <v>1.0598388944155976</v>
+        <v>1.0598388939610974</v>
       </c>
       <c r="U38">
-        <v>1.0597951657256965</v>
+        <v>1.0597951665799918</v>
       </c>
       <c r="V38">
-        <v>1.0598243360774857</v>
+        <v>1.059824336876074</v>
       </c>
       <c r="W38">
-        <v>1.0598585751513645</v>
+        <v>1.059858574259058</v>
       </c>
       <c r="X38">
-        <v>1.059896511695876</v>
+        <v>1.0598965128121056</v>
       </c>
       <c r="Y38">
-        <v>1.0600381885147372</v>
+        <v>1.0600381878582628</v>
       </c>
     </row>
     <row r="39" spans="1:25">
@@ -3469,76 +3469,76 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1.0599262108180594</v>
+        <v>1.0599262116734414</v>
       </c>
       <c r="C39">
-        <v>1.0600144985351339</v>
+        <v>1.060014499795642</v>
       </c>
       <c r="D39">
-        <v>1.0600765734180848</v>
+        <v>1.0600765743513476</v>
       </c>
       <c r="E39">
-        <v>1.0601118445154731</v>
+        <v>1.0601118462547583</v>
       </c>
       <c r="F39">
-        <v>1.0601040578817167</v>
+        <v>1.06010405864934</v>
       </c>
       <c r="G39">
-        <v>1.06008296741171</v>
+        <v>1.060082967943126</v>
       </c>
       <c r="H39">
-        <v>1.060044161226664</v>
+        <v>1.0600441619440482</v>
       </c>
       <c r="I39">
-        <v>1.060013766812197</v>
+        <v>1.0600137674960417</v>
       </c>
       <c r="J39">
-        <v>1.0599604834335676</v>
+        <v>1.0599604841638597</v>
       </c>
       <c r="K39">
-        <v>1.059896679538582</v>
+        <v>1.0598966801541703</v>
       </c>
       <c r="L39">
-        <v>1.059855546635309</v>
+        <v>1.0598555471477231</v>
       </c>
       <c r="M39">
-        <v>1.0598348452082034</v>
+        <v>1.0598348457231166</v>
       </c>
       <c r="N39">
-        <v>1.0598113047570477</v>
+        <v>1.0598113052691107</v>
       </c>
       <c r="O39">
-        <v>1.0598315727619263</v>
+        <v>1.0598315734042996</v>
       </c>
       <c r="P39">
-        <v>1.059825988479269</v>
+        <v>1.0598259906970142</v>
       </c>
       <c r="Q39">
-        <v>1.0598390001840416</v>
+        <v>1.0598390001779454</v>
       </c>
       <c r="R39">
-        <v>1.059778802377587</v>
+        <v>1.0597788023526922</v>
       </c>
       <c r="S39">
-        <v>1.0597185006015661</v>
+        <v>1.0597185003260263</v>
       </c>
       <c r="T39">
-        <v>1.05956824546541</v>
+        <v>1.05956824501091</v>
       </c>
       <c r="U39">
-        <v>1.0595102710241509</v>
+        <v>1.0595102718784462</v>
       </c>
       <c r="V39">
-        <v>1.0595479888396613</v>
+        <v>1.0595479896382498</v>
       </c>
       <c r="W39">
-        <v>1.0595961886878011</v>
+        <v>1.0595961877954947</v>
       </c>
       <c r="X39">
-        <v>1.059654353926741</v>
+        <v>1.0596543550429702</v>
       </c>
       <c r="Y39">
-        <v>1.0598330686418298</v>
+        <v>1.0598330679853554</v>
       </c>
     </row>
     <row r="40" spans="1:25">
@@ -3546,76 +3546,76 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>1.0599728996715523</v>
+        <v>1.059972900526934</v>
       </c>
       <c r="C40">
-        <v>1.0600577021072053</v>
+        <v>1.0600577033677137</v>
       </c>
       <c r="D40">
-        <v>1.0601172123550067</v>
+        <v>1.0601172132882695</v>
       </c>
       <c r="E40">
-        <v>1.060150773698408</v>
+        <v>1.060150775437693</v>
       </c>
       <c r="F40">
-        <v>1.0601433816230665</v>
+        <v>1.06014338239069</v>
       </c>
       <c r="G40">
-        <v>1.060123277549616</v>
+        <v>1.0601232780810323</v>
       </c>
       <c r="H40">
-        <v>1.0600865099197916</v>
+        <v>1.0600865106371753</v>
       </c>
       <c r="I40">
-        <v>1.0600576937437922</v>
+        <v>1.060057694427637</v>
       </c>
       <c r="J40">
-        <v>1.060006843486512</v>
+        <v>1.060006844216804</v>
       </c>
       <c r="K40">
-        <v>1.0599459987992281</v>
+        <v>1.0599459994148162</v>
       </c>
       <c r="L40">
-        <v>1.0599066414237726</v>
+        <v>1.0599066419361867</v>
       </c>
       <c r="M40">
-        <v>1.0598865976001755</v>
+        <v>1.059886598115089</v>
       </c>
       <c r="N40">
-        <v>1.0598636489924633</v>
+        <v>1.0598636495045268</v>
       </c>
       <c r="O40">
-        <v>1.059882996352116</v>
+        <v>1.059882996994489</v>
       </c>
       <c r="P40">
-        <v>1.0598774778298143</v>
+        <v>1.0598774800475594</v>
       </c>
       <c r="Q40">
-        <v>1.059890884096747</v>
+        <v>1.059890884090651</v>
       </c>
       <c r="R40">
-        <v>1.0598331194263602</v>
+        <v>1.0598331194014654</v>
       </c>
       <c r="S40">
-        <v>1.059774724706095</v>
+        <v>1.0597747244305549</v>
       </c>
       <c r="T40">
-        <v>1.059630716840872</v>
+        <v>1.059630716386372</v>
       </c>
       <c r="U40">
-        <v>1.059576030448839</v>
+        <v>1.0595760313031342</v>
       </c>
       <c r="V40">
-        <v>1.0596117754338232</v>
+        <v>1.0596117762324115</v>
       </c>
       <c r="W40">
-        <v>1.0596567529984855</v>
+        <v>1.059656752106179</v>
       </c>
       <c r="X40">
-        <v>1.059710249228439</v>
+        <v>1.0597102503446683</v>
       </c>
       <c r="Y40">
-        <v>1.0598804150966872</v>
+        <v>1.0598804144402125</v>
       </c>
     </row>
     <row r="41" spans="1:25">
@@ -3623,76 +3623,76 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1.0599343352997155</v>
+        <v>1.0599343361550972</v>
       </c>
       <c r="C41">
-        <v>1.0600220165227399</v>
+        <v>1.060022017783248</v>
       </c>
       <c r="D41">
-        <v>1.060083645119542</v>
+        <v>1.0600836460528047</v>
       </c>
       <c r="E41">
-        <v>1.0601186186937386</v>
+        <v>1.0601186204330237</v>
       </c>
       <c r="F41">
-        <v>1.0601109007191156</v>
+        <v>1.0601109014867391</v>
       </c>
       <c r="G41">
-        <v>1.0600899818971126</v>
+        <v>1.0600899824285288</v>
       </c>
       <c r="H41">
-        <v>1.0600515304520375</v>
+        <v>1.0600515311694212</v>
       </c>
       <c r="I41">
-        <v>1.0600214106756747</v>
+        <v>1.0600214113595194</v>
       </c>
       <c r="J41">
-        <v>1.0599685506986685</v>
+        <v>1.0599685514289605</v>
       </c>
       <c r="K41">
-        <v>1.0599052617535822</v>
+        <v>1.0599052623691703</v>
       </c>
       <c r="L41">
-        <v>1.0598644378212927</v>
+        <v>1.0598644383337068</v>
       </c>
       <c r="M41">
-        <v>1.059843850828085</v>
+        <v>1.0598438513429982</v>
       </c>
       <c r="N41">
-        <v>1.0598204133675304</v>
+        <v>1.059820413879594</v>
       </c>
       <c r="O41">
-        <v>1.0598405211648498</v>
+        <v>1.0598405218072229</v>
       </c>
       <c r="P41">
-        <v>1.0598349483255836</v>
+        <v>1.0598349505433287</v>
       </c>
       <c r="Q41">
-        <v>1.059848028690713</v>
+        <v>1.059848028684617</v>
       </c>
       <c r="R41">
-        <v>1.0597882542906882</v>
+        <v>1.0597882542657935</v>
       </c>
       <c r="S41">
-        <v>1.059728284374794</v>
+        <v>1.0597282840992541</v>
       </c>
       <c r="T41">
-        <v>1.059579116372949</v>
+        <v>1.0595791159184489</v>
       </c>
       <c r="U41">
-        <v>1.0595217141115278</v>
+        <v>1.059521714965823</v>
       </c>
       <c r="V41">
-        <v>1.0595590886188118</v>
+        <v>1.0595590894174</v>
       </c>
       <c r="W41">
-        <v>1.0596067277322667</v>
+        <v>1.05960672683996</v>
       </c>
       <c r="X41">
-        <v>1.0596640804826682</v>
+        <v>1.0596640815988978</v>
       </c>
       <c r="Y41">
-        <v>1.0598413075566833</v>
+        <v>1.0598413069002088</v>
       </c>
     </row>
     <row r="42" spans="1:25">
@@ -3700,76 +3700,76 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>1.0607222448463631</v>
+        <v>1.0607222457289525</v>
       </c>
       <c r="C42">
-        <v>1.0607379063776983</v>
+        <v>1.0607379075698296</v>
       </c>
       <c r="D42">
-        <v>1.0607492932723601</v>
+        <v>1.0607492947225658</v>
       </c>
       <c r="E42">
-        <v>1.0607568025395597</v>
+        <v>1.0607568041672972</v>
       </c>
       <c r="F42">
-        <v>1.0607550761339606</v>
+        <v>1.0607550777207981</v>
       </c>
       <c r="G42">
-        <v>1.0607507429225123</v>
+        <v>1.060750744219498</v>
       </c>
       <c r="H42">
-        <v>1.0607451566442598</v>
+        <v>1.0607451578931633</v>
       </c>
       <c r="I42">
-        <v>1.0607412784539902</v>
+        <v>1.060741279505374</v>
       </c>
       <c r="J42">
-        <v>1.0607331949672634</v>
+        <v>1.0607331957589472</v>
       </c>
       <c r="K42">
-        <v>1.0607245002842964</v>
+        <v>1.0607245007574342</v>
       </c>
       <c r="L42">
-        <v>1.0607203200535054</v>
+        <v>1.0607203202555704</v>
       </c>
       <c r="M42">
-        <v>1.0607173506956726</v>
+        <v>1.0607173508288503</v>
       </c>
       <c r="N42">
-        <v>1.0607136140746574</v>
+        <v>1.0607136141573499</v>
       </c>
       <c r="O42">
-        <v>1.0607178756853248</v>
+        <v>1.060717875775743</v>
       </c>
       <c r="P42">
-        <v>1.0607177348354515</v>
+        <v>1.0607177349292118</v>
       </c>
       <c r="Q42">
-        <v>1.0607181936330998</v>
+        <v>1.0607181936340577</v>
       </c>
       <c r="R42">
-        <v>1.0607062208604252</v>
+        <v>1.060706220861715</v>
       </c>
       <c r="S42">
-        <v>1.060692258065844</v>
+        <v>1.0606922580676474</v>
       </c>
       <c r="T42">
-        <v>1.060654745320064</v>
+        <v>1.060654745320762</v>
       </c>
       <c r="U42">
-        <v>1.0606359916955415</v>
+        <v>1.0606359916959331</v>
       </c>
       <c r="V42">
-        <v>1.06064519343562</v>
+        <v>1.0606451934361796</v>
       </c>
       <c r="W42">
-        <v>1.060660219395704</v>
+        <v>1.0606602193967432</v>
       </c>
       <c r="X42">
-        <v>1.0606802286687944</v>
+        <v>1.0606802290264976</v>
       </c>
       <c r="Y42">
-        <v>1.0607192704241664</v>
+        <v>1.0607192712551747</v>
       </c>
     </row>
     <row r="43" spans="1:25">
@@ -3777,76 +3777,76 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.005543210776890797</v>
+        <v>0.005543216553314499</v>
       </c>
       <c r="C43">
-        <v>0.005528793318808333</v>
+        <v>0.005528807440765452</v>
       </c>
       <c r="D43">
-        <v>0.00551223525026349</v>
+        <v>0.005512262435480395</v>
       </c>
       <c r="E43">
-        <v>0.005496364442194605</v>
+        <v>0.005496405953073223</v>
       </c>
       <c r="F43">
-        <v>0.005500480419877007</v>
+        <v>0.005500518142537831</v>
       </c>
       <c r="G43">
-        <v>0.005509552923144533</v>
+        <v>0.005509582479480846</v>
       </c>
       <c r="H43">
-        <v>0.005504984573985944</v>
+        <v>0.0055050018750782154</v>
       </c>
       <c r="I43">
-        <v>0.005455431218230066</v>
+        <v>0.005455442145396013</v>
       </c>
       <c r="J43">
-        <v>0.005366501852585875</v>
+        <v>0.005366507216649406</v>
       </c>
       <c r="K43">
-        <v>0.005045673986312808</v>
+        <v>0.005045675942986834</v>
       </c>
       <c r="L43">
-        <v>0.004137585054974901</v>
+        <v>0.004137585714209737</v>
       </c>
       <c r="M43">
-        <v>0.0036706545250408014</v>
+        <v>0.0036706549468966715</v>
       </c>
       <c r="N43">
-        <v>0.003065151000802855</v>
+        <v>0.003065151266152246</v>
       </c>
       <c r="O43">
-        <v>0.0030642865598931464</v>
+        <v>0.0030642868745466107</v>
       </c>
       <c r="P43">
-        <v>0.0031333076745185665</v>
+        <v>0.003133308000359347</v>
       </c>
       <c r="Q43">
-        <v>0.0036979248249435237</v>
+        <v>0.0036979248251107497</v>
       </c>
       <c r="R43">
-        <v>0.004542036341097894</v>
+        <v>0.004542036341281064</v>
       </c>
       <c r="S43">
-        <v>0.0052729240544352254</v>
+        <v>0.005272924054666326</v>
       </c>
       <c r="T43">
-        <v>0.00557449434053528</v>
+        <v>0.005574494340602924</v>
       </c>
       <c r="U43">
-        <v>0.005594379986954245</v>
+        <v>0.005594379986972916</v>
       </c>
       <c r="V43">
-        <v>0.005594136186696152</v>
+        <v>0.005594136186732594</v>
       </c>
       <c r="W43">
-        <v>0.005593671735475404</v>
+        <v>0.00559367173559034</v>
       </c>
       <c r="X43">
-        <v>0.005562557807680728</v>
+        <v>0.0055625584721906455</v>
       </c>
       <c r="Y43">
-        <v>0.005545295303669473</v>
+        <v>0.005545300320597284</v>
       </c>
     </row>
     <row r="44" spans="1:25">
@@ -3854,76 +3854,76 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.0026016441437480215</v>
+        <v>0.0026017010927289514</v>
       </c>
       <c r="C44">
-        <v>0.0025617637176387847</v>
+        <v>0.0025618406400523108</v>
       </c>
       <c r="D44">
-        <v>0.002523542803536603</v>
+        <v>0.0025236363785130144</v>
       </c>
       <c r="E44">
-        <v>0.0024927739771608195</v>
+        <v>0.0024928790075913667</v>
       </c>
       <c r="F44">
-        <v>0.0025002938502168407</v>
+        <v>0.0025003962415209484</v>
       </c>
       <c r="G44">
-        <v>0.002517984341705698</v>
+        <v>0.0025180680301331035</v>
       </c>
       <c r="H44">
-        <v>0.002541691325596948</v>
+        <v>0.0025417719113235257</v>
       </c>
       <c r="I44">
-        <v>0.00253687726211243</v>
+        <v>0.002536945102686897</v>
       </c>
       <c r="J44">
-        <v>0.0025183714213022263</v>
+        <v>0.0025184225045824372</v>
       </c>
       <c r="K44">
-        <v>0.0023887459559205747</v>
+        <v>0.002388776484903209</v>
       </c>
       <c r="L44">
-        <v>0.0019634291541221417</v>
+        <v>0.0019634421921592114</v>
       </c>
       <c r="M44">
-        <v>0.0017397926084973497</v>
+        <v>0.0017398012016090782</v>
       </c>
       <c r="N44">
-        <v>0.0014468326266921052</v>
+        <v>0.0014468379622950183</v>
       </c>
       <c r="O44">
-        <v>0.001444338165312825</v>
+        <v>0.001444343999415315</v>
       </c>
       <c r="P44">
-        <v>0.0014780923277709155</v>
+        <v>0.0014780983775084576</v>
       </c>
       <c r="Q44">
-        <v>0.0018338195325004942</v>
+        <v>0.0018338195943112803</v>
       </c>
       <c r="R44">
-        <v>0.002255080902844892</v>
+        <v>0.00225508098608369</v>
       </c>
       <c r="S44">
-        <v>0.002619639769081388</v>
+        <v>0.0026196398854511265</v>
       </c>
       <c r="T44">
-        <v>0.002772802323601228</v>
+        <v>0.00277280236863084</v>
       </c>
       <c r="U44">
-        <v>0.002784007871436627</v>
+        <v>0.002784007896708614</v>
       </c>
       <c r="V44">
-        <v>0.002783132504799323</v>
+        <v>0.002783132540902331</v>
       </c>
       <c r="W44">
-        <v>0.0027814799559348203</v>
+        <v>0.0027814800229760015</v>
       </c>
       <c r="X44">
-        <v>0.0026653417813121525</v>
+        <v>0.002665364861816037</v>
       </c>
       <c r="Y44">
-        <v>0.002607916897365172</v>
+        <v>0.002607970518052215</v>
       </c>
     </row>
     <row r="45" spans="1:25">
@@ -3931,76 +3931,76 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.0030174879189325586</v>
+        <v>0.0030174922071637034</v>
       </c>
       <c r="C45">
-        <v>0.003003582579134008</v>
+        <v>0.003003591107617607</v>
       </c>
       <c r="D45">
-        <v>0.002989646275149049</v>
+        <v>0.0029896603722338764</v>
       </c>
       <c r="E45">
-        <v>0.0029778986933167925</v>
+        <v>0.0029779178788118094</v>
       </c>
       <c r="F45">
-        <v>0.002980812056655238</v>
+        <v>0.002980830050830264</v>
       </c>
       <c r="G45">
-        <v>0.0029875638904322123</v>
+        <v>0.002987578957743676</v>
       </c>
       <c r="H45">
-        <v>0.0029995431870453683</v>
+        <v>0.002999553263625042</v>
       </c>
       <c r="I45">
-        <v>0.003007477374696653</v>
+        <v>0.0030074845759068473</v>
       </c>
       <c r="J45">
-        <v>0.003017441082954534</v>
+        <v>0.0030174453564807808</v>
       </c>
       <c r="K45">
-        <v>0.0030277810960222537</v>
+        <v>0.003027783215366385</v>
       </c>
       <c r="L45">
-        <v>0.0030353704909244976</v>
+        <v>0.0030353715697464248</v>
       </c>
       <c r="M45">
-        <v>0.0030381763665317287</v>
+        <v>0.0030381771782676207</v>
       </c>
       <c r="N45">
-        <v>0.0030410211942402576</v>
+        <v>0.003041021785059303</v>
       </c>
       <c r="O45">
-        <v>0.0030394981274838007</v>
+        <v>0.003039498823799456</v>
       </c>
       <c r="P45">
-        <v>0.0030394022833947717</v>
+        <v>0.0030394030221926214</v>
       </c>
       <c r="Q45">
-        <v>0.0030856533793237567</v>
+        <v>0.003085653379914206</v>
       </c>
       <c r="R45">
-        <v>0.00308591350749978</v>
+        <v>0.003085913508015535</v>
       </c>
       <c r="S45">
-        <v>0.003086075372641988</v>
+        <v>0.0030860753731277372</v>
       </c>
       <c r="T45">
-        <v>0.0030873545220929375</v>
+        <v>0.0030873545222573633</v>
       </c>
       <c r="U45">
-        <v>0.0030879273343879005</v>
+        <v>0.003087927334559311</v>
       </c>
       <c r="V45">
-        <v>0.003087591045676653</v>
+        <v>0.0030875910457778158</v>
       </c>
       <c r="W45">
-        <v>0.003086964467585218</v>
+        <v>0.0030869644678386235</v>
       </c>
       <c r="X45">
-        <v>0.0030395568829671912</v>
+        <v>0.0030395578372533188</v>
       </c>
       <c r="Y45">
-        <v>0.0030197085863435803</v>
+        <v>0.0030197131883690255</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -4008,76 +4008,76 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.0014927786303834654</v>
+        <v>0.0014927860085135823</v>
       </c>
       <c r="C46">
-        <v>0.001478360620368579</v>
+        <v>0.0014783768281015745</v>
       </c>
       <c r="D46">
-        <v>0.001461863450325579</v>
+        <v>0.0014618919373217524</v>
       </c>
       <c r="E46">
-        <v>0.0014462028851444043</v>
+        <v>0.0014462434033654418</v>
       </c>
       <c r="F46">
-        <v>0.0014502465267364683</v>
+        <v>0.0014502839836385798</v>
       </c>
       <c r="G46">
-        <v>0.0014592040322579378</v>
+        <v>0.0014592345931364668</v>
       </c>
       <c r="H46">
-        <v>0.0014740190020067132</v>
+        <v>0.0014740383364800105</v>
       </c>
       <c r="I46">
-        <v>0.001483292013207172</v>
+        <v>0.0014833049320844389</v>
       </c>
       <c r="J46">
-        <v>0.00149383993165437</v>
+        <v>0.0014938467847597846</v>
       </c>
       <c r="K46">
-        <v>0.0015043457879751882</v>
+        <v>0.001504348519993441</v>
       </c>
       <c r="L46">
-        <v>0.0015126984257843807</v>
+        <v>0.0015126993733219356</v>
       </c>
       <c r="M46">
-        <v>0.0015155590153404395</v>
+        <v>0.001515559611580973</v>
       </c>
       <c r="N46">
-        <v>0.0015183989102339009</v>
+        <v>0.0015183992600645562</v>
       </c>
       <c r="O46">
-        <v>0.0015175403256076885</v>
+        <v>0.0015175407316653205</v>
       </c>
       <c r="P46">
-        <v>0.0015173556165918466</v>
+        <v>0.0015173560436266107</v>
       </c>
       <c r="Q46">
-        <v>0.0015426728392106505</v>
+        <v>0.001542672839722055</v>
       </c>
       <c r="R46">
-        <v>0.0015425442306110833</v>
+        <v>0.0015425442312401883</v>
       </c>
       <c r="S46">
-        <v>0.0015423889457866291</v>
+        <v>0.001542388946587051</v>
       </c>
       <c r="T46">
-        <v>0.0015432415725084823</v>
+        <v>0.001543241572782907</v>
       </c>
       <c r="U46">
-        <v>0.0015436529358035004</v>
+        <v>0.0015436529359410041</v>
       </c>
       <c r="V46">
-        <v>0.0015434096230811118</v>
+        <v>0.0015434096232845697</v>
       </c>
       <c r="W46">
-        <v>0.0015429461708321905</v>
+        <v>0.0015429461712493213</v>
       </c>
       <c r="X46">
-        <v>0.0015120512625961691</v>
+        <v>0.0015120523603006672</v>
       </c>
       <c r="Y46">
-        <v>0.0014948633037233103</v>
+        <v>0.0014948697809265366</v>
       </c>
     </row>
     <row r="47" spans="1:25">
@@ -4085,76 +4085,76 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.00012981853758627153</v>
+        <v>0.00012983018686528838</v>
       </c>
       <c r="C47">
-        <v>0.00023823768274234617</v>
+        <v>0.00023828378637001868</v>
       </c>
       <c r="D47">
-        <v>0.0005090183440607347</v>
+        <v>0.0005091624297957389</v>
       </c>
       <c r="E47">
-        <v>0.0012646997751756092</v>
+        <v>0.0012643768481853815</v>
       </c>
       <c r="F47">
-        <v>0.001042288249571784</v>
+        <v>0.0010422683041951776</v>
       </c>
       <c r="G47">
-        <v>0.000683818549014621</v>
+        <v>0.0006839690249447176</v>
       </c>
       <c r="H47">
-        <v>0.0004048846666420185</v>
+        <v>0.00040496582868916836</v>
       </c>
       <c r="I47">
-        <v>0.0003190665951533705</v>
+        <v>0.0003191078044299155</v>
       </c>
       <c r="J47">
-        <v>0.00022004256108342437</v>
+        <v>0.00022005009966164895</v>
       </c>
       <c r="K47">
-        <v>0.00016381204308991707</v>
+        <v>0.00016380786328421484</v>
       </c>
       <c r="L47">
-        <v>0.00016579303486539124</v>
+        <v>0.00016578496791926282</v>
       </c>
       <c r="M47">
-        <v>0.00017977230876654396</v>
+        <v>0.00017975889031541484</v>
       </c>
       <c r="N47">
-        <v>0.00020361319602732282</v>
+        <v>0.00020358921164747491</v>
       </c>
       <c r="O47">
-        <v>0.00031936741691695027</v>
+        <v>0.00031931358254061893</v>
       </c>
       <c r="P47">
-        <v>0.0005408363581319854</v>
+        <v>0.0005408182660333865</v>
       </c>
       <c r="Q47">
-        <v>-7.079116357049724e-10</v>
+        <v>-6.771580456699149e-10</v>
       </c>
       <c r="R47">
-        <v>-7.081657078374095e-10</v>
+        <v>-6.774137987908786e-10</v>
       </c>
       <c r="S47">
-        <v>-7.091683579402634e-10</v>
+        <v>-6.784231358565317e-10</v>
       </c>
       <c r="T47">
-        <v>-7.10133673187664e-10</v>
+        <v>-6.7939482077493e-10</v>
       </c>
       <c r="U47">
-        <v>-7.10226132133917e-10</v>
+        <v>-6.794878458401783e-10</v>
       </c>
       <c r="V47">
-        <v>-7.10152049243446e-10</v>
+        <v>-6.794133167869289e-10</v>
       </c>
       <c r="W47">
-        <v>-7.101119880706228e-10</v>
+        <v>-6.79372990417206e-10</v>
       </c>
       <c r="X47">
-        <v>0.0020617346276837955</v>
+        <v>0.0020616180771177986</v>
       </c>
       <c r="Y47">
-        <v>0.004322735264989018</v>
+        <v>0.004322854184342137</v>
       </c>
     </row>
     <row r="48" spans="1:25">
@@ -4162,76 +4162,76 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>6.824662744294638e-5</v>
+        <v>6.822762919308896e-5</v>
       </c>
       <c r="C48">
-        <v>0.00011518941916943798</v>
+        <v>0.00011516849788980254</v>
       </c>
       <c r="D48">
-        <v>0.00020658800432837848</v>
+        <v>0.00020659115333743476</v>
       </c>
       <c r="E48">
-        <v>0.00036645711237990393</v>
+        <v>0.000366582366238957</v>
       </c>
       <c r="F48">
-        <v>0.00032812204090671527</v>
+        <v>0.0003282013978297207</v>
       </c>
       <c r="G48">
-        <v>0.00024733120547263895</v>
+        <v>0.0002473560148556595</v>
       </c>
       <c r="H48">
-        <v>0.00018900529960125587</v>
+        <v>0.00018900736617214067</v>
       </c>
       <c r="I48">
-        <v>0.00016832550428322074</v>
+        <v>0.00016832140791249307</v>
       </c>
       <c r="J48">
-        <v>0.0001267187497684535</v>
+        <v>0.00012670492654660588</v>
       </c>
       <c r="K48">
-        <v>0.00010683055121581624</v>
+        <v>0.00010681386802764581</v>
       </c>
       <c r="L48">
-        <v>0.00013526747569332187</v>
+        <v>0.00013525169731714857</v>
       </c>
       <c r="M48">
-        <v>0.00015603049046993909</v>
+        <v>0.00015601508831361636</v>
       </c>
       <c r="N48">
-        <v>0.0001911153347776507</v>
+        <v>0.00019110213895604764</v>
       </c>
       <c r="O48">
-        <v>0.00031982317202793335</v>
+        <v>0.00031981229191020244</v>
       </c>
       <c r="P48">
-        <v>0.0004687919235271169</v>
+        <v>0.00046870483879821233</v>
       </c>
       <c r="Q48">
-        <v>-7.06473685436807e-10</v>
+        <v>-6.757105596923211e-10</v>
       </c>
       <c r="R48">
-        <v>-7.059882459249698e-10</v>
+        <v>-6.752218753197872e-10</v>
       </c>
       <c r="S48">
-        <v>-7.082365244264584e-10</v>
+        <v>-6.774850760984306e-10</v>
       </c>
       <c r="T48">
-        <v>-7.132287166269217e-10</v>
+        <v>-6.8251038533918e-10</v>
       </c>
       <c r="U48">
-        <v>-7.144215233119321e-10</v>
+        <v>-6.83710996895012e-10</v>
       </c>
       <c r="V48">
-        <v>-7.134417106642613e-10</v>
+        <v>-6.827246971608536e-10</v>
       </c>
       <c r="W48">
-        <v>-7.131511444201628e-10</v>
+        <v>-6.824323286948852e-10</v>
       </c>
       <c r="X48">
-        <v>0.0009626754289723141</v>
+        <v>0.0009626619728130728</v>
       </c>
       <c r="Y48">
-        <v>0.002230568094978152</v>
+        <v>0.0022305839176888754</v>
       </c>
     </row>
     <row r="49" spans="1:25">
@@ -4239,76 +4239,76 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>4.1622300364282556e-8</v>
+        <v>4.269226637103986e-8</v>
       </c>
       <c r="C49">
-        <v>4.161257921783042e-8</v>
+        <v>4.268213827935467e-8</v>
       </c>
       <c r="D49">
-        <v>4.1606589688943275e-8</v>
+        <v>4.267589850055653e-8</v>
       </c>
       <c r="E49">
-        <v>4.160592413388896e-8</v>
+        <v>4.2675202512299345e-8</v>
       </c>
       <c r="F49">
-        <v>4.160536904972141e-8</v>
+        <v>4.2674626064195624e-8</v>
       </c>
       <c r="G49">
-        <v>4.160542103864314e-8</v>
+        <v>4.2674681464355496e-8</v>
       </c>
       <c r="H49">
-        <v>4.160759456746238e-8</v>
+        <v>4.267694590282668e-8</v>
       </c>
       <c r="I49">
-        <v>4.160930864668436e-8</v>
+        <v>4.267873180445659e-8</v>
       </c>
       <c r="J49">
-        <v>4.1613189219301695e-8</v>
+        <v>4.268277492845827e-8</v>
       </c>
       <c r="K49">
-        <v>4.1617436166152846e-8</v>
+        <v>4.268719991404678e-8</v>
       </c>
       <c r="L49">
-        <v>4.161710135632503e-8</v>
+        <v>4.268685131839362e-8</v>
       </c>
       <c r="M49">
-        <v>4.161564760438237e-8</v>
+        <v>4.268533690506981e-8</v>
       </c>
       <c r="N49">
-        <v>4.1613640217324205e-8</v>
+        <v>4.26832456446966e-8</v>
       </c>
       <c r="O49">
-        <v>4.16083645865332e-8</v>
+        <v>4.267774918244502e-8</v>
       </c>
       <c r="P49">
-        <v>4.1604462458155795e-8</v>
+        <v>4.267368405147144e-8</v>
       </c>
       <c r="Q49">
-        <v>4.524253930144871e-5</v>
+        <v>4.524176675725393e-5</v>
       </c>
       <c r="R49">
-        <v>4.737933883479786e-5</v>
+        <v>4.7375506925532515e-5</v>
       </c>
       <c r="S49">
-        <v>0.0001053315030875088</v>
+        <v>0.00010528674161622821</v>
       </c>
       <c r="T49">
-        <v>0.002542366061699555</v>
+        <v>0.002542372233333681</v>
       </c>
       <c r="U49">
-        <v>0.003858073943127054</v>
+        <v>0.003858104833138854</v>
       </c>
       <c r="V49">
-        <v>0.0030161643477410035</v>
+        <v>0.0030161491012373307</v>
       </c>
       <c r="W49">
-        <v>0.0019092395751661394</v>
+        <v>0.001909267321131283</v>
       </c>
       <c r="X49">
-        <v>4.159574524119571e-8</v>
+        <v>4.2664601962952106e-8</v>
       </c>
       <c r="Y49">
-        <v>4.158705142284249e-8</v>
+        <v>4.26555452847922e-8</v>
       </c>
     </row>
     <row r="50" spans="1:25">
@@ -4316,76 +4316,76 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>4.163255234254027e-8</v>
+        <v>4.2702951790532134e-8</v>
       </c>
       <c r="C50">
-        <v>4.161388074175109e-8</v>
+        <v>4.268349820196073e-8</v>
       </c>
       <c r="D50">
-        <v>4.160118391653171e-8</v>
+        <v>4.267027025965277e-8</v>
       </c>
       <c r="E50">
-        <v>4.159512775979881e-8</v>
+        <v>4.2663960588380516e-8</v>
       </c>
       <c r="F50">
-        <v>4.159582052880555e-8</v>
+        <v>4.2664682677567975e-8</v>
       </c>
       <c r="G50">
-        <v>4.159870859292707e-8</v>
+        <v>4.266769149889071e-8</v>
       </c>
       <c r="H50">
-        <v>4.1602801001111186e-8</v>
+        <v>4.267195477853231e-8</v>
       </c>
       <c r="I50">
-        <v>4.160501277984887e-8</v>
+        <v>4.267425896729984e-8</v>
       </c>
       <c r="J50">
-        <v>4.1611495681069994e-8</v>
+        <v>4.268101310475547e-8</v>
       </c>
       <c r="K50">
-        <v>4.161620197803105e-8</v>
+        <v>4.2685916399865615e-8</v>
       </c>
       <c r="L50">
-        <v>4.160994437817766e-8</v>
+        <v>4.2679396720382564e-8</v>
       </c>
       <c r="M50">
-        <v>4.1606804594095417e-8</v>
+        <v>4.2676125406873336e-8</v>
       </c>
       <c r="N50">
-        <v>4.1603038904312827e-8</v>
+        <v>4.267220198342294e-8</v>
       </c>
       <c r="O50">
-        <v>4.159614030375238e-8</v>
+        <v>4.266501445491234e-8</v>
       </c>
       <c r="P50">
-        <v>4.159291277607296e-8</v>
+        <v>4.2661651109941746e-8</v>
       </c>
       <c r="Q50">
-        <v>1.4945373287842826e-5</v>
+        <v>1.4945349843162398e-5</v>
       </c>
       <c r="R50">
-        <v>1.264804682445932e-5</v>
+        <v>1.2648009500593276e-5</v>
       </c>
       <c r="S50">
-        <v>1.773479655090394e-5</v>
+        <v>1.7734611405127522e-5</v>
       </c>
       <c r="T50">
-        <v>0.0009580868125407241</v>
+        <v>0.0009580659159978454</v>
       </c>
       <c r="U50">
-        <v>0.0022506584248045075</v>
+        <v>0.0022506868890342017</v>
       </c>
       <c r="V50">
-        <v>0.0018784462358369493</v>
+        <v>0.0018784841898270216</v>
       </c>
       <c r="W50">
-        <v>0.0006311141115969499</v>
+        <v>0.0006310690309623485</v>
       </c>
       <c r="X50">
-        <v>4.158010811305259e-8</v>
+        <v>4.2648309656933967e-8</v>
       </c>
       <c r="Y50">
-        <v>4.1554539735841555e-8</v>
+        <v>4.262167143705247e-8</v>
       </c>
     </row>
     <row r="51" spans="1:25">
@@ -4393,73 +4393,73 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.011787033797759206</v>
+        <v>0.011787043738294265</v>
       </c>
       <c r="C51">
-        <v>0.01201331579364947</v>
+        <v>0.012013368406779173</v>
       </c>
       <c r="D51">
-        <v>0.01249683942409697</v>
+        <v>0.012497027793086703</v>
       </c>
       <c r="E51">
-        <v>0.013698260414804183</v>
+        <v>0.013698140877597013</v>
       </c>
       <c r="F51">
-        <v>0.014688390456772062</v>
+        <v>0.014688250845923416</v>
       </c>
       <c r="G51">
-        <v>0.015337974283155913</v>
+        <v>0.015337976498903567</v>
       </c>
       <c r="H51">
-        <v>0.015722570918997866</v>
+        <v>0.015722649113057326</v>
       </c>
       <c r="I51">
-        <v>0.016025640385121307</v>
+        <v>0.0160257566022849</v>
       </c>
       <c r="J51">
-        <v>0.016234637014793486</v>
+        <v>0.0162347592677267</v>
       </c>
       <c r="K51">
-        <v>0.016390214647901365</v>
+        <v>0.01639033180395206</v>
       </c>
       <c r="L51">
-        <v>0.016547674223548373</v>
+        <v>0.016547782589947654</v>
       </c>
       <c r="M51">
-        <v>0.016718414110931744</v>
+        <v>0.016718508603813714</v>
       </c>
       <c r="N51">
-        <v>0.016911802843325892</v>
+        <v>0.016911873425146558</v>
       </c>
       <c r="O51">
-        <v>0.017215158091118482</v>
+        <v>0.01721517640461364</v>
       </c>
       <c r="P51">
-        <v>0.01772890883717286</v>
+        <v>0.017728908837677932</v>
       </c>
       <c r="Q51">
-        <v>0.017681284439076336</v>
+        <v>0.017681285282001732</v>
       </c>
       <c r="R51">
-        <v>0.017631410778071756</v>
+        <v>0.017631415683800167</v>
       </c>
       <c r="S51">
-        <v>0.017520534837953915</v>
+        <v>0.017520586890228475</v>
       </c>
       <c r="T51">
-        <v>0.014844359361537919</v>
+        <v>0.014844404946557416</v>
       </c>
       <c r="U51">
-        <v>0.010783228220373565</v>
+        <v>0.010783241318792538</v>
       </c>
       <c r="V51">
-        <v>0.007608317706001746</v>
+        <v>0.00760834688257375</v>
       </c>
       <c r="W51">
-        <v>0.0055985911627994215</v>
+        <v>0.005598591162294375</v>
       </c>
       <c r="X51">
-        <v>0.007557195274104036</v>
+        <v>0.007557083425448954</v>
       </c>
       <c r="Y51">
         <v>0.01166375</v>
@@ -4470,73 +4470,73 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.0058984154723314905</v>
+        <v>0.005898396297257864</v>
       </c>
       <c r="C52">
-        <v>0.006007801616457465</v>
+        <v>0.00600776144025507</v>
       </c>
       <c r="D52">
-        <v>0.0062040164298495125</v>
+        <v>0.006203978119851675</v>
       </c>
       <c r="E52">
-        <v>0.00655210690226541</v>
+        <v>0.0065521864583464855</v>
       </c>
       <c r="F52">
-        <v>0.006863779056052549</v>
+        <v>0.006863932876092428</v>
       </c>
       <c r="G52">
-        <v>0.007098699913137248</v>
+        <v>0.007098876176845833</v>
       </c>
       <c r="H52">
-        <v>0.0072782111553363355</v>
+        <v>0.007278388256862231</v>
       </c>
       <c r="I52">
-        <v>0.0074380765896551</v>
+        <v>0.007438248674106502</v>
       </c>
       <c r="J52">
-        <v>0.00755841560036073</v>
+        <v>0.007558573426943562</v>
       </c>
       <c r="K52">
-        <v>0.007659860817487357</v>
+        <v>0.007660001669026247</v>
       </c>
       <c r="L52">
-        <v>0.0077883211194545625</v>
+        <v>0.0077884458557967795</v>
       </c>
       <c r="M52">
-        <v>0.00793650628876459</v>
+        <v>0.007936615267457444</v>
       </c>
       <c r="N52">
-        <v>0.008118022064130826</v>
+        <v>0.008118117381358338</v>
       </c>
       <c r="O52">
-        <v>0.008421810292146519</v>
+        <v>0.0084218941481315</v>
       </c>
       <c r="P52">
-        <v>0.00886711883748383</v>
+        <v>0.008867118837988632</v>
       </c>
       <c r="Q52">
-        <v>0.008851386194451891</v>
+        <v>0.008851386248860272</v>
       </c>
       <c r="R52">
-        <v>0.008838071790263625</v>
+        <v>0.00883807191318834</v>
       </c>
       <c r="S52">
-        <v>0.008819402910543239</v>
+        <v>0.00881940325757212</v>
       </c>
       <c r="T52">
-        <v>0.007810889798722564</v>
+        <v>0.007810912171294786</v>
       </c>
       <c r="U52">
-        <v>0.005441774988648952</v>
+        <v>0.005441767428049127</v>
       </c>
       <c r="V52">
-        <v>0.0034644624836825373</v>
+        <v>0.0034644150006953793</v>
       </c>
       <c r="W52">
-        <v>0.002800131162402687</v>
+        <v>0.0028001311618979846</v>
       </c>
       <c r="X52">
-        <v>0.0037146290513915296</v>
+        <v>0.0037146151431128697</v>
       </c>
       <c r="Y52">
         <v>0.005833624999999999</v>

</xml_diff>

<commit_message>
all seems to work well
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -854,7 +854,7 @@
         <v>0.06173114629133221</v>
       </c>
       <c r="C5">
-        <v>0.0572924580189984</v>
+        <v>0.05729245801899839</v>
       </c>
       <c r="D5">
         <v>0.05427437097296479</v>
@@ -863,10 +863,10 @@
         <v>0.05293621220309018</v>
       </c>
       <c r="F5">
-        <v>0.053195715829821244</v>
+        <v>0.05319571582982124</v>
       </c>
       <c r="G5">
-        <v>0.05405661479838581</v>
+        <v>0.05405661479838582</v>
       </c>
       <c r="H5">
         <v>0.055706056954738334</v>
@@ -902,7 +902,7 @@
         <v>0.06662726716583452</v>
       </c>
       <c r="S5">
-        <v>0.07117868709503243</v>
+        <v>0.07117868709503244</v>
       </c>
       <c r="T5">
         <v>0.07813610371844927</v>
@@ -917,7 +917,7 @@
         <v>0.07728283375464502</v>
       </c>
       <c r="X5">
-        <v>0.07669483002782823</v>
+        <v>0.07669483002782822</v>
       </c>
       <c r="Y5">
         <v>0.06895605111911352</v>
@@ -928,7 +928,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.042801443560451874</v>
+        <v>0.04280144356045187</v>
       </c>
       <c r="C6">
         <v>0.03977589808733105</v>
@@ -940,13 +940,13 @@
         <v>0.03715273330417834</v>
       </c>
       <c r="F6">
-        <v>0.03725226107653093</v>
+        <v>0.03725226107653092</v>
       </c>
       <c r="G6">
         <v>0.03771321964849193</v>
       </c>
       <c r="H6">
-        <v>0.03876949313869838</v>
+        <v>0.03876949313869839</v>
       </c>
       <c r="I6">
         <v>0.039636547458981444</v>
@@ -979,7 +979,7 @@
         <v>0.04623827257424411</v>
       </c>
       <c r="S6">
-        <v>0.049316313859699375</v>
+        <v>0.04931631385969938</v>
       </c>
       <c r="T6">
         <v>0.053040488551201796</v>
@@ -994,7 +994,7 @@
         <v>0.0527270916587816</v>
       </c>
       <c r="X6">
-        <v>0.05403223133659517</v>
+        <v>0.05403223133659516</v>
       </c>
       <c r="Y6">
         <v>0.04975971613656475</v>
@@ -1236,37 +1236,37 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.009594357663375656</v>
+        <v>0.009594357663375654</v>
       </c>
       <c r="C10">
         <v>0.008996286661527035</v>
       </c>
       <c r="D10">
-        <v>0.008747280970884284</v>
+        <v>0.008747280970884286</v>
       </c>
       <c r="E10">
-        <v>0.009155933770505099</v>
+        <v>0.009155933770505097</v>
       </c>
       <c r="F10">
         <v>0.009013798834025439</v>
       </c>
       <c r="G10">
-        <v>0.008855442696598565</v>
+        <v>0.008855442696598567</v>
       </c>
       <c r="H10">
         <v>0.00898967775354143</v>
       </c>
       <c r="I10">
-        <v>0.009223753030530968</v>
+        <v>0.00922375303053097</v>
       </c>
       <c r="J10">
-        <v>0.009617928537382501</v>
+        <v>0.0096179285373825</v>
       </c>
       <c r="K10">
         <v>0.010161569894650538</v>
       </c>
       <c r="L10">
-        <v>0.010523480313139513</v>
+        <v>0.01052348031313951</v>
       </c>
       <c r="M10">
         <v>0.010670763898993851</v>
@@ -1275,7 +1275,7 @@
         <v>0.010814573722841773</v>
       </c>
       <c r="O10">
-        <v>0.010743672538856797</v>
+        <v>0.010743672538856795</v>
       </c>
       <c r="P10">
         <v>0.010978521623073683</v>
@@ -1287,16 +1287,16 @@
         <v>0.01096356239448917</v>
       </c>
       <c r="S10">
-        <v>0.011292244719964172</v>
+        <v>0.01129224471996417</v>
       </c>
       <c r="T10">
-        <v>0.010121448489469284</v>
+        <v>0.010121448489469283</v>
       </c>
       <c r="U10">
         <v>0.009472186158058648</v>
       </c>
       <c r="V10">
-        <v>0.009914262326124119</v>
+        <v>0.00991426232612412</v>
       </c>
       <c r="W10">
         <v>0.010367994305393282</v>
@@ -1331,7 +1331,7 @@
         <v>0.016595154974473503</v>
       </c>
       <c r="H11">
-        <v>0.01689698825103955</v>
+        <v>0.016896988251039552</v>
       </c>
       <c r="I11">
         <v>0.017049786345542276</v>
@@ -1358,13 +1358,13 @@
         <v>0.01673117759331875</v>
       </c>
       <c r="Q11">
-        <v>0.016827441928582803</v>
+        <v>0.016827441928582806</v>
       </c>
       <c r="R11">
         <v>0.018750025284345762</v>
       </c>
       <c r="S11">
-        <v>0.020918594523088863</v>
+        <v>0.020918594523088866</v>
       </c>
       <c r="T11">
         <v>0.02391242140094724</v>
@@ -1373,10 +1373,10 @@
         <v>0.024419953375940565</v>
       </c>
       <c r="V11">
-        <v>0.023991942115673442</v>
+        <v>0.023991942115673445</v>
       </c>
       <c r="W11">
-        <v>0.023932607316467288</v>
+        <v>0.02393260731646729</v>
       </c>
       <c r="X11">
         <v>0.023632787775337945</v>
@@ -1627,7 +1627,7 @@
         <v>0.009712995860138731</v>
       </c>
       <c r="D15">
-        <v>0.008588524844934255</v>
+        <v>0.008588524844934256</v>
       </c>
       <c r="E15">
         <v>0.007851234640988955</v>
@@ -1636,28 +1636,28 @@
         <v>0.008020266865080804</v>
       </c>
       <c r="G15">
-        <v>0.008445862443217898</v>
+        <v>0.0084458624432179</v>
       </c>
       <c r="H15">
         <v>0.009354423186373497</v>
       </c>
       <c r="I15">
-        <v>0.010107414051398823</v>
+        <v>0.010107414051398821</v>
       </c>
       <c r="J15">
-        <v>0.011287067379352377</v>
+        <v>0.011287067379352379</v>
       </c>
       <c r="K15">
-        <v>0.012938446488027345</v>
+        <v>0.012938446488027344</v>
       </c>
       <c r="L15">
-        <v>0.014641028105134794</v>
+        <v>0.014641028105134792</v>
       </c>
       <c r="M15">
         <v>0.015402562944672321</v>
       </c>
       <c r="N15">
-        <v>0.016272673931691625</v>
+        <v>0.01627267393169162</v>
       </c>
       <c r="O15">
         <v>0.01585539775176105</v>
@@ -1666,7 +1666,7 @@
         <v>0.015816977835937163</v>
       </c>
       <c r="Q15">
-        <v>0.015360503554972973</v>
+        <v>0.015360503554972975</v>
       </c>
       <c r="R15">
         <v>0.015628683535162013</v>
@@ -1778,19 +1778,19 @@
         <v>0.002132556301988195</v>
       </c>
       <c r="C17">
-        <v>0.0018189625943495836</v>
+        <v>0.0018189625943495834</v>
       </c>
       <c r="D17">
-        <v>0.0015970837212705756</v>
+        <v>0.0015970837212705754</v>
       </c>
       <c r="E17">
-        <v>0.0014544550401362098</v>
+        <v>0.0014544550401362102</v>
       </c>
       <c r="F17">
-        <v>0.0014869497807992397</v>
+        <v>0.00148694978079924</v>
       </c>
       <c r="G17">
-        <v>0.0015693084307062172</v>
+        <v>0.0015693084306723838</v>
       </c>
       <c r="H17">
         <v>0.0017523077469673253</v>
@@ -1805,13 +1805,13 @@
         <v>0.0026120929256859835</v>
       </c>
       <c r="L17">
-        <v>0.003217419002824309</v>
+        <v>0.0032174190028243085</v>
       </c>
       <c r="M17">
         <v>0.0035077319299388404</v>
       </c>
       <c r="N17">
-        <v>0.0038607033728156044</v>
+        <v>0.003860703372815604</v>
       </c>
       <c r="O17">
         <v>0.0037698319547875897</v>
@@ -1835,7 +1835,7 @@
         <v>0.003884400416020618</v>
       </c>
       <c r="V17">
-        <v>0.0036851780306577553</v>
+        <v>0.003685178030657755</v>
       </c>
       <c r="W17">
         <v>0.0033600105233111766</v>
@@ -1844,7 +1844,7 @@
         <v>0.0030025887799725284</v>
       </c>
       <c r="Y17">
-        <v>0.0021929773586243056</v>
+        <v>0.002192977358624305</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -1929,7 +1929,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.0017166305519427246</v>
+        <v>0.0017166305519427238</v>
       </c>
       <c r="C19">
         <v>0.0013771098371934596</v>
@@ -1938,25 +1938,25 @@
         <v>0.0011309982326361742</v>
       </c>
       <c r="E19">
-        <v>0.0009694363322106775</v>
+        <v>0.0009694363322106774</v>
       </c>
       <c r="F19">
-        <v>0.0010065130801263568</v>
+        <v>0.0010065130801263573</v>
       </c>
       <c r="G19">
-        <v>0.001099755141655008</v>
+        <v>0.0010997551416550085</v>
       </c>
       <c r="H19">
-        <v>0.0012944747262608595</v>
+        <v>0.0012944747262608597</v>
       </c>
       <c r="I19">
         <v>0.0014465786316822185</v>
       </c>
       <c r="J19">
-        <v>0.0016833443498209325</v>
+        <v>0.001683344349820932</v>
       </c>
       <c r="K19">
-        <v>0.0019730902318151147</v>
+        <v>0.0019730902318151142</v>
       </c>
       <c r="L19">
         <v>0.002145558576331036</v>
@@ -1965,19 +1965,19 @@
         <v>0.0022094427359246886</v>
       </c>
       <c r="N19">
-        <v>0.002266620566783339</v>
+        <v>0.002266620566783338</v>
       </c>
       <c r="O19">
-        <v>0.0021747941516446147</v>
+        <v>0.0021747941516446143</v>
       </c>
       <c r="P19">
         <v>0.002181586408484786</v>
       </c>
       <c r="Q19">
-        <v>0.002175275393828362</v>
+        <v>0.0021752753938283627</v>
       </c>
       <c r="R19">
-        <v>0.002421762136024393</v>
+        <v>0.0024217621360243928</v>
       </c>
       <c r="S19">
         <v>0.0026149914765346677</v>
@@ -1986,7 +1986,7 @@
         <v>0.003246953059250751</v>
       </c>
       <c r="U19">
-        <v>0.00357966941695784</v>
+        <v>0.0035796694169578404</v>
       </c>
       <c r="V19">
         <v>0.0033800375175084907</v>
@@ -1995,10 +1995,10 @@
         <v>0.0030540224223885577</v>
       </c>
       <c r="X19">
-        <v>0.002628475975867827</v>
+        <v>0.0026284759758678274</v>
       </c>
       <c r="Y19">
-        <v>0.0017816727963679462</v>
+        <v>0.0017816727963679464</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2009,22 +2009,22 @@
         <v>0.002434268316658558</v>
       </c>
       <c r="C20">
-        <v>0.0017558840019390263</v>
+        <v>0.0017558840019390265</v>
       </c>
       <c r="D20">
         <v>0.0012685659306243054</v>
       </c>
       <c r="E20">
-        <v>0.0009532120227600926</v>
+        <v>0.0009532120227600928</v>
       </c>
       <c r="F20">
         <v>0.0010251024906983877</v>
       </c>
       <c r="G20">
-        <v>0.0012072017063794824</v>
+        <v>0.0012072017063794818</v>
       </c>
       <c r="H20">
-        <v>0.0016104558142704512</v>
+        <v>0.001610455814270451</v>
       </c>
       <c r="I20">
         <v>0.001970843809466825</v>
@@ -2314,10 +2314,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.0018463421277981433</v>
+        <v>0.001846342127798143</v>
       </c>
       <c r="C24">
-        <v>0.0015802027502797025</v>
+        <v>0.0015802027502797023</v>
       </c>
       <c r="D24">
         <v>0.0014161337051687855</v>
@@ -2326,13 +2326,13 @@
         <v>0.0013584208848756822</v>
       </c>
       <c r="F24">
-        <v>0.0013682843438753208</v>
+        <v>0.0013682843438753206</v>
       </c>
       <c r="G24">
         <v>0.0014077854839831775</v>
       </c>
       <c r="H24">
-        <v>0.0014992518773795825</v>
+        <v>0.0014992518773795827</v>
       </c>
       <c r="I24">
         <v>0.001577146996257638</v>
@@ -2341,10 +2341,10 @@
         <v>0.0017239210717937717</v>
       </c>
       <c r="K24">
-        <v>0.0018958336364028876</v>
+        <v>0.0018958336364028874</v>
       </c>
       <c r="L24">
-        <v>0.0019604493410998974</v>
+        <v>0.001960449341099897</v>
       </c>
       <c r="M24">
         <v>0.001995735500086282</v>
@@ -2359,7 +2359,7 @@
         <v>0.0020089411657370467</v>
       </c>
       <c r="Q24">
-        <v>0.00197206278570875</v>
+        <v>0.0019720627857087504</v>
       </c>
       <c r="R24">
         <v>0.00224548279002488</v>
@@ -2368,16 +2368,16 @@
         <v>0.0025269054523356393</v>
       </c>
       <c r="T24">
-        <v>0.002968183543242613</v>
+        <v>0.0029681835432426133</v>
       </c>
       <c r="U24">
-        <v>0.00310791392813711</v>
+        <v>0.0031079139281371105</v>
       </c>
       <c r="V24">
         <v>0.003015853582112814</v>
       </c>
       <c r="W24">
-        <v>0.0029069794497548667</v>
+        <v>0.002906979449754867</v>
       </c>
       <c r="X24">
         <v>0.0029756877656410483</v>
@@ -2477,13 +2477,13 @@
         <v>6.634582195276093e-5</v>
       </c>
       <c r="E26">
-        <v>6.0660797453363474e-5</v>
+        <v>6.066079745336348e-5</v>
       </c>
       <c r="F26">
         <v>6.194804278306645e-5</v>
       </c>
       <c r="G26">
-        <v>6.52309452758584e-5</v>
+        <v>6.523094527579469e-5</v>
       </c>
       <c r="H26">
         <v>6.861178983234295e-5</v>
@@ -2504,7 +2504,7 @@
         <v>7.79646391492745e-5</v>
       </c>
       <c r="N26">
-        <v>7.863617151641397e-5</v>
+        <v>7.863617151641398e-5</v>
       </c>
       <c r="O26">
         <v>7.510259907322417e-5</v>
@@ -2622,55 +2622,55 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>8.95693843438484e-5</v>
+        <v>8.956938434384838e-5</v>
       </c>
       <c r="C28">
-        <v>7.809459765198285e-5</v>
+        <v>7.809459765198282e-5</v>
       </c>
       <c r="D28">
-        <v>7.334033775303703e-5</v>
+        <v>7.334033775303704e-5</v>
       </c>
       <c r="E28">
-        <v>7.943405901815051e-5</v>
+        <v>7.94340590181505e-5</v>
       </c>
       <c r="F28">
         <v>7.731455807598618e-5</v>
       </c>
       <c r="G28">
-        <v>7.504087684466095e-5</v>
+        <v>7.504087684466098e-5</v>
       </c>
       <c r="H28">
         <v>7.777782052175033e-5</v>
       </c>
       <c r="I28">
-        <v>8.218819185227767e-5</v>
+        <v>8.218819185227768e-5</v>
       </c>
       <c r="J28">
-        <v>8.98849089203474e-5</v>
+        <v>8.988490892034737e-5</v>
       </c>
       <c r="K28">
-        <v>0.0001010237182317479</v>
+        <v>0.00010102371823174789</v>
       </c>
       <c r="L28">
-        <v>0.00010875287311219125</v>
+        <v>0.00010875287311219122</v>
       </c>
       <c r="M28">
-        <v>0.00011195610912586112</v>
+        <v>0.00011195610912586111</v>
       </c>
       <c r="N28">
-        <v>0.00011510579649084599</v>
+        <v>0.00011510579649084596</v>
       </c>
       <c r="O28">
-        <v>0.0001132623587180167</v>
+        <v>0.00011326235871801669</v>
       </c>
       <c r="P28">
-        <v>0.00011803530064702117</v>
+        <v>0.00011803530064702119</v>
       </c>
       <c r="Q28">
-        <v>0.00010788233706276635</v>
+        <v>0.00010788233706276634</v>
       </c>
       <c r="R28">
-        <v>0.00011888007672745649</v>
+        <v>0.00011888007672745646</v>
       </c>
       <c r="S28">
         <v>0.00012669134184615963</v>
@@ -2679,13 +2679,13 @@
         <v>0.00010655486296455761</v>
       </c>
       <c r="U28">
-        <v>9.669793835323105e-5</v>
+        <v>9.669793835323107e-5</v>
       </c>
       <c r="V28">
-        <v>0.0001034731400243381</v>
+        <v>0.00010347314002433812</v>
       </c>
       <c r="W28">
-        <v>0.00011016977985867443</v>
+        <v>0.00011016977985867445</v>
       </c>
       <c r="X28">
         <v>0.0001756216638967524</v>
@@ -2717,7 +2717,7 @@
         <v>0.0002610264732759833</v>
       </c>
       <c r="H29">
-        <v>0.00027164339529887454</v>
+        <v>0.0002716433952988746</v>
       </c>
       <c r="I29">
         <v>0.0002777586530995801</v>
@@ -2735,7 +2735,7 @@
         <v>0.00029735902164500927</v>
       </c>
       <c r="N29">
-        <v>0.0002990088298206349</v>
+        <v>0.00029900882982063497</v>
       </c>
       <c r="O29">
         <v>0.0002892589421411053</v>
@@ -2744,22 +2744,22 @@
         <v>0.0002956135231291228</v>
       </c>
       <c r="Q29">
-        <v>0.00029333727745617946</v>
+        <v>0.0002933372774561795</v>
       </c>
       <c r="R29">
         <v>0.00035447439072222445</v>
       </c>
       <c r="S29">
-        <v>0.0004325220136146411</v>
+        <v>0.00043252201361464117</v>
       </c>
       <c r="T29">
-        <v>0.0005683578539228638</v>
+        <v>0.0005683578539228639</v>
       </c>
       <c r="U29">
         <v>0.0005986753030599317</v>
       </c>
       <c r="V29">
-        <v>0.0005745977235727924</v>
+        <v>0.0005745977235727925</v>
       </c>
       <c r="W29">
         <v>0.000565163560772316</v>
@@ -3715,7 +3715,7 @@
         <v>1.0607550777207981</v>
       </c>
       <c r="G42">
-        <v>1.060750744219498</v>
+        <v>1.0607507442194988</v>
       </c>
       <c r="H42">
         <v>1.0607451578931633</v>
@@ -3863,13 +3863,13 @@
         <v>0.0025236363785130144</v>
       </c>
       <c r="E44">
-        <v>0.0024928790075913667</v>
+        <v>0.002492879007591367</v>
       </c>
       <c r="F44">
-        <v>0.0025003962415209484</v>
+        <v>0.002500396241520949</v>
       </c>
       <c r="G44">
-        <v>0.0025180680301331035</v>
+        <v>0.0025180680301669363</v>
       </c>
       <c r="H44">
         <v>0.0025417719113235257</v>
@@ -3887,7 +3887,7 @@
         <v>0.0019634421921592114</v>
       </c>
       <c r="M44">
-        <v>0.0017398012016090782</v>
+        <v>0.0017398012016090784</v>
       </c>
       <c r="N44">
         <v>0.0014468379622950183</v>
@@ -3943,7 +3943,7 @@
         <v>0.0029779178788118094</v>
       </c>
       <c r="F45">
-        <v>0.002980830050830264</v>
+        <v>0.0029808300508302643</v>
       </c>
       <c r="G45">
         <v>0.002987578957743676</v>
@@ -3973,7 +3973,7 @@
         <v>0.003039498823799456</v>
       </c>
       <c r="P45">
-        <v>0.0030394030221926214</v>
+        <v>0.003039403022192622</v>
       </c>
       <c r="Q45">
         <v>0.003085653379914206</v>
@@ -4014,13 +4014,13 @@
         <v>0.0014783768281015745</v>
       </c>
       <c r="D46">
-        <v>0.0014618919373217524</v>
+        <v>0.0014618919373217527</v>
       </c>
       <c r="E46">
         <v>0.0014462434033654418</v>
       </c>
       <c r="F46">
-        <v>0.0014502839836385798</v>
+        <v>0.00145028398363858</v>
       </c>
       <c r="G46">
         <v>0.0014592345931364668</v>
@@ -4085,49 +4085,49 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.00012983018686528838</v>
+        <v>0.0001298301868652885</v>
       </c>
       <c r="C47">
-        <v>0.00023828378637001868</v>
+        <v>0.00023828378637001906</v>
       </c>
       <c r="D47">
-        <v>0.0005091624297957389</v>
+        <v>0.00050916242979574</v>
       </c>
       <c r="E47">
-        <v>0.0012643768481853815</v>
+        <v>0.0012643768481853798</v>
       </c>
       <c r="F47">
-        <v>0.0010422683041951776</v>
+        <v>0.0010422683041951771</v>
       </c>
       <c r="G47">
-        <v>0.0006839690249447176</v>
+        <v>0.0006839690249447188</v>
       </c>
       <c r="H47">
-        <v>0.00040496582868916836</v>
+        <v>0.000404965828689168</v>
       </c>
       <c r="I47">
-        <v>0.0003191078044299155</v>
+        <v>0.0003191078044299158</v>
       </c>
       <c r="J47">
-        <v>0.00022005009966164895</v>
+        <v>0.00022005009966164922</v>
       </c>
       <c r="K47">
-        <v>0.00016380786328421484</v>
+        <v>0.00016380786328421495</v>
       </c>
       <c r="L47">
-        <v>0.00016578496791926282</v>
+        <v>0.00016578496791926276</v>
       </c>
       <c r="M47">
-        <v>0.00017975889031541484</v>
+        <v>0.00017975889031541487</v>
       </c>
       <c r="N47">
-        <v>0.00020358921164747491</v>
+        <v>0.0002035892116474746</v>
       </c>
       <c r="O47">
         <v>0.00031931358254061893</v>
       </c>
       <c r="P47">
-        <v>0.0005408182660333865</v>
+        <v>0.0005408182660333852</v>
       </c>
       <c r="Q47">
         <v>-6.771580456699149e-10</v>
@@ -4151,7 +4151,7 @@
         <v>-6.79372990417206e-10</v>
       </c>
       <c r="X47">
-        <v>0.0020616180771177986</v>
+        <v>0.0020616180771177994</v>
       </c>
       <c r="Y47">
         <v>0.004322854184342137</v>
@@ -4162,55 +4162,55 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>6.822762919308896e-5</v>
+        <v>6.82276291930889e-5</v>
       </c>
       <c r="C48">
-        <v>0.00011516849788980254</v>
+        <v>0.00011516849788980244</v>
       </c>
       <c r="D48">
-        <v>0.00020659115333743476</v>
+        <v>0.0002065911533374347</v>
       </c>
       <c r="E48">
-        <v>0.000366582366238957</v>
+        <v>0.0003665823662389574</v>
       </c>
       <c r="F48">
-        <v>0.0003282013978297207</v>
+        <v>0.00032820139782972096</v>
       </c>
       <c r="G48">
-        <v>0.0002473560148556595</v>
+        <v>0.00024735601485565946</v>
       </c>
       <c r="H48">
-        <v>0.00018900736617214067</v>
+        <v>0.00018900736617214037</v>
       </c>
       <c r="I48">
-        <v>0.00016832140791249307</v>
+        <v>0.00016832140791249296</v>
       </c>
       <c r="J48">
-        <v>0.00012670492654660588</v>
+        <v>0.00012670492654660574</v>
       </c>
       <c r="K48">
-        <v>0.00010681386802764581</v>
+        <v>0.00010681386802764574</v>
       </c>
       <c r="L48">
-        <v>0.00013525169731714857</v>
+        <v>0.0001352516973171484</v>
       </c>
       <c r="M48">
-        <v>0.00015601508831361636</v>
+        <v>0.0001560150883136162</v>
       </c>
       <c r="N48">
-        <v>0.00019110213895604764</v>
+        <v>0.0001911021389560473</v>
       </c>
       <c r="O48">
-        <v>0.00031981229191020244</v>
+        <v>0.00031981229191020195</v>
       </c>
       <c r="P48">
-        <v>0.00046870483879821233</v>
+        <v>0.000468704838798212</v>
       </c>
       <c r="Q48">
-        <v>-6.757105596923211e-10</v>
+        <v>-6.757105596923208e-10</v>
       </c>
       <c r="R48">
-        <v>-6.752218753197872e-10</v>
+        <v>-6.752218753197846e-10</v>
       </c>
       <c r="S48">
         <v>-6.774850760984306e-10</v>
@@ -4263,7 +4263,7 @@
         <v>4.267873180445659e-8</v>
       </c>
       <c r="J49">
-        <v>4.268277492845827e-8</v>
+        <v>4.2682774928458264e-8</v>
       </c>
       <c r="K49">
         <v>4.268719991404678e-8</v>
@@ -4281,28 +4281,28 @@
         <v>4.267774918244502e-8</v>
       </c>
       <c r="P49">
-        <v>4.267368405147144e-8</v>
+        <v>4.2673684051471447e-8</v>
       </c>
       <c r="Q49">
-        <v>4.524176675725393e-5</v>
+        <v>4.52417667572539e-5</v>
       </c>
       <c r="R49">
-        <v>4.7375506925532515e-5</v>
+        <v>4.737550692553245e-5</v>
       </c>
       <c r="S49">
-        <v>0.00010528674161622821</v>
+        <v>0.00010528674161622818</v>
       </c>
       <c r="T49">
-        <v>0.002542372233333681</v>
+        <v>0.0025423722333336816</v>
       </c>
       <c r="U49">
         <v>0.003858104833138854</v>
       </c>
       <c r="V49">
-        <v>0.0030161491012373307</v>
+        <v>0.0030161491012373294</v>
       </c>
       <c r="W49">
-        <v>0.001909267321131283</v>
+        <v>0.0019092673211312822</v>
       </c>
       <c r="X49">
         <v>4.2664601962952106e-8</v>
@@ -4322,13 +4322,13 @@
         <v>4.268349820196073e-8</v>
       </c>
       <c r="D50">
-        <v>4.267027025965277e-8</v>
+        <v>4.2670270259652766e-8</v>
       </c>
       <c r="E50">
         <v>4.2663960588380516e-8</v>
       </c>
       <c r="F50">
-        <v>4.2664682677567975e-8</v>
+        <v>4.266468267756797e-8</v>
       </c>
       <c r="G50">
         <v>4.266769149889071e-8</v>
@@ -4361,25 +4361,25 @@
         <v>4.2661651109941746e-8</v>
       </c>
       <c r="Q50">
-        <v>1.4945349843162398e-5</v>
+        <v>1.4945349843161515e-5</v>
       </c>
       <c r="R50">
-        <v>1.2648009500593276e-5</v>
+        <v>1.2648009500593127e-5</v>
       </c>
       <c r="S50">
-        <v>1.7734611405127522e-5</v>
+        <v>1.7734611405127454e-5</v>
       </c>
       <c r="T50">
-        <v>0.0009580659159978454</v>
+        <v>0.0009580659159978448</v>
       </c>
       <c r="U50">
         <v>0.0022506868890342017</v>
       </c>
       <c r="V50">
-        <v>0.0018784841898270216</v>
+        <v>0.001878484189827021</v>
       </c>
       <c r="W50">
-        <v>0.0006310690309623485</v>
+        <v>0.0006310690309623481</v>
       </c>
       <c r="X50">
         <v>4.2648309656933967e-8</v>
@@ -4399,7 +4399,7 @@
         <v>0.012013368406779173</v>
       </c>
       <c r="D51">
-        <v>0.012497027793086703</v>
+        <v>0.012497027793086705</v>
       </c>
       <c r="E51">
         <v>0.013698140877597013</v>
@@ -4408,10 +4408,10 @@
         <v>0.014688250845923416</v>
       </c>
       <c r="G51">
-        <v>0.015337976498903567</v>
+        <v>0.01533797649890357</v>
       </c>
       <c r="H51">
-        <v>0.015722649113057326</v>
+        <v>0.01572264911305733</v>
       </c>
       <c r="I51">
         <v>0.0160257566022849</v>
@@ -4450,16 +4450,16 @@
         <v>0.014844404946557416</v>
       </c>
       <c r="U51">
-        <v>0.010783241318792538</v>
+        <v>0.010783241318792536</v>
       </c>
       <c r="V51">
-        <v>0.00760834688257375</v>
+        <v>0.0076083468825737495</v>
       </c>
       <c r="W51">
         <v>0.005598591162294375</v>
       </c>
       <c r="X51">
-        <v>0.007557083425448954</v>
+        <v>0.007557083425448955</v>
       </c>
       <c r="Y51">
         <v>0.01166375</v>
@@ -4473,7 +4473,7 @@
         <v>0.005898396297257864</v>
       </c>
       <c r="C52">
-        <v>0.00600776144025507</v>
+        <v>0.006007761440255069</v>
       </c>
       <c r="D52">
         <v>0.006203978119851675</v>
@@ -4482,10 +4482,10 @@
         <v>0.0065521864583464855</v>
       </c>
       <c r="F52">
-        <v>0.006863932876092428</v>
+        <v>0.006863932876092429</v>
       </c>
       <c r="G52">
-        <v>0.007098876176845833</v>
+        <v>0.007098876176845834</v>
       </c>
       <c r="H52">
         <v>0.007278388256862231</v>
@@ -4494,7 +4494,7 @@
         <v>0.007438248674106502</v>
       </c>
       <c r="J52">
-        <v>0.007558573426943562</v>
+        <v>0.007558573426943563</v>
       </c>
       <c r="K52">
         <v>0.007660001669026247</v>
@@ -4518,7 +4518,7 @@
         <v>0.008851386248860272</v>
       </c>
       <c r="R52">
-        <v>0.00883807191318834</v>
+        <v>0.008838071913188339</v>
       </c>
       <c r="S52">
         <v>0.00881940325757212</v>
@@ -4530,7 +4530,7 @@
         <v>0.005441767428049127</v>
       </c>
       <c r="V52">
-        <v>0.0034644150006953793</v>
+        <v>0.003464415000695379</v>
       </c>
       <c r="W52">
         <v>0.0028001311618979846</v>

</xml_diff>

<commit_message>
Tset now made an array, no longer should cause chronology issues while getting output/plotting
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -860,13 +860,13 @@
         <v>0.05427437097296479</v>
       </c>
       <c r="E5">
-        <v>0.05293621220309018</v>
+        <v>0.05293621220309017</v>
       </c>
       <c r="F5">
         <v>0.05319571582982124</v>
       </c>
       <c r="G5">
-        <v>0.05405661479838582</v>
+        <v>0.05405661479838581</v>
       </c>
       <c r="H5">
         <v>0.055706056954738334</v>
@@ -887,7 +887,7 @@
         <v>0.06224222716344458</v>
       </c>
       <c r="N5">
-        <v>0.062381283999564545</v>
+        <v>0.06238128399956454</v>
       </c>
       <c r="O5">
         <v>0.061412239842530233</v>
@@ -928,7 +928,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.04280144356045187</v>
+        <v>0.042801443560451874</v>
       </c>
       <c r="C6">
         <v>0.03977589808733105</v>
@@ -937,7 +937,7 @@
         <v>0.037797662115997346</v>
       </c>
       <c r="E6">
-        <v>0.03715273330417834</v>
+        <v>0.037152733304178336</v>
       </c>
       <c r="F6">
         <v>0.03725226107653092</v>
@@ -946,7 +946,7 @@
         <v>0.03771321964849193</v>
       </c>
       <c r="H6">
-        <v>0.03876949313869839</v>
+        <v>0.03876949313869838</v>
       </c>
       <c r="I6">
         <v>0.039636547458981444</v>
@@ -976,10 +976,10 @@
         <v>0.04308383191541627</v>
       </c>
       <c r="R6">
-        <v>0.04623827257424411</v>
+        <v>0.046238272574244114</v>
       </c>
       <c r="S6">
-        <v>0.04931631385969938</v>
+        <v>0.049316313859699375</v>
       </c>
       <c r="T6">
         <v>0.053040488551201796</v>
@@ -1236,13 +1236,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.009594357663375654</v>
+        <v>0.009594357663375656</v>
       </c>
       <c r="C10">
         <v>0.008996286661527035</v>
       </c>
       <c r="D10">
-        <v>0.008747280970884286</v>
+        <v>0.008747280970884284</v>
       </c>
       <c r="E10">
         <v>0.009155933770505097</v>
@@ -1251,13 +1251,13 @@
         <v>0.009013798834025439</v>
       </c>
       <c r="G10">
-        <v>0.008855442696598567</v>
+        <v>0.008855442696598565</v>
       </c>
       <c r="H10">
         <v>0.00898967775354143</v>
       </c>
       <c r="I10">
-        <v>0.00922375303053097</v>
+        <v>0.009223753030530968</v>
       </c>
       <c r="J10">
         <v>0.0096179285373825</v>
@@ -1266,7 +1266,7 @@
         <v>0.010161569894650538</v>
       </c>
       <c r="L10">
-        <v>0.01052348031313951</v>
+        <v>0.010523480313139513</v>
       </c>
       <c r="M10">
         <v>0.010670763898993851</v>
@@ -1275,10 +1275,10 @@
         <v>0.010814573722841773</v>
       </c>
       <c r="O10">
-        <v>0.010743672538856795</v>
+        <v>0.010743672538856797</v>
       </c>
       <c r="P10">
-        <v>0.010978521623073683</v>
+        <v>0.010978521623073684</v>
       </c>
       <c r="Q10">
         <v>0.010472452962352136</v>
@@ -1290,16 +1290,16 @@
         <v>0.01129224471996417</v>
       </c>
       <c r="T10">
-        <v>0.010121448489469283</v>
+        <v>0.010121448489469284</v>
       </c>
       <c r="U10">
-        <v>0.009472186158058648</v>
+        <v>0.00947218615805865</v>
       </c>
       <c r="V10">
-        <v>0.00991426232612412</v>
+        <v>0.009914262326124119</v>
       </c>
       <c r="W10">
-        <v>0.010367994305393282</v>
+        <v>0.010367994305393284</v>
       </c>
       <c r="X10">
         <v>0.013392605141400893</v>
@@ -1331,7 +1331,7 @@
         <v>0.016595154974473503</v>
       </c>
       <c r="H11">
-        <v>0.016896988251039552</v>
+        <v>0.01689698825103955</v>
       </c>
       <c r="I11">
         <v>0.017049786345542276</v>
@@ -1364,7 +1364,7 @@
         <v>0.018750025284345762</v>
       </c>
       <c r="S11">
-        <v>0.020918594523088866</v>
+        <v>0.020918594523088863</v>
       </c>
       <c r="T11">
         <v>0.02391242140094724</v>
@@ -1373,7 +1373,7 @@
         <v>0.024419953375940565</v>
       </c>
       <c r="V11">
-        <v>0.023991942115673445</v>
+        <v>0.023991942115673442</v>
       </c>
       <c r="W11">
         <v>0.02393260731646729</v>
@@ -1624,25 +1624,25 @@
         <v>0.011262585310224699</v>
       </c>
       <c r="C15">
-        <v>0.009712995860138731</v>
+        <v>0.00971299586013873</v>
       </c>
       <c r="D15">
         <v>0.008588524844934256</v>
       </c>
       <c r="E15">
-        <v>0.007851234640988955</v>
+        <v>0.007851234640988957</v>
       </c>
       <c r="F15">
         <v>0.008020266865080804</v>
       </c>
       <c r="G15">
-        <v>0.0084458624432179</v>
+        <v>0.008445862443217898</v>
       </c>
       <c r="H15">
         <v>0.009354423186373497</v>
       </c>
       <c r="I15">
-        <v>0.010107414051398821</v>
+        <v>0.010107414051398823</v>
       </c>
       <c r="J15">
         <v>0.011287067379352379</v>
@@ -1657,7 +1657,7 @@
         <v>0.015402562944672321</v>
       </c>
       <c r="N15">
-        <v>0.01627267393169162</v>
+        <v>0.016272673931691625</v>
       </c>
       <c r="O15">
         <v>0.01585539775176105</v>
@@ -1666,7 +1666,7 @@
         <v>0.015816977835937163</v>
       </c>
       <c r="Q15">
-        <v>0.015360503554972975</v>
+        <v>0.015360503554972973</v>
       </c>
       <c r="R15">
         <v>0.015628683535162013</v>
@@ -1775,31 +1775,31 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.002132556301988195</v>
+        <v>0.0021325563019881947</v>
       </c>
       <c r="C17">
-        <v>0.0018189625943495834</v>
+        <v>0.001818962594349584</v>
       </c>
       <c r="D17">
-        <v>0.0015970837212705754</v>
+        <v>0.0015970837212705752</v>
       </c>
       <c r="E17">
-        <v>0.0014544550401362102</v>
+        <v>0.0014544550401362098</v>
       </c>
       <c r="F17">
-        <v>0.00148694978079924</v>
+        <v>0.0014869497807992397</v>
       </c>
       <c r="G17">
-        <v>0.0015693084306723838</v>
+        <v>0.0015693084306990048</v>
       </c>
       <c r="H17">
         <v>0.0017523077469673253</v>
       </c>
       <c r="I17">
-        <v>0.001917157629195325</v>
+        <v>0.0019171576291953246</v>
       </c>
       <c r="J17">
-        <v>0.002182399748626265</v>
+        <v>0.0021823997486262645</v>
       </c>
       <c r="K17">
         <v>0.0026120929256859835</v>
@@ -1811,7 +1811,7 @@
         <v>0.0035077319299388404</v>
       </c>
       <c r="N17">
-        <v>0.003860703372815604</v>
+        <v>0.0038607033728156044</v>
       </c>
       <c r="O17">
         <v>0.0037698319547875897</v>
@@ -1823,10 +1823,10 @@
         <v>0.003427046745302235</v>
       </c>
       <c r="R17">
-        <v>0.0032525806248035532</v>
+        <v>0.003252580624803554</v>
       </c>
       <c r="S17">
-        <v>0.003081514315098725</v>
+        <v>0.0030815143150987245</v>
       </c>
       <c r="T17">
         <v>0.003562069052952501</v>
@@ -1844,7 +1844,7 @@
         <v>0.0030025887799725284</v>
       </c>
       <c r="Y17">
-        <v>0.002192977358624305</v>
+        <v>0.0021929773586243056</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -1929,7 +1929,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.0017166305519427238</v>
+        <v>0.0017166305519427242</v>
       </c>
       <c r="C19">
         <v>0.0013771098371934596</v>
@@ -1938,34 +1938,34 @@
         <v>0.0011309982326361742</v>
       </c>
       <c r="E19">
-        <v>0.0009694363322106774</v>
+        <v>0.0009694363322106779</v>
       </c>
       <c r="F19">
         <v>0.0010065130801263573</v>
       </c>
       <c r="G19">
-        <v>0.0010997551416550085</v>
+        <v>0.001099755141655008</v>
       </c>
       <c r="H19">
         <v>0.0012944747262608597</v>
       </c>
       <c r="I19">
-        <v>0.0014465786316822185</v>
+        <v>0.0014465786316822183</v>
       </c>
       <c r="J19">
-        <v>0.001683344349820932</v>
+        <v>0.0016833443498209325</v>
       </c>
       <c r="K19">
         <v>0.0019730902318151142</v>
       </c>
       <c r="L19">
-        <v>0.002145558576331036</v>
+        <v>0.0021455585763310364</v>
       </c>
       <c r="M19">
         <v>0.0022094427359246886</v>
       </c>
       <c r="N19">
-        <v>0.002266620566783338</v>
+        <v>0.002266620566783339</v>
       </c>
       <c r="O19">
         <v>0.0021747941516446143</v>
@@ -1974,7 +1974,7 @@
         <v>0.002181586408484786</v>
       </c>
       <c r="Q19">
-        <v>0.0021752753938283627</v>
+        <v>0.002175275393828362</v>
       </c>
       <c r="R19">
         <v>0.0024217621360243928</v>
@@ -1986,19 +1986,19 @@
         <v>0.003246953059250751</v>
       </c>
       <c r="U19">
-        <v>0.0035796694169578404</v>
+        <v>0.00357966941695784</v>
       </c>
       <c r="V19">
-        <v>0.0033800375175084907</v>
+        <v>0.003380037517508491</v>
       </c>
       <c r="W19">
         <v>0.0030540224223885577</v>
       </c>
       <c r="X19">
-        <v>0.0026284759758678274</v>
+        <v>0.002628475975867827</v>
       </c>
       <c r="Y19">
-        <v>0.0017816727963679464</v>
+        <v>0.0017816727963679462</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2009,28 +2009,28 @@
         <v>0.002434268316658558</v>
       </c>
       <c r="C20">
-        <v>0.0017558840019390265</v>
+        <v>0.001755884001939026</v>
       </c>
       <c r="D20">
         <v>0.0012685659306243054</v>
       </c>
       <c r="E20">
-        <v>0.0009532120227600928</v>
+        <v>0.0009532120227600929</v>
       </c>
       <c r="F20">
         <v>0.0010251024906983877</v>
       </c>
       <c r="G20">
-        <v>0.0012072017063794818</v>
+        <v>0.0012072017063794822</v>
       </c>
       <c r="H20">
-        <v>0.001610455814270451</v>
+        <v>0.0016104558142704508</v>
       </c>
       <c r="I20">
         <v>0.001970843809466825</v>
       </c>
       <c r="J20">
-        <v>0.002542796187003667</v>
+        <v>0.0025427961870036677</v>
       </c>
       <c r="K20">
         <v>0.003453330536527349</v>
@@ -2072,7 +2072,7 @@
         <v>0.005149386183092092</v>
       </c>
       <c r="X20">
-        <v>0.00426436685742628</v>
+        <v>0.0042643668574262805</v>
       </c>
       <c r="Y20">
         <v>0.002564277624621613</v>
@@ -2314,40 +2314,40 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.001846342127798143</v>
+        <v>0.0018463421277981431</v>
       </c>
       <c r="C24">
-        <v>0.0015802027502797023</v>
+        <v>0.0015802027502797025</v>
       </c>
       <c r="D24">
         <v>0.0014161337051687855</v>
       </c>
       <c r="E24">
-        <v>0.0013584208848756822</v>
+        <v>0.001358420884875682</v>
       </c>
       <c r="F24">
-        <v>0.0013682843438753206</v>
+        <v>0.0013682843438753208</v>
       </c>
       <c r="G24">
         <v>0.0014077854839831775</v>
       </c>
       <c r="H24">
-        <v>0.0014992518773795827</v>
+        <v>0.0014992518773795825</v>
       </c>
       <c r="I24">
         <v>0.001577146996257638</v>
       </c>
       <c r="J24">
-        <v>0.0017239210717937717</v>
+        <v>0.0017239210717937719</v>
       </c>
       <c r="K24">
-        <v>0.0018958336364028874</v>
+        <v>0.0018958336364028876</v>
       </c>
       <c r="L24">
-        <v>0.001960449341099897</v>
+        <v>0.0019604493410998974</v>
       </c>
       <c r="M24">
-        <v>0.001995735500086282</v>
+        <v>0.0019957355000862816</v>
       </c>
       <c r="N24">
         <v>0.0020325480768637154</v>
@@ -2368,7 +2368,7 @@
         <v>0.0025269054523356393</v>
       </c>
       <c r="T24">
-        <v>0.0029681835432426133</v>
+        <v>0.002968183543242613</v>
       </c>
       <c r="U24">
         <v>0.0031079139281371105</v>
@@ -2383,7 +2383,7 @@
         <v>0.0029756877656410483</v>
       </c>
       <c r="Y24">
-        <v>0.0024597953338401355</v>
+        <v>0.002459795333840135</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -2391,7 +2391,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.0001055669018014682</v>
+        <v>0.00010556690180146822</v>
       </c>
       <c r="C25">
         <v>9.039348036244795e-5</v>
@@ -2477,13 +2477,13 @@
         <v>6.634582195276093e-5</v>
       </c>
       <c r="E26">
-        <v>6.066079745336348e-5</v>
+        <v>6.0660797453363474e-5</v>
       </c>
       <c r="F26">
         <v>6.194804278306645e-5</v>
       </c>
       <c r="G26">
-        <v>6.523094527579469e-5</v>
+        <v>6.523094527584482e-5</v>
       </c>
       <c r="H26">
         <v>6.861178983234295e-5</v>
@@ -2498,13 +2498,13 @@
         <v>7.993643642350706e-5</v>
       </c>
       <c r="L26">
-        <v>7.771472082418952e-5</v>
+        <v>7.771472082418953e-5</v>
       </c>
       <c r="M26">
-        <v>7.79646391492745e-5</v>
+        <v>7.796463914927448e-5</v>
       </c>
       <c r="N26">
-        <v>7.863617151641398e-5</v>
+        <v>7.863617151641397e-5</v>
       </c>
       <c r="O26">
         <v>7.510259907322417e-5</v>
@@ -2516,7 +2516,7 @@
         <v>7.786243809684615e-5</v>
       </c>
       <c r="R26">
-        <v>9.286752751972836e-5</v>
+        <v>9.286752751972837e-5</v>
       </c>
       <c r="S26">
         <v>0.00011217243570701032</v>
@@ -2622,13 +2622,13 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>8.956938434384838e-5</v>
+        <v>8.95693843438484e-5</v>
       </c>
       <c r="C28">
         <v>7.809459765198282e-5</v>
       </c>
       <c r="D28">
-        <v>7.334033775303704e-5</v>
+        <v>7.334033775303703e-5</v>
       </c>
       <c r="E28">
         <v>7.94340590181505e-5</v>
@@ -2637,28 +2637,28 @@
         <v>7.731455807598618e-5</v>
       </c>
       <c r="G28">
-        <v>7.504087684466098e-5</v>
+        <v>7.504087684466095e-5</v>
       </c>
       <c r="H28">
-        <v>7.777782052175033e-5</v>
+        <v>7.777782052175031e-5</v>
       </c>
       <c r="I28">
-        <v>8.218819185227768e-5</v>
+        <v>8.218819185227766e-5</v>
       </c>
       <c r="J28">
-        <v>8.988490892034737e-5</v>
+        <v>8.98849089203474e-5</v>
       </c>
       <c r="K28">
-        <v>0.00010102371823174789</v>
+        <v>0.00010102371823174792</v>
       </c>
       <c r="L28">
-        <v>0.00010875287311219122</v>
+        <v>0.00010875287311219125</v>
       </c>
       <c r="M28">
-        <v>0.00011195610912586111</v>
+        <v>0.00011195610912586112</v>
       </c>
       <c r="N28">
-        <v>0.00011510579649084596</v>
+        <v>0.00011510579649084598</v>
       </c>
       <c r="O28">
         <v>0.00011326235871801669</v>
@@ -2667,22 +2667,22 @@
         <v>0.00011803530064702119</v>
       </c>
       <c r="Q28">
-        <v>0.00010788233706276634</v>
+        <v>0.00010788233706276635</v>
       </c>
       <c r="R28">
-        <v>0.00011888007672745646</v>
+        <v>0.00011888007672745647</v>
       </c>
       <c r="S28">
         <v>0.00012669134184615963</v>
       </c>
       <c r="T28">
-        <v>0.00010655486296455761</v>
+        <v>0.00010655486296455764</v>
       </c>
       <c r="U28">
         <v>9.669793835323107e-5</v>
       </c>
       <c r="V28">
-        <v>0.00010347314002433812</v>
+        <v>0.0001034731400243381</v>
       </c>
       <c r="W28">
         <v>0.00011016977985867445</v>
@@ -2717,25 +2717,25 @@
         <v>0.0002610264732759833</v>
       </c>
       <c r="H29">
-        <v>0.0002716433952988746</v>
+        <v>0.00027164339529887454</v>
       </c>
       <c r="I29">
         <v>0.0002777586530995801</v>
       </c>
       <c r="J29">
-        <v>0.00029580732913763965</v>
+        <v>0.0002958073291376397</v>
       </c>
       <c r="K29">
         <v>0.00030919123220410615</v>
       </c>
       <c r="L29">
-        <v>0.0002974640722703857</v>
+        <v>0.00029746407227038574</v>
       </c>
       <c r="M29">
         <v>0.00029735902164500927</v>
       </c>
       <c r="N29">
-        <v>0.00029900882982063497</v>
+        <v>0.0002990088298206349</v>
       </c>
       <c r="O29">
         <v>0.0002892589421411053</v>
@@ -2750,7 +2750,7 @@
         <v>0.00035447439072222445</v>
       </c>
       <c r="S29">
-        <v>0.00043252201361464117</v>
+        <v>0.0004325220136146411</v>
       </c>
       <c r="T29">
         <v>0.0005683578539228639</v>
@@ -2759,16 +2759,16 @@
         <v>0.0005986753030599317</v>
       </c>
       <c r="V29">
-        <v>0.0005745977235727925</v>
+        <v>0.0005745977235727924</v>
       </c>
       <c r="W29">
         <v>0.000565163560772316</v>
       </c>
       <c r="X29">
-        <v>0.0005438449431188449</v>
+        <v>0.0005438449431188448</v>
       </c>
       <c r="Y29">
-        <v>0.0004393817729784901</v>
+        <v>0.00043938177297849005</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -3715,7 +3715,7 @@
         <v>1.0607550777207981</v>
       </c>
       <c r="G42">
-        <v>1.0607507442194988</v>
+        <v>1.060750744219498</v>
       </c>
       <c r="H42">
         <v>1.0607451578931633</v>
@@ -3863,19 +3863,19 @@
         <v>0.0025236363785130144</v>
       </c>
       <c r="E44">
-        <v>0.002492879007591367</v>
+        <v>0.0024928790075913667</v>
       </c>
       <c r="F44">
-        <v>0.002500396241520949</v>
+        <v>0.0025003962415209484</v>
       </c>
       <c r="G44">
-        <v>0.0025180680301669363</v>
+        <v>0.002518068030140315</v>
       </c>
       <c r="H44">
         <v>0.0025417719113235257</v>
       </c>
       <c r="I44">
-        <v>0.002536945102686897</v>
+        <v>0.0025369451026868964</v>
       </c>
       <c r="J44">
         <v>0.0025184225045824372</v>
@@ -3887,7 +3887,7 @@
         <v>0.0019634421921592114</v>
       </c>
       <c r="M44">
-        <v>0.0017398012016090784</v>
+        <v>0.0017398012016090782</v>
       </c>
       <c r="N44">
         <v>0.0014468379622950183</v>
@@ -3943,7 +3943,7 @@
         <v>0.0029779178788118094</v>
       </c>
       <c r="F45">
-        <v>0.0029808300508302643</v>
+        <v>0.002980830050830264</v>
       </c>
       <c r="G45">
         <v>0.002987578957743676</v>
@@ -3973,7 +3973,7 @@
         <v>0.003039498823799456</v>
       </c>
       <c r="P45">
-        <v>0.003039403022192622</v>
+        <v>0.0030394030221926214</v>
       </c>
       <c r="Q45">
         <v>0.003085653379914206</v>
@@ -4014,13 +4014,13 @@
         <v>0.0014783768281015745</v>
       </c>
       <c r="D46">
-        <v>0.0014618919373217527</v>
+        <v>0.0014618919373217524</v>
       </c>
       <c r="E46">
         <v>0.0014462434033654418</v>
       </c>
       <c r="F46">
-        <v>0.00145028398363858</v>
+        <v>0.0014502839836385798</v>
       </c>
       <c r="G46">
         <v>0.0014592345931364668</v>
@@ -4085,49 +4085,49 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.0001298301868652885</v>
+        <v>0.00012983018686528827</v>
       </c>
       <c r="C47">
-        <v>0.00023828378637001906</v>
+        <v>0.00023828378637001896</v>
       </c>
       <c r="D47">
-        <v>0.00050916242979574</v>
+        <v>0.0005091624297957388</v>
       </c>
       <c r="E47">
-        <v>0.0012643768481853798</v>
+        <v>0.0012643768481853807</v>
       </c>
       <c r="F47">
-        <v>0.0010422683041951771</v>
+        <v>0.001042268304195178</v>
       </c>
       <c r="G47">
-        <v>0.0006839690249447188</v>
+        <v>0.0006839690249447174</v>
       </c>
       <c r="H47">
-        <v>0.000404965828689168</v>
+        <v>0.00040496582868916825</v>
       </c>
       <c r="I47">
-        <v>0.0003191078044299158</v>
+        <v>0.00031910780442991516</v>
       </c>
       <c r="J47">
-        <v>0.00022005009966164922</v>
+        <v>0.00022005009966164868</v>
       </c>
       <c r="K47">
-        <v>0.00016380786328421495</v>
+        <v>0.00016380786328421473</v>
       </c>
       <c r="L47">
-        <v>0.00016578496791926276</v>
+        <v>0.00016578496791926274</v>
       </c>
       <c r="M47">
-        <v>0.00017975889031541487</v>
+        <v>0.00017975889031541484</v>
       </c>
       <c r="N47">
-        <v>0.0002035892116474746</v>
+        <v>0.00020358921164747467</v>
       </c>
       <c r="O47">
         <v>0.00031931358254061893</v>
       </c>
       <c r="P47">
-        <v>0.0005408182660333852</v>
+        <v>0.0005408182660333861</v>
       </c>
       <c r="Q47">
         <v>-6.771580456699149e-10</v>
@@ -4151,7 +4151,7 @@
         <v>-6.79372990417206e-10</v>
       </c>
       <c r="X47">
-        <v>0.0020616180771177994</v>
+        <v>0.0020616180771178003</v>
       </c>
       <c r="Y47">
         <v>0.004322854184342137</v>
@@ -4162,49 +4162,49 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>6.82276291930889e-5</v>
+        <v>6.822762919308893e-5</v>
       </c>
       <c r="C48">
-        <v>0.00011516849788980244</v>
+        <v>0.00011516849788980254</v>
       </c>
       <c r="D48">
-        <v>0.0002065911533374347</v>
+        <v>0.00020659115333743466</v>
       </c>
       <c r="E48">
-        <v>0.0003665823662389574</v>
+        <v>0.0003665823662389568</v>
       </c>
       <c r="F48">
-        <v>0.00032820139782972096</v>
+        <v>0.00032820139782972047</v>
       </c>
       <c r="G48">
-        <v>0.00024735601485565946</v>
+        <v>0.00024735601485565935</v>
       </c>
       <c r="H48">
-        <v>0.00018900736617214037</v>
+        <v>0.00018900736617214064</v>
       </c>
       <c r="I48">
-        <v>0.00016832140791249296</v>
+        <v>0.00016832140791249307</v>
       </c>
       <c r="J48">
-        <v>0.00012670492654660574</v>
+        <v>0.00012670492654660582</v>
       </c>
       <c r="K48">
-        <v>0.00010681386802764574</v>
+        <v>0.00010681386802764582</v>
       </c>
       <c r="L48">
-        <v>0.0001352516973171484</v>
+        <v>0.00013525169731714863</v>
       </c>
       <c r="M48">
-        <v>0.0001560150883136162</v>
+        <v>0.00015601508831361636</v>
       </c>
       <c r="N48">
-        <v>0.0001911021389560473</v>
+        <v>0.00019110213895604766</v>
       </c>
       <c r="O48">
-        <v>0.00031981229191020195</v>
+        <v>0.00031981229191020244</v>
       </c>
       <c r="P48">
-        <v>0.000468704838798212</v>
+        <v>0.00046870483879821217</v>
       </c>
       <c r="Q48">
         <v>-6.757105596923208e-10</v>
@@ -4228,7 +4228,7 @@
         <v>-6.824323286948852e-10</v>
       </c>
       <c r="X48">
-        <v>0.0009626619728130728</v>
+        <v>0.0009626619728130724</v>
       </c>
       <c r="Y48">
         <v>0.0022305839176888754</v>
@@ -4248,7 +4248,7 @@
         <v>4.267589850055653e-8</v>
       </c>
       <c r="E49">
-        <v>4.2675202512299345e-8</v>
+        <v>4.267520251229934e-8</v>
       </c>
       <c r="F49">
         <v>4.2674626064195624e-8</v>
@@ -4281,28 +4281,28 @@
         <v>4.267774918244502e-8</v>
       </c>
       <c r="P49">
-        <v>4.2673684051471447e-8</v>
+        <v>4.267368405147144e-8</v>
       </c>
       <c r="Q49">
-        <v>4.52417667572539e-5</v>
+        <v>4.5241766757253904e-5</v>
       </c>
       <c r="R49">
-        <v>4.737550692553245e-5</v>
+        <v>4.737550692553251e-5</v>
       </c>
       <c r="S49">
-        <v>0.00010528674161622818</v>
+        <v>0.00010528674161622821</v>
       </c>
       <c r="T49">
-        <v>0.0025423722333336816</v>
+        <v>0.0025423722333336803</v>
       </c>
       <c r="U49">
-        <v>0.003858104833138854</v>
+        <v>0.0038581048331388537</v>
       </c>
       <c r="V49">
-        <v>0.0030161491012373294</v>
+        <v>0.0030161491012373307</v>
       </c>
       <c r="W49">
-        <v>0.0019092673211312822</v>
+        <v>0.0019092673211312827</v>
       </c>
       <c r="X49">
         <v>4.2664601962952106e-8</v>
@@ -4322,13 +4322,13 @@
         <v>4.268349820196073e-8</v>
       </c>
       <c r="D50">
-        <v>4.2670270259652766e-8</v>
+        <v>4.267027025965277e-8</v>
       </c>
       <c r="E50">
         <v>4.2663960588380516e-8</v>
       </c>
       <c r="F50">
-        <v>4.266468267756797e-8</v>
+        <v>4.2664682677567975e-8</v>
       </c>
       <c r="G50">
         <v>4.266769149889071e-8</v>
@@ -4361,25 +4361,25 @@
         <v>4.2661651109941746e-8</v>
       </c>
       <c r="Q50">
-        <v>1.4945349843161515e-5</v>
+        <v>1.494534984316151e-5</v>
       </c>
       <c r="R50">
-        <v>1.2648009500593127e-5</v>
+        <v>1.264800950059313e-5</v>
       </c>
       <c r="S50">
-        <v>1.7734611405127454e-5</v>
+        <v>1.7734611405127447e-5</v>
       </c>
       <c r="T50">
-        <v>0.0009580659159978448</v>
+        <v>0.0009580659159978453</v>
       </c>
       <c r="U50">
         <v>0.0022506868890342017</v>
       </c>
       <c r="V50">
-        <v>0.001878484189827021</v>
+        <v>0.0018784841898270214</v>
       </c>
       <c r="W50">
-        <v>0.0006310690309623481</v>
+        <v>0.0006310690309623486</v>
       </c>
       <c r="X50">
         <v>4.2648309656933967e-8</v>
@@ -4396,7 +4396,7 @@
         <v>0.011787043738294265</v>
       </c>
       <c r="C51">
-        <v>0.012013368406779173</v>
+        <v>0.012013368406779175</v>
       </c>
       <c r="D51">
         <v>0.012497027793086705</v>
@@ -4405,7 +4405,7 @@
         <v>0.013698140877597013</v>
       </c>
       <c r="F51">
-        <v>0.014688250845923416</v>
+        <v>0.014688250845923418</v>
       </c>
       <c r="G51">
         <v>0.01533797649890357</v>
@@ -4423,7 +4423,7 @@
         <v>0.01639033180395206</v>
       </c>
       <c r="L51">
-        <v>0.016547782589947654</v>
+        <v>0.016547782589947657</v>
       </c>
       <c r="M51">
         <v>0.016718508603813714</v>
@@ -4432,7 +4432,7 @@
         <v>0.016911873425146558</v>
       </c>
       <c r="O51">
-        <v>0.01721517640461364</v>
+        <v>0.017215176404613636</v>
       </c>
       <c r="P51">
         <v>0.017728908837677932</v>
@@ -4447,13 +4447,13 @@
         <v>0.017520586890228475</v>
       </c>
       <c r="T51">
-        <v>0.014844404946557416</v>
+        <v>0.014844404946557418</v>
       </c>
       <c r="U51">
-        <v>0.010783241318792536</v>
+        <v>0.010783241318792538</v>
       </c>
       <c r="V51">
-        <v>0.0076083468825737495</v>
+        <v>0.00760834688257375</v>
       </c>
       <c r="W51">
         <v>0.005598591162294375</v>
@@ -4473,19 +4473,19 @@
         <v>0.005898396297257864</v>
       </c>
       <c r="C52">
-        <v>0.006007761440255069</v>
+        <v>0.00600776144025507</v>
       </c>
       <c r="D52">
         <v>0.006203978119851675</v>
       </c>
       <c r="E52">
-        <v>0.0065521864583464855</v>
+        <v>0.006552186458346486</v>
       </c>
       <c r="F52">
-        <v>0.006863932876092429</v>
+        <v>0.006863932876092428</v>
       </c>
       <c r="G52">
-        <v>0.007098876176845834</v>
+        <v>0.007098876176845833</v>
       </c>
       <c r="H52">
         <v>0.007278388256862231</v>
@@ -4530,13 +4530,13 @@
         <v>0.005441767428049127</v>
       </c>
       <c r="V52">
-        <v>0.003464415000695379</v>
+        <v>0.0034644150006953793</v>
       </c>
       <c r="W52">
         <v>0.0028001311618979846</v>
       </c>
       <c r="X52">
-        <v>0.0037146151431128697</v>
+        <v>0.0037146151431128693</v>
       </c>
       <c r="Y52">
         <v>0.005833624999999999</v>

</xml_diff>

<commit_message>
able to run output on labpc as well
</commit_message>
<xml_diff>
--- a/decision_variables.xlsx
+++ b/decision_variables.xlsx
@@ -854,7 +854,7 @@
         <v>0.06173114629133221</v>
       </c>
       <c r="C5">
-        <v>0.05729245801899839</v>
+        <v>0.0572924580189984</v>
       </c>
       <c r="D5">
         <v>0.05427437097296479</v>
@@ -866,7 +866,7 @@
         <v>0.053195715829821244</v>
       </c>
       <c r="G5">
-        <v>0.05405661479838581</v>
+        <v>0.05405661479838582</v>
       </c>
       <c r="H5">
         <v>0.055706056954738334</v>
@@ -878,7 +878,7 @@
         <v>0.05934596275255661</v>
       </c>
       <c r="K5">
-        <v>0.06177021061536756</v>
+        <v>0.061770210615367555</v>
       </c>
       <c r="L5">
         <v>0.06204071841054558</v>
@@ -979,7 +979,7 @@
         <v>0.046238272574244114</v>
       </c>
       <c r="S6">
-        <v>0.049316313859699375</v>
+        <v>0.04931631385969938</v>
       </c>
       <c r="T6">
         <v>0.053040488551201796</v>
@@ -997,7 +997,7 @@
         <v>0.05403223133659516</v>
       </c>
       <c r="Y6">
-        <v>0.04975971613656475</v>
+        <v>0.04975971613656474</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1097,7 +1097,7 @@
         <v>0.007971813579067568</v>
       </c>
       <c r="G8">
-        <v>0.008171788676130066</v>
+        <v>0.00817178867613007</v>
       </c>
       <c r="H8">
         <v>0.008351694521937954</v>
@@ -1239,10 +1239,10 @@
         <v>0.009594357663375656</v>
       </c>
       <c r="C10">
-        <v>0.008996286661527034</v>
+        <v>0.008996286661527035</v>
       </c>
       <c r="D10">
-        <v>0.008747280970884286</v>
+        <v>0.008747280970884284</v>
       </c>
       <c r="E10">
         <v>0.009155933770505097</v>
@@ -1260,16 +1260,16 @@
         <v>0.009223753030530968</v>
       </c>
       <c r="J10">
-        <v>0.009617928537382501</v>
+        <v>0.0096179285373825</v>
       </c>
       <c r="K10">
         <v>0.010161569894650538</v>
       </c>
       <c r="L10">
-        <v>0.010523480313139513</v>
+        <v>0.01052348031313951</v>
       </c>
       <c r="M10">
-        <v>0.010670763898993851</v>
+        <v>0.01067076389899385</v>
       </c>
       <c r="N10">
         <v>0.010814573722841773</v>
@@ -1278,7 +1278,7 @@
         <v>0.010743672538856797</v>
       </c>
       <c r="P10">
-        <v>0.010978521623073681</v>
+        <v>0.010978521623073683</v>
       </c>
       <c r="Q10">
         <v>0.010472452962352136</v>
@@ -1287,7 +1287,7 @@
         <v>0.01096356239448917</v>
       </c>
       <c r="S10">
-        <v>0.011292244719964172</v>
+        <v>0.01129224471996417</v>
       </c>
       <c r="T10">
         <v>0.010121448489469284</v>
@@ -1302,7 +1302,7 @@
         <v>0.010367994305393282</v>
       </c>
       <c r="X10">
-        <v>0.013392605141400893</v>
+        <v>0.013392605141400891</v>
       </c>
       <c r="Y10">
         <v>0.013920971644932337</v>
@@ -1328,7 +1328,7 @@
         <v>0.016275924791880957</v>
       </c>
       <c r="G11">
-        <v>0.016595154974473503</v>
+        <v>0.0165951549744735</v>
       </c>
       <c r="H11">
         <v>0.01689698825103955</v>
@@ -1349,7 +1349,7 @@
         <v>0.01694506296072802</v>
       </c>
       <c r="N11">
-        <v>0.016753610656320042</v>
+        <v>0.01675361065632004</v>
       </c>
       <c r="O11">
         <v>0.016508908406540488</v>
@@ -1364,13 +1364,13 @@
         <v>0.018750025284345766</v>
       </c>
       <c r="S11">
-        <v>0.020918594523088863</v>
+        <v>0.020918594523088866</v>
       </c>
       <c r="T11">
         <v>0.023912421400947237</v>
       </c>
       <c r="U11">
-        <v>0.02441995337594056</v>
+        <v>0.024419953375940565</v>
       </c>
       <c r="V11">
         <v>0.023991942115673442</v>
@@ -1621,31 +1621,31 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.0112625853102247</v>
+        <v>0.011262585310224699</v>
       </c>
       <c r="C15">
         <v>0.009712995860138731</v>
       </c>
       <c r="D15">
-        <v>0.008588524844934255</v>
+        <v>0.008588524844934256</v>
       </c>
       <c r="E15">
         <v>0.007851234640988957</v>
       </c>
       <c r="F15">
-        <v>0.008020266865080804</v>
+        <v>0.008020266865080805</v>
       </c>
       <c r="G15">
-        <v>0.008445862443217898</v>
+        <v>0.0084458624432179</v>
       </c>
       <c r="H15">
-        <v>0.009354423186373499</v>
+        <v>0.009354423186373497</v>
       </c>
       <c r="I15">
         <v>0.010107414051398821</v>
       </c>
       <c r="J15">
-        <v>0.011287067379352375</v>
+        <v>0.011287067379352377</v>
       </c>
       <c r="K15">
         <v>0.012938446488027345</v>
@@ -1657,7 +1657,7 @@
         <v>0.015402562944672321</v>
       </c>
       <c r="N15">
-        <v>0.016272673931691625</v>
+        <v>0.01627267393169162</v>
       </c>
       <c r="O15">
         <v>0.01585539775176105</v>
@@ -1666,7 +1666,7 @@
         <v>0.015816977835937163</v>
       </c>
       <c r="Q15">
-        <v>0.015360503554972975</v>
+        <v>0.015360503554972973</v>
       </c>
       <c r="R15">
         <v>0.015628683535162013</v>
@@ -1775,43 +1775,43 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.0021325563019881956</v>
+        <v>0.002132556301988195</v>
       </c>
       <c r="C17">
-        <v>0.001818962594349584</v>
+        <v>0.0018189625943495831</v>
       </c>
       <c r="D17">
-        <v>0.0015970837212705754</v>
+        <v>0.0015970837212705752</v>
       </c>
       <c r="E17">
-        <v>0.0014544550401362096</v>
+        <v>0.0014544550401362098</v>
       </c>
       <c r="F17">
-        <v>0.0014869497807992395</v>
+        <v>0.0014869497807992401</v>
       </c>
       <c r="G17">
-        <v>0.0015693084306254066</v>
+        <v>0.0015693084308455176</v>
       </c>
       <c r="H17">
-        <v>0.0017523077469673253</v>
+        <v>0.0017523077469673257</v>
       </c>
       <c r="I17">
         <v>0.001917157629195325</v>
       </c>
       <c r="J17">
-        <v>0.002182399748626265</v>
+        <v>0.0021823997486262645</v>
       </c>
       <c r="K17">
-        <v>0.0026120929256859835</v>
+        <v>0.002612092925685983</v>
       </c>
       <c r="L17">
-        <v>0.003217419002824309</v>
+        <v>0.0032174190028243085</v>
       </c>
       <c r="M17">
         <v>0.00350773192993884</v>
       </c>
       <c r="N17">
-        <v>0.003860703372815604</v>
+        <v>0.0038607033728156035</v>
       </c>
       <c r="O17">
         <v>0.00376983195478759</v>
@@ -1820,22 +1820,22 @@
         <v>0.0037427474334845406</v>
       </c>
       <c r="Q17">
-        <v>0.0034270467453022353</v>
+        <v>0.003427046745302235</v>
       </c>
       <c r="R17">
-        <v>0.003252580624803554</v>
+        <v>0.0032525806248035537</v>
       </c>
       <c r="S17">
-        <v>0.0030815143150987245</v>
+        <v>0.003081514315098725</v>
       </c>
       <c r="T17">
-        <v>0.0035620690529525006</v>
+        <v>0.003562069052952501</v>
       </c>
       <c r="U17">
         <v>0.003884400416020618</v>
       </c>
       <c r="V17">
-        <v>0.003685178030657755</v>
+        <v>0.0036851780306577553</v>
       </c>
       <c r="W17">
         <v>0.0033600105233111766</v>
@@ -1929,31 +1929,31 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.0017166305519427242</v>
+        <v>0.0017166305519427246</v>
       </c>
       <c r="C19">
-        <v>0.0013771098371934598</v>
+        <v>0.0013771098371934596</v>
       </c>
       <c r="D19">
-        <v>0.001130998232636174</v>
+        <v>0.0011309982326361747</v>
       </c>
       <c r="E19">
-        <v>0.0009694363322106776</v>
+        <v>0.0009694363322106779</v>
       </c>
       <c r="F19">
-        <v>0.0010065130801263566</v>
+        <v>0.001006513080126357</v>
       </c>
       <c r="G19">
-        <v>0.0010997551416550083</v>
+        <v>0.0010997551416550085</v>
       </c>
       <c r="H19">
-        <v>0.0012944747262608595</v>
+        <v>0.0012944747262608604</v>
       </c>
       <c r="I19">
-        <v>0.0014465786316822187</v>
+        <v>0.0014465786316822185</v>
       </c>
       <c r="J19">
-        <v>0.001683344349820932</v>
+        <v>0.0016833443498209325</v>
       </c>
       <c r="K19">
         <v>0.0019730902318151147</v>
@@ -1962,10 +1962,10 @@
         <v>0.002145558576331036</v>
       </c>
       <c r="M19">
-        <v>0.0022094427359246886</v>
+        <v>0.002209442735924688</v>
       </c>
       <c r="N19">
-        <v>0.002266620566783339</v>
+        <v>0.002266620566783338</v>
       </c>
       <c r="O19">
         <v>0.0021747941516446147</v>
@@ -1974,7 +1974,7 @@
         <v>0.0021815864084847856</v>
       </c>
       <c r="Q19">
-        <v>0.0021752753938283627</v>
+        <v>0.002175275393828362</v>
       </c>
       <c r="R19">
         <v>0.0024217621360243936</v>
@@ -1983,7 +1983,7 @@
         <v>0.0026149914765346677</v>
       </c>
       <c r="T19">
-        <v>0.0032469530592507513</v>
+        <v>0.003246953059250751</v>
       </c>
       <c r="U19">
         <v>0.0035796694169578404</v>
@@ -1992,13 +1992,13 @@
         <v>0.0033800375175084907</v>
       </c>
       <c r="W19">
-        <v>0.003054022422388558</v>
+        <v>0.0030540224223885577</v>
       </c>
       <c r="X19">
-        <v>0.002628475975867827</v>
+        <v>0.0026284759758678274</v>
       </c>
       <c r="Y19">
-        <v>0.0017816727963679462</v>
+        <v>0.0017816727963679457</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2006,22 +2006,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.0024342683166585577</v>
+        <v>0.0024342683166585573</v>
       </c>
       <c r="C20">
-        <v>0.0017558840019390267</v>
+        <v>0.0017558840019390265</v>
       </c>
       <c r="D20">
-        <v>0.001268565930624305</v>
+        <v>0.0012685659306243052</v>
       </c>
       <c r="E20">
         <v>0.0009532120227600924</v>
       </c>
       <c r="F20">
-        <v>0.0010251024906983875</v>
+        <v>0.001025102490698388</v>
       </c>
       <c r="G20">
-        <v>0.0012072017063794814</v>
+        <v>0.0012072017063794816</v>
       </c>
       <c r="H20">
         <v>0.0016104558142704514</v>
@@ -2030,10 +2030,10 @@
         <v>0.0019708438094668246</v>
       </c>
       <c r="J20">
-        <v>0.0025427961870036664</v>
+        <v>0.002542796187003667</v>
       </c>
       <c r="K20">
-        <v>0.003453330536527349</v>
+        <v>0.0034533305365273487</v>
       </c>
       <c r="L20">
         <v>0.004713021144795998</v>
@@ -2072,7 +2072,7 @@
         <v>0.005149386183092093</v>
       </c>
       <c r="X20">
-        <v>0.0042643668574262805</v>
+        <v>0.00426436685742628</v>
       </c>
       <c r="Y20">
         <v>0.0025642776246216133</v>
@@ -2314,10 +2314,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.0018463421277981435</v>
+        <v>0.001846342127798143</v>
       </c>
       <c r="C24">
-        <v>0.0015802027502797023</v>
+        <v>0.0015802027502797025</v>
       </c>
       <c r="D24">
         <v>0.0014161337051687855</v>
@@ -2326,13 +2326,13 @@
         <v>0.0013584208848756822</v>
       </c>
       <c r="F24">
-        <v>0.0013682843438753206</v>
+        <v>0.001368284343875321</v>
       </c>
       <c r="G24">
         <v>0.0014077854839831775</v>
       </c>
       <c r="H24">
-        <v>0.0014992518773795822</v>
+        <v>0.0014992518773795825</v>
       </c>
       <c r="I24">
         <v>0.001577146996257638</v>
@@ -2341,16 +2341,16 @@
         <v>0.0017239210717937717</v>
       </c>
       <c r="K24">
-        <v>0.0018958336364028878</v>
+        <v>0.0018958336364028876</v>
       </c>
       <c r="L24">
-        <v>0.001960449341099897</v>
+        <v>0.0019604493410998974</v>
       </c>
       <c r="M24">
-        <v>0.001995735500086282</v>
+        <v>0.0019957355000862816</v>
       </c>
       <c r="N24">
-        <v>0.002032548076863715</v>
+        <v>0.0020325480768637154</v>
       </c>
       <c r="O24">
         <v>0.0019713887108367837</v>
@@ -2471,19 +2471,19 @@
         <v>8.870995275787644e-5</v>
       </c>
       <c r="C26">
-        <v>7.539686427426897e-5</v>
+        <v>7.539686427426895e-5</v>
       </c>
       <c r="D26">
         <v>6.634582195276093e-5</v>
       </c>
       <c r="E26">
-        <v>6.066079745336347e-5</v>
+        <v>6.066079745336348e-5</v>
       </c>
       <c r="F26">
         <v>6.194804278306645e-5</v>
       </c>
       <c r="G26">
-        <v>6.523094527570619e-5</v>
+        <v>6.523094527612083e-5</v>
       </c>
       <c r="H26">
         <v>6.861178983234295e-5</v>
@@ -2498,7 +2498,7 @@
         <v>7.993643642350706e-5</v>
       </c>
       <c r="L26">
-        <v>7.771472082418952e-5</v>
+        <v>7.771472082418953e-5</v>
       </c>
       <c r="M26">
         <v>7.796463914927448e-5</v>
@@ -2516,7 +2516,7 @@
         <v>7.786243809684615e-5</v>
       </c>
       <c r="R26">
-        <v>9.286752751972837e-5</v>
+        <v>9.286752751972836e-5</v>
       </c>
       <c r="S26">
         <v>0.00011217243570701032</v>
@@ -2631,7 +2631,7 @@
         <v>7.334033775303704e-5</v>
       </c>
       <c r="E28">
-        <v>7.943405901815051e-5</v>
+        <v>7.94340590181505e-5</v>
       </c>
       <c r="F28">
         <v>7.731455807598619e-5</v>
@@ -2643,55 +2643,55 @@
         <v>7.777782052175031e-5</v>
       </c>
       <c r="I28">
-        <v>8.218819185227767e-5</v>
+        <v>8.218819185227764e-5</v>
       </c>
       <c r="J28">
-        <v>8.98849089203474e-5</v>
+        <v>8.988490892034739e-5</v>
       </c>
       <c r="K28">
-        <v>0.0001010237182317479</v>
+        <v>0.00010102371823174788</v>
       </c>
       <c r="L28">
-        <v>0.00010875287311219125</v>
+        <v>0.00010875287311219122</v>
       </c>
       <c r="M28">
-        <v>0.00011195610912586112</v>
+        <v>0.0001119561091258611</v>
       </c>
       <c r="N28">
-        <v>0.00011510579649084598</v>
+        <v>0.00011510579649084596</v>
       </c>
       <c r="O28">
-        <v>0.0001132623587180167</v>
+        <v>0.00011326235871801669</v>
       </c>
       <c r="P28">
-        <v>0.00011803530064702113</v>
+        <v>0.00011803530064702116</v>
       </c>
       <c r="Q28">
-        <v>0.00010788233706276634</v>
+        <v>0.00010788233706276635</v>
       </c>
       <c r="R28">
-        <v>0.00011888007672745649</v>
+        <v>0.00011888007672745647</v>
       </c>
       <c r="S28">
         <v>0.00012669134184615963</v>
       </c>
       <c r="T28">
-        <v>0.00010655486296455765</v>
+        <v>0.00010655486296455767</v>
       </c>
       <c r="U28">
         <v>9.669793835323108e-5</v>
       </c>
       <c r="V28">
-        <v>0.0001034731400243381</v>
+        <v>0.00010347314002433814</v>
       </c>
       <c r="W28">
-        <v>0.00011016977985867443</v>
+        <v>0.00011016977985867442</v>
       </c>
       <c r="X28">
-        <v>0.0001756216638967524</v>
+        <v>0.00017562166389675237</v>
       </c>
       <c r="Y28">
-        <v>0.00018569598612568056</v>
+        <v>0.00018569598612568053</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -2717,7 +2717,7 @@
         <v>0.0002610264732759833</v>
       </c>
       <c r="H29">
-        <v>0.00027164339529887454</v>
+        <v>0.0002716433952988745</v>
       </c>
       <c r="I29">
         <v>0.0002777586530995801</v>
@@ -2750,7 +2750,7 @@
         <v>0.00035447439072222456</v>
       </c>
       <c r="S29">
-        <v>0.0004325220136146411</v>
+        <v>0.00043252201361464117</v>
       </c>
       <c r="T29">
         <v>0.0005683578539228638</v>
@@ -2762,7 +2762,7 @@
         <v>0.0005745977235727924</v>
       </c>
       <c r="W29">
-        <v>0.000565163560772316</v>
+        <v>0.0005651635607723161</v>
       </c>
       <c r="X29">
         <v>0.0005438449431188449</v>
@@ -3715,7 +3715,7 @@
         <v>1.0607550777207981</v>
       </c>
       <c r="G42">
-        <v>1.0607507442194994</v>
+        <v>1.060750744219496</v>
       </c>
       <c r="H42">
         <v>1.0607451578931633</v>
@@ -3863,13 +3863,13 @@
         <v>0.0025236363785130144</v>
       </c>
       <c r="E44">
-        <v>0.0024928790075913667</v>
+        <v>0.002492879007591367</v>
       </c>
       <c r="F44">
-        <v>0.0025003962415209484</v>
+        <v>0.002500396241520949</v>
       </c>
       <c r="G44">
-        <v>0.002518068030213912</v>
+        <v>0.0025180680299938044</v>
       </c>
       <c r="H44">
         <v>0.0025417719113235257</v>
@@ -3887,7 +3887,7 @@
         <v>0.0019634421921592114</v>
       </c>
       <c r="M44">
-        <v>0.0017398012016090782</v>
+        <v>0.0017398012016090784</v>
       </c>
       <c r="N44">
         <v>0.0014468379622950183</v>
@@ -3931,7 +3931,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.003017492207163704</v>
+        <v>0.0030174922071637034</v>
       </c>
       <c r="C45">
         <v>0.003003591107617607</v>
@@ -3943,7 +3943,7 @@
         <v>0.0029779178788118094</v>
       </c>
       <c r="F45">
-        <v>0.002980830050830264</v>
+        <v>0.0029808300508302643</v>
       </c>
       <c r="G45">
         <v>0.002987578957743676</v>
@@ -4020,7 +4020,7 @@
         <v>0.0014462434033654418</v>
       </c>
       <c r="F46">
-        <v>0.0014502839836385798</v>
+        <v>0.00145028398363858</v>
       </c>
       <c r="G46">
         <v>0.0014592345931364668</v>
@@ -4085,49 +4085,49 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.00012983018686528838</v>
+        <v>0.00012983018686528832</v>
       </c>
       <c r="C47">
-        <v>0.0002382837863700189</v>
+        <v>0.00023828378637001896</v>
       </c>
       <c r="D47">
-        <v>0.0005091624297957394</v>
+        <v>0.0005091624297957392</v>
       </c>
       <c r="E47">
-        <v>0.001264376848185382</v>
+        <v>0.001264376848185381</v>
       </c>
       <c r="F47">
-        <v>0.0010422683041951771</v>
+        <v>0.0010422683041951784</v>
       </c>
       <c r="G47">
-        <v>0.0006839690249447191</v>
+        <v>0.0006839690249447178</v>
       </c>
       <c r="H47">
-        <v>0.00040496582868916863</v>
+        <v>0.0004049658286891686</v>
       </c>
       <c r="I47">
         <v>0.0003191078044299154</v>
       </c>
       <c r="J47">
-        <v>0.00022005009966164892</v>
+        <v>0.000220050099661649</v>
       </c>
       <c r="K47">
-        <v>0.00016380786328421462</v>
+        <v>0.0001638078632842148</v>
       </c>
       <c r="L47">
-        <v>0.00016578496791926252</v>
+        <v>0.00016578496791926276</v>
       </c>
       <c r="M47">
-        <v>0.00017975889031541479</v>
+        <v>0.0001797588903154149</v>
       </c>
       <c r="N47">
-        <v>0.00020358921164747456</v>
+        <v>0.0002035892116474746</v>
       </c>
       <c r="O47">
         <v>0.0003193135825406185</v>
       </c>
       <c r="P47">
-        <v>0.0005408182660333845</v>
+        <v>0.0005408182660333854</v>
       </c>
       <c r="Q47">
         <v>-6.771580456699149e-10</v>
@@ -4151,7 +4151,7 @@
         <v>-6.79372990417206e-10</v>
       </c>
       <c r="X47">
-        <v>0.0020616180771178</v>
+        <v>0.002061618077117799</v>
       </c>
       <c r="Y47">
         <v>0.004322854184342137</v>
@@ -4165,46 +4165,46 @@
         <v>6.82276291930889e-5</v>
       </c>
       <c r="C48">
-        <v>0.00011516849788980247</v>
+        <v>0.00011516849788980243</v>
       </c>
       <c r="D48">
-        <v>0.00020659115333743468</v>
+        <v>0.00020659115333743474</v>
       </c>
       <c r="E48">
-        <v>0.00036658236623895735</v>
+        <v>0.0003665823662389573</v>
       </c>
       <c r="F48">
-        <v>0.0003282013978297207</v>
+        <v>0.0003282013978297205</v>
       </c>
       <c r="G48">
-        <v>0.0002473560148556594</v>
+        <v>0.00024735601485565957</v>
       </c>
       <c r="H48">
-        <v>0.00018900736617214067</v>
+        <v>0.0001890073661721407</v>
       </c>
       <c r="I48">
-        <v>0.000168321407912493</v>
+        <v>0.00016832140791249298</v>
       </c>
       <c r="J48">
         <v>0.00012670492654660582</v>
       </c>
       <c r="K48">
-        <v>0.00010681386802764569</v>
+        <v>0.0001068138680276457</v>
       </c>
       <c r="L48">
-        <v>0.00013525169731714844</v>
+        <v>0.00013525169731714846</v>
       </c>
       <c r="M48">
-        <v>0.0001560150883136163</v>
+        <v>0.00015601508831361636</v>
       </c>
       <c r="N48">
-        <v>0.00019110213895604766</v>
+        <v>0.0001911021389560476</v>
       </c>
       <c r="O48">
         <v>0.00031981229191020217</v>
       </c>
       <c r="P48">
-        <v>0.0004687048387982117</v>
+        <v>0.0004687048387982119</v>
       </c>
       <c r="Q48">
         <v>-6.75710559692321e-10</v>
@@ -4225,13 +4225,13 @@
         <v>-6.827246971608536e-10</v>
       </c>
       <c r="W48">
-        <v>-6.824323286948845e-10</v>
+        <v>-6.824323286948852e-10</v>
       </c>
       <c r="X48">
-        <v>0.000962661972813072</v>
+        <v>0.0009626619728130721</v>
       </c>
       <c r="Y48">
-        <v>0.0022305839176888754</v>
+        <v>0.002230583917688876</v>
       </c>
     </row>
     <row r="49" spans="1:25">
@@ -4284,22 +4284,22 @@
         <v>4.267368405147144e-8</v>
       </c>
       <c r="Q49">
-        <v>4.524176675725392e-5</v>
+        <v>4.524176675725376e-5</v>
       </c>
       <c r="R49">
-        <v>4.7375506925532515e-5</v>
+        <v>4.737550692553246e-5</v>
       </c>
       <c r="S49">
-        <v>0.0001052867416162281</v>
+        <v>0.00010528674161622804</v>
       </c>
       <c r="T49">
-        <v>0.0025423722333336816</v>
+        <v>0.0025423722333336803</v>
       </c>
       <c r="U49">
-        <v>0.0038581048331388533</v>
+        <v>0.003858104833138853</v>
       </c>
       <c r="V49">
-        <v>0.0030161491012373302</v>
+        <v>0.0030161491012373294</v>
       </c>
       <c r="W49">
         <v>0.0019092673211312835</v>
@@ -4352,7 +4352,7 @@
         <v>4.2676125406873336e-8</v>
       </c>
       <c r="N50">
-        <v>4.2672201983422955e-8</v>
+        <v>4.267220198342294e-8</v>
       </c>
       <c r="O50">
         <v>4.266501445491234e-8</v>
@@ -4361,13 +4361,13 @@
         <v>4.2661651109941746e-8</v>
       </c>
       <c r="Q50">
-        <v>1.4945349843162344e-5</v>
+        <v>1.4945349843162325e-5</v>
       </c>
       <c r="R50">
-        <v>1.2648009500593273e-5</v>
+        <v>1.2648009500593263e-5</v>
       </c>
       <c r="S50">
-        <v>1.7734611405127515e-5</v>
+        <v>1.7734611405127525e-5</v>
       </c>
       <c r="T50">
         <v>0.0009580659159978463</v>
@@ -4376,10 +4376,10 @@
         <v>0.0022506868890342017</v>
       </c>
       <c r="V50">
-        <v>0.0018784841898270219</v>
+        <v>0.0018784841898270214</v>
       </c>
       <c r="W50">
-        <v>0.0006310690309623469</v>
+        <v>0.0006310690309623471</v>
       </c>
       <c r="X50">
         <v>4.2648309656933967e-8</v>
@@ -4396,16 +4396,16 @@
         <v>0.011787043738294265</v>
       </c>
       <c r="C51">
-        <v>0.012013368406779173</v>
+        <v>0.012013368406779175</v>
       </c>
       <c r="D51">
-        <v>0.012497027793086703</v>
+        <v>0.012497027793086705</v>
       </c>
       <c r="E51">
         <v>0.013698140877597013</v>
       </c>
       <c r="F51">
-        <v>0.014688250845923416</v>
+        <v>0.014688250845923418</v>
       </c>
       <c r="G51">
         <v>0.01533797649890357</v>
@@ -4417,7 +4417,7 @@
         <v>0.0160257566022849</v>
       </c>
       <c r="J51">
-        <v>0.0162347592677267</v>
+        <v>0.016234759267726703</v>
       </c>
       <c r="K51">
         <v>0.01639033180395206</v>
@@ -4453,13 +4453,13 @@
         <v>0.010783241318792538</v>
       </c>
       <c r="V51">
-        <v>0.00760834688257375</v>
+        <v>0.007608346882573751</v>
       </c>
       <c r="W51">
         <v>0.005598591162294375</v>
       </c>
       <c r="X51">
-        <v>0.007557083425448955</v>
+        <v>0.007557083425448954</v>
       </c>
       <c r="Y51">
         <v>0.01166375</v>
@@ -4488,7 +4488,7 @@
         <v>0.007098876176845834</v>
       </c>
       <c r="H52">
-        <v>0.007278388256862231</v>
+        <v>0.007278388256862232</v>
       </c>
       <c r="I52">
         <v>0.007438248674106503</v>
@@ -4524,7 +4524,7 @@
         <v>0.00881940325757212</v>
       </c>
       <c r="T52">
-        <v>0.0078109121712947845</v>
+        <v>0.007810912171294785</v>
       </c>
       <c r="U52">
         <v>0.005441767428049126</v>
@@ -4536,7 +4536,7 @@
         <v>0.0028001311618979846</v>
       </c>
       <c r="X52">
-        <v>0.0037146151431128693</v>
+        <v>0.003714615143112869</v>
       </c>
       <c r="Y52">
         <v>0.005833624999999999</v>

</xml_diff>